<commit_message>
Added more game data and updated notebook
</commit_message>
<xml_diff>
--- a/data/nba_points_2024_2025.xlsx
+++ b/data/nba_points_2024_2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Documents/nba/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Documents/nba-points/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F45F96-481A-9745-9DC2-A8A9E1501457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C48B42F-372F-D441-856E-7CC777A0B3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22940" yWindow="500" windowWidth="45860" windowHeight="28300" xr2:uid="{4B944735-6DC1-314A-AF10-68EBB82A81F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2905" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3025" uniqueCount="147">
   <si>
     <t>Date</t>
   </si>
@@ -1001,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78582E2E-5746-944D-860C-ACA920BD70CB}">
-  <dimension ref="A1:Y480"/>
+  <dimension ref="A1:Y500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G482" sqref="G482"/>
+    <sheetView tabSelected="1" topLeftCell="A459" workbookViewId="0">
+      <selection activeCell="M501" sqref="M501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1179,15 +1179,15 @@
       </c>
       <c r="V2" s="7">
         <f>SUM(O:O)</f>
-        <v>477</v>
+        <v>497</v>
       </c>
       <c r="W2" s="12">
         <f>SUM(P:P)</f>
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="X2" s="15">
         <f>SUM(R:R)</f>
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="Y2" s="20">
         <f>SUM(T:T)</f>
@@ -1342,15 +1342,15 @@
       </c>
       <c r="W4" s="14">
         <f>W2/V2</f>
-        <v>0.51153039832285119</v>
+        <v>0.51106639839034207</v>
       </c>
       <c r="X4" s="16">
         <f>X2/V2</f>
-        <v>0.48637316561844862</v>
+        <v>0.48692152917505033</v>
       </c>
       <c r="Y4" s="21">
         <f>Y2/V2</f>
-        <v>2.0964360587002098E-3</v>
+        <v>2.012072434607646E-3</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1498,11 +1498,11 @@
       </c>
       <c r="W6" s="22">
         <f>AVERAGE(Q:Q)</f>
-        <v>15.372950819672131</v>
+        <v>15.187007874015748</v>
       </c>
       <c r="X6" s="23">
         <f>AVERAGE(S:S)</f>
-        <v>15.661637931034482</v>
+        <v>15.440082644628099</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1650,11 +1650,11 @@
       </c>
       <c r="W8" s="22">
         <f>MEDIAN(Q:Q)</f>
-        <v>12.25</v>
+        <v>12</v>
       </c>
       <c r="X8" s="23">
         <f>MEDIAN(S:S)</f>
-        <v>13.75</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -33813,34 +33813,34 @@
         <v>108</v>
       </c>
       <c r="M475" s="10">
-        <f t="shared" ref="M475:M480" si="21">K475+L475</f>
+        <f t="shared" ref="M475:M500" si="21">K475+L475</f>
         <v>223</v>
       </c>
       <c r="N475" s="10">
-        <f t="shared" ref="N475:N480" si="22">(L475-K475)*-1</f>
+        <f t="shared" ref="N475:N500" si="22">(L475-K475)*-1</f>
         <v>7</v>
       </c>
       <c r="O475" s="10">
         <v>1</v>
       </c>
       <c r="P475" s="10">
-        <f t="shared" ref="P475:P480" si="23">IF(M475&gt;I475,1,0)</f>
+        <f t="shared" ref="P475:P500" si="23">IF(M475&gt;I475,1,0)</f>
         <v>0</v>
       </c>
       <c r="Q475" s="10" t="str">
-        <f t="shared" ref="Q475:Q480" si="24">IF(P475=1,(M475-I475), "")</f>
+        <f t="shared" ref="Q475:Q500" si="24">IF(P475=1,(M475-I475), "")</f>
         <v/>
       </c>
       <c r="R475" s="10">
-        <f t="shared" ref="R475:R480" si="25">IF(M475&lt;I475, 1, 0)</f>
+        <f t="shared" ref="R475:R500" si="25">IF(M475&lt;I475, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="S475" s="10">
-        <f t="shared" ref="S475:S480" si="26">IF(R475=1,(I475-M475),"")</f>
+        <f t="shared" ref="S475:S500" si="26">IF(R475=1,(I475-M475),"")</f>
         <v>3.5</v>
       </c>
       <c r="T475" s="10">
-        <f t="shared" ref="T475:T480" si="27">IF(M475=I475,1,0)</f>
+        <f t="shared" ref="T475:T500" si="27">IF(M475=I475,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -34185,6 +34185,1386 @@
         <v>23.5</v>
       </c>
       <c r="T480" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="481" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A481" s="6">
+        <v>45657</v>
+      </c>
+      <c r="B481" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C481" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D481" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E481" s="7">
+        <v>0</v>
+      </c>
+      <c r="F481" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G481" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H481" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I481" s="7">
+        <v>230.5</v>
+      </c>
+      <c r="J481" s="8">
+        <v>-17.5</v>
+      </c>
+      <c r="K481" s="7">
+        <v>71</v>
+      </c>
+      <c r="L481" s="7">
+        <v>125</v>
+      </c>
+      <c r="M481" s="7">
+        <f t="shared" si="21"/>
+        <v>196</v>
+      </c>
+      <c r="N481" s="7">
+        <f t="shared" si="22"/>
+        <v>-54</v>
+      </c>
+      <c r="O481" s="7">
+        <v>1</v>
+      </c>
+      <c r="P481" s="7">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q481" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R481" s="7">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S481" s="7">
+        <f t="shared" si="26"/>
+        <v>34.5</v>
+      </c>
+      <c r="T481" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="482" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A482" s="6">
+        <v>45657</v>
+      </c>
+      <c r="B482" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C482" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D482" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E482" s="7">
+        <v>0</v>
+      </c>
+      <c r="F482" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G482" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H482" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I482" s="7">
+        <v>229</v>
+      </c>
+      <c r="J482" s="8">
+        <v>-1.5</v>
+      </c>
+      <c r="K482" s="7">
+        <v>120</v>
+      </c>
+      <c r="L482" s="7">
+        <v>112</v>
+      </c>
+      <c r="M482" s="7">
+        <f t="shared" si="21"/>
+        <v>232</v>
+      </c>
+      <c r="N482" s="7">
+        <f t="shared" si="22"/>
+        <v>8</v>
+      </c>
+      <c r="O482" s="7">
+        <v>1</v>
+      </c>
+      <c r="P482" s="7">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q482" s="7">
+        <f t="shared" si="24"/>
+        <v>3</v>
+      </c>
+      <c r="R482" s="7">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S482" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T482" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="483" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A483" s="6">
+        <v>45657</v>
+      </c>
+      <c r="B483" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C483" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D483" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E483" s="7">
+        <v>0</v>
+      </c>
+      <c r="F483" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G483" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H483" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="I483" s="7">
+        <v>217.5</v>
+      </c>
+      <c r="J483" s="8">
+        <v>-2.5</v>
+      </c>
+      <c r="K483" s="7">
+        <v>86</v>
+      </c>
+      <c r="L483" s="7">
+        <v>122</v>
+      </c>
+      <c r="M483" s="7">
+        <f t="shared" si="21"/>
+        <v>208</v>
+      </c>
+      <c r="N483" s="7">
+        <f t="shared" si="22"/>
+        <v>-36</v>
+      </c>
+      <c r="O483" s="7">
+        <v>1</v>
+      </c>
+      <c r="P483" s="7">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q483" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R483" s="7">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S483" s="7">
+        <f t="shared" si="26"/>
+        <v>9.5</v>
+      </c>
+      <c r="T483" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="484" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A484" s="6">
+        <v>45657</v>
+      </c>
+      <c r="B484" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C484" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D484" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E484" s="7">
+        <v>0</v>
+      </c>
+      <c r="F484" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G484" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H484" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I484" s="7">
+        <v>215.5</v>
+      </c>
+      <c r="J484" s="8">
+        <v>-7.5</v>
+      </c>
+      <c r="K484" s="7">
+        <v>105</v>
+      </c>
+      <c r="L484" s="7">
+        <v>113</v>
+      </c>
+      <c r="M484" s="7">
+        <f t="shared" si="21"/>
+        <v>218</v>
+      </c>
+      <c r="N484" s="7">
+        <f t="shared" si="22"/>
+        <v>-8</v>
+      </c>
+      <c r="O484" s="7">
+        <v>1</v>
+      </c>
+      <c r="P484" s="7">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q484" s="7">
+        <f t="shared" si="24"/>
+        <v>2.5</v>
+      </c>
+      <c r="R484" s="7">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S484" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T484" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="485" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A485" s="6">
+        <v>45657</v>
+      </c>
+      <c r="B485" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C485" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D485" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E485" s="7">
+        <v>0</v>
+      </c>
+      <c r="F485" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G485" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="H485" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I485" s="7">
+        <v>237.5</v>
+      </c>
+      <c r="J485" s="8">
+        <v>-7.5</v>
+      </c>
+      <c r="K485" s="7">
+        <v>117</v>
+      </c>
+      <c r="L485" s="7">
+        <v>112</v>
+      </c>
+      <c r="M485" s="7">
+        <f t="shared" si="21"/>
+        <v>229</v>
+      </c>
+      <c r="N485" s="7">
+        <f t="shared" si="22"/>
+        <v>5</v>
+      </c>
+      <c r="O485" s="7">
+        <v>1</v>
+      </c>
+      <c r="P485" s="7">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q485" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R485" s="7">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S485" s="7">
+        <f t="shared" si="26"/>
+        <v>8.5</v>
+      </c>
+      <c r="T485" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="486" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A486" s="6">
+        <v>45657</v>
+      </c>
+      <c r="B486" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C486" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D486" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E486" s="7">
+        <v>0</v>
+      </c>
+      <c r="F486" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G486" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H486" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I486" s="7">
+        <v>227.5</v>
+      </c>
+      <c r="J486" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="K486" s="7">
+        <v>122</v>
+      </c>
+      <c r="L486" s="7">
+        <v>110</v>
+      </c>
+      <c r="M486" s="7">
+        <f t="shared" si="21"/>
+        <v>232</v>
+      </c>
+      <c r="N486" s="7">
+        <f t="shared" si="22"/>
+        <v>12</v>
+      </c>
+      <c r="O486" s="7">
+        <v>1</v>
+      </c>
+      <c r="P486" s="7">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q486" s="7">
+        <f t="shared" si="24"/>
+        <v>4.5</v>
+      </c>
+      <c r="R486" s="7">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S486" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T486" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="487" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A487" s="9">
+        <v>45658</v>
+      </c>
+      <c r="B487" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C487" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D487" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E487" s="10">
+        <v>0</v>
+      </c>
+      <c r="F487" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G487" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H487" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I487" s="10">
+        <v>212.5</v>
+      </c>
+      <c r="J487" s="11">
+        <v>-2.5</v>
+      </c>
+      <c r="K487" s="10">
+        <v>96</v>
+      </c>
+      <c r="L487" s="10">
+        <v>105</v>
+      </c>
+      <c r="M487" s="10">
+        <f t="shared" si="21"/>
+        <v>201</v>
+      </c>
+      <c r="N487" s="10">
+        <f t="shared" si="22"/>
+        <v>-9</v>
+      </c>
+      <c r="O487" s="10">
+        <v>1</v>
+      </c>
+      <c r="P487" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q487" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R487" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S487" s="10">
+        <f t="shared" si="26"/>
+        <v>11.5</v>
+      </c>
+      <c r="T487" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="488" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A488" s="9">
+        <v>45658</v>
+      </c>
+      <c r="B488" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C488" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D488" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E488" s="10">
+        <v>0</v>
+      </c>
+      <c r="F488" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G488" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H488" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I488" s="10">
+        <v>236.5</v>
+      </c>
+      <c r="J488" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="K488" s="10">
+        <v>107</v>
+      </c>
+      <c r="L488" s="10">
+        <v>125</v>
+      </c>
+      <c r="M488" s="10">
+        <f t="shared" si="21"/>
+        <v>232</v>
+      </c>
+      <c r="N488" s="10">
+        <f t="shared" si="22"/>
+        <v>-18</v>
+      </c>
+      <c r="O488" s="10">
+        <v>1</v>
+      </c>
+      <c r="P488" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q488" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R488" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S488" s="10">
+        <f t="shared" si="26"/>
+        <v>4.5</v>
+      </c>
+      <c r="T488" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="489" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A489" s="9">
+        <v>45658</v>
+      </c>
+      <c r="B489" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C489" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D489" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E489" s="10">
+        <v>0</v>
+      </c>
+      <c r="F489" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G489" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H489" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="I489" s="10">
+        <v>231</v>
+      </c>
+      <c r="J489" s="11">
+        <v>-14.5</v>
+      </c>
+      <c r="K489" s="10">
+        <v>103</v>
+      </c>
+      <c r="L489" s="10">
+        <v>119</v>
+      </c>
+      <c r="M489" s="10">
+        <f t="shared" si="21"/>
+        <v>222</v>
+      </c>
+      <c r="N489" s="10">
+        <f t="shared" si="22"/>
+        <v>-16</v>
+      </c>
+      <c r="O489" s="10">
+        <v>1</v>
+      </c>
+      <c r="P489" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q489" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R489" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S489" s="10">
+        <f t="shared" si="26"/>
+        <v>9</v>
+      </c>
+      <c r="T489" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="490" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A490" s="9">
+        <v>45658</v>
+      </c>
+      <c r="B490" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C490" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D490" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E490" s="10">
+        <v>0</v>
+      </c>
+      <c r="F490" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G490" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H490" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I490" s="10">
+        <v>223.5</v>
+      </c>
+      <c r="J490" s="11">
+        <v>-1</v>
+      </c>
+      <c r="K490" s="10">
+        <v>113</v>
+      </c>
+      <c r="L490" s="10">
+        <v>130</v>
+      </c>
+      <c r="M490" s="10">
+        <f t="shared" si="21"/>
+        <v>243</v>
+      </c>
+      <c r="N490" s="10">
+        <f t="shared" si="22"/>
+        <v>-17</v>
+      </c>
+      <c r="O490" s="10">
+        <v>1</v>
+      </c>
+      <c r="P490" s="10">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q490" s="10">
+        <f t="shared" si="24"/>
+        <v>19.5</v>
+      </c>
+      <c r="R490" s="10">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S490" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T490" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="491" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A491" s="9">
+        <v>45658</v>
+      </c>
+      <c r="B491" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C491" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D491" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E491" s="10">
+        <v>0</v>
+      </c>
+      <c r="F491" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G491" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H491" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="I491" s="10">
+        <v>221.5</v>
+      </c>
+      <c r="J491" s="11">
+        <v>-9</v>
+      </c>
+      <c r="K491" s="10">
+        <v>108</v>
+      </c>
+      <c r="L491" s="10">
+        <v>119</v>
+      </c>
+      <c r="M491" s="10">
+        <f t="shared" si="21"/>
+        <v>227</v>
+      </c>
+      <c r="N491" s="10">
+        <f t="shared" si="22"/>
+        <v>-11</v>
+      </c>
+      <c r="O491" s="10">
+        <v>1</v>
+      </c>
+      <c r="P491" s="10">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q491" s="10">
+        <f t="shared" si="24"/>
+        <v>5.5</v>
+      </c>
+      <c r="R491" s="10">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S491" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T491" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="492" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A492" s="9">
+        <v>45658</v>
+      </c>
+      <c r="B492" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C492" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D492" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E492" s="10">
+        <v>0</v>
+      </c>
+      <c r="F492" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G492" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H492" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I492" s="10">
+        <v>222.5</v>
+      </c>
+      <c r="J492" s="11">
+        <v>-5.5</v>
+      </c>
+      <c r="K492" s="10">
+        <v>99</v>
+      </c>
+      <c r="L492" s="10">
+        <v>110</v>
+      </c>
+      <c r="M492" s="10">
+        <f t="shared" si="21"/>
+        <v>209</v>
+      </c>
+      <c r="N492" s="10">
+        <f t="shared" si="22"/>
+        <v>-11</v>
+      </c>
+      <c r="O492" s="10">
+        <v>1</v>
+      </c>
+      <c r="P492" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q492" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R492" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S492" s="10">
+        <f t="shared" si="26"/>
+        <v>13.5</v>
+      </c>
+      <c r="T492" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="493" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A493" s="9">
+        <v>45658</v>
+      </c>
+      <c r="B493" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C493" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D493" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E493" s="10">
+        <v>0</v>
+      </c>
+      <c r="F493" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G493" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="H493" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="I493" s="10">
+        <v>245.5</v>
+      </c>
+      <c r="J493" s="11">
+        <v>-5</v>
+      </c>
+      <c r="K493" s="10">
+        <v>120</v>
+      </c>
+      <c r="L493" s="10">
+        <v>139</v>
+      </c>
+      <c r="M493" s="10">
+        <f t="shared" si="21"/>
+        <v>259</v>
+      </c>
+      <c r="N493" s="10">
+        <f t="shared" si="22"/>
+        <v>-19</v>
+      </c>
+      <c r="O493" s="10">
+        <v>1</v>
+      </c>
+      <c r="P493" s="10">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q493" s="10">
+        <f t="shared" si="24"/>
+        <v>13.5</v>
+      </c>
+      <c r="R493" s="10">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S493" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T493" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="494" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A494" s="9">
+        <v>45658</v>
+      </c>
+      <c r="B494" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C494" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D494" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E494" s="10">
+        <v>0</v>
+      </c>
+      <c r="F494" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G494" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H494" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I494" s="10">
+        <v>224.5</v>
+      </c>
+      <c r="J494" s="11">
+        <v>-7</v>
+      </c>
+      <c r="K494" s="10">
+        <v>107</v>
+      </c>
+      <c r="L494" s="10">
+        <v>113</v>
+      </c>
+      <c r="M494" s="10">
+        <f t="shared" si="21"/>
+        <v>220</v>
+      </c>
+      <c r="N494" s="10">
+        <f t="shared" si="22"/>
+        <v>-6</v>
+      </c>
+      <c r="O494" s="10">
+        <v>1</v>
+      </c>
+      <c r="P494" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q494" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R494" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S494" s="10">
+        <f t="shared" si="26"/>
+        <v>4.5</v>
+      </c>
+      <c r="T494" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="495" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A495" s="6">
+        <v>45659</v>
+      </c>
+      <c r="B495" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C495" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D495" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E495" s="7">
+        <v>0</v>
+      </c>
+      <c r="F495" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G495" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H495" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="I495" s="7">
+        <v>226.5</v>
+      </c>
+      <c r="J495" s="8">
+        <v>-2.5</v>
+      </c>
+      <c r="K495" s="7">
+        <v>128</v>
+      </c>
+      <c r="L495" s="7">
+        <v>115</v>
+      </c>
+      <c r="M495" s="7">
+        <f t="shared" si="21"/>
+        <v>243</v>
+      </c>
+      <c r="N495" s="7">
+        <f t="shared" si="22"/>
+        <v>13</v>
+      </c>
+      <c r="O495" s="7">
+        <v>1</v>
+      </c>
+      <c r="P495" s="7">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q495" s="7">
+        <f t="shared" si="24"/>
+        <v>16.5</v>
+      </c>
+      <c r="R495" s="7">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S495" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T495" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="496" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A496" s="6">
+        <v>45659</v>
+      </c>
+      <c r="B496" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C496" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D496" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E496" s="7">
+        <v>0</v>
+      </c>
+      <c r="F496" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G496" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H496" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="I496" s="7">
+        <v>221</v>
+      </c>
+      <c r="J496" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="K496" s="7">
+        <v>118</v>
+      </c>
+      <c r="L496" s="7">
+        <v>115</v>
+      </c>
+      <c r="M496" s="7">
+        <f t="shared" si="21"/>
+        <v>233</v>
+      </c>
+      <c r="N496" s="7">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="O496" s="7">
+        <v>1</v>
+      </c>
+      <c r="P496" s="7">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q496" s="7">
+        <f t="shared" si="24"/>
+        <v>12</v>
+      </c>
+      <c r="R496" s="7">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S496" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T496" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="497" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A497" s="6">
+        <v>45659</v>
+      </c>
+      <c r="B497" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C497" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D497" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E497" s="7">
+        <v>0</v>
+      </c>
+      <c r="F497" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G497" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H497" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I497" s="7">
+        <v>217</v>
+      </c>
+      <c r="J497" s="8">
+        <v>-9.5</v>
+      </c>
+      <c r="K497" s="7">
+        <v>98</v>
+      </c>
+      <c r="L497" s="7">
+        <v>116</v>
+      </c>
+      <c r="M497" s="7">
+        <f t="shared" si="21"/>
+        <v>214</v>
+      </c>
+      <c r="N497" s="7">
+        <f t="shared" si="22"/>
+        <v>-18</v>
+      </c>
+      <c r="O497" s="7">
+        <v>1</v>
+      </c>
+      <c r="P497" s="7">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q497" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R497" s="7">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S497" s="7">
+        <f t="shared" si="26"/>
+        <v>3</v>
+      </c>
+      <c r="T497" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="498" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A498" s="6">
+        <v>45659</v>
+      </c>
+      <c r="B498" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C498" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D498" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E498" s="7">
+        <v>0</v>
+      </c>
+      <c r="F498" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G498" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="H498" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="I498" s="7">
+        <v>218.5</v>
+      </c>
+      <c r="J498" s="8">
+        <v>-13.5</v>
+      </c>
+      <c r="K498" s="7">
+        <v>113</v>
+      </c>
+      <c r="L498" s="7">
+        <v>110</v>
+      </c>
+      <c r="M498" s="7">
+        <f t="shared" si="21"/>
+        <v>223</v>
+      </c>
+      <c r="N498" s="7">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="O498" s="7">
+        <v>1</v>
+      </c>
+      <c r="P498" s="7">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q498" s="7">
+        <f t="shared" si="24"/>
+        <v>4.5</v>
+      </c>
+      <c r="R498" s="7">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S498" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T498" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="499" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A499" s="6">
+        <v>45659</v>
+      </c>
+      <c r="B499" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C499" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D499" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E499" s="7">
+        <v>0</v>
+      </c>
+      <c r="F499" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G499" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H499" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I499" s="7">
+        <v>219</v>
+      </c>
+      <c r="J499" s="8">
+        <v>-2.5</v>
+      </c>
+      <c r="K499" s="7">
+        <v>105</v>
+      </c>
+      <c r="L499" s="7">
+        <v>139</v>
+      </c>
+      <c r="M499" s="7">
+        <f t="shared" si="21"/>
+        <v>244</v>
+      </c>
+      <c r="N499" s="7">
+        <f t="shared" si="22"/>
+        <v>-34</v>
+      </c>
+      <c r="O499" s="7">
+        <v>1</v>
+      </c>
+      <c r="P499" s="7">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q499" s="7">
+        <f t="shared" si="24"/>
+        <v>25</v>
+      </c>
+      <c r="R499" s="7">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S499" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T499" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="500" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A500" s="6">
+        <v>45659</v>
+      </c>
+      <c r="B500" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C500" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D500" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E500" s="7">
+        <v>0</v>
+      </c>
+      <c r="F500" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G500" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H500" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I500" s="7">
+        <v>224.5</v>
+      </c>
+      <c r="J500" s="8">
+        <v>-8</v>
+      </c>
+      <c r="K500" s="7">
+        <v>106</v>
+      </c>
+      <c r="L500" s="7">
+        <v>114</v>
+      </c>
+      <c r="M500" s="7">
+        <f t="shared" si="21"/>
+        <v>220</v>
+      </c>
+      <c r="N500" s="7">
+        <f t="shared" si="22"/>
+        <v>-8</v>
+      </c>
+      <c r="O500" s="7">
+        <v>1</v>
+      </c>
+      <c r="P500" s="7">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q500" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R500" s="7">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S500" s="7">
+        <f t="shared" si="26"/>
+        <v>4.5</v>
+      </c>
+      <c r="T500" s="7">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added 2 days of game data. Updated EDA notebook
</commit_message>
<xml_diff>
--- a/data/nba_points_2024_2025.xlsx
+++ b/data/nba_points_2024_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Documents/nba-points/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C48B42F-372F-D441-856E-7CC777A0B3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE039625-2A52-9446-B17E-4753E1F41A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22940" yWindow="500" windowWidth="45860" windowHeight="28300" xr2:uid="{4B944735-6DC1-314A-AF10-68EBB82A81F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3025" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3133" uniqueCount="147">
   <si>
     <t>Date</t>
   </si>
@@ -1001,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78582E2E-5746-944D-860C-ACA920BD70CB}">
-  <dimension ref="A1:Y500"/>
+  <dimension ref="A1:Y518"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A459" workbookViewId="0">
-      <selection activeCell="M501" sqref="M501"/>
+    <sheetView tabSelected="1" topLeftCell="A473" workbookViewId="0">
+      <selection activeCell="Q502" sqref="Q502"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1179,15 +1179,15 @@
       </c>
       <c r="V2" s="7">
         <f>SUM(O:O)</f>
-        <v>497</v>
+        <v>515</v>
       </c>
       <c r="W2" s="12">
         <f>SUM(P:P)</f>
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="X2" s="15">
         <f>SUM(R:R)</f>
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="Y2" s="20">
         <f>SUM(T:T)</f>
@@ -1342,15 +1342,15 @@
       </c>
       <c r="W4" s="14">
         <f>W2/V2</f>
-        <v>0.51106639839034207</v>
+        <v>0.51067961165048548</v>
       </c>
       <c r="X4" s="16">
         <f>X2/V2</f>
-        <v>0.48692152917505033</v>
+        <v>0.48737864077669901</v>
       </c>
       <c r="Y4" s="21">
         <f>Y2/V2</f>
-        <v>2.012072434607646E-3</v>
+        <v>1.9417475728155339E-3</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1498,11 +1498,11 @@
       </c>
       <c r="W6" s="22">
         <f>AVERAGE(Q:Q)</f>
-        <v>15.187007874015748</v>
+        <v>15.20722433460076</v>
       </c>
       <c r="X6" s="23">
         <f>AVERAGE(S:S)</f>
-        <v>15.440082644628099</v>
+        <v>15.350597609561753</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -33813,34 +33813,34 @@
         <v>108</v>
       </c>
       <c r="M475" s="10">
-        <f t="shared" ref="M475:M500" si="21">K475+L475</f>
+        <f t="shared" ref="M475:M518" si="21">K475+L475</f>
         <v>223</v>
       </c>
       <c r="N475" s="10">
-        <f t="shared" ref="N475:N500" si="22">(L475-K475)*-1</f>
+        <f t="shared" ref="N475:N518" si="22">(L475-K475)*-1</f>
         <v>7</v>
       </c>
       <c r="O475" s="10">
         <v>1</v>
       </c>
       <c r="P475" s="10">
-        <f t="shared" ref="P475:P500" si="23">IF(M475&gt;I475,1,0)</f>
+        <f t="shared" ref="P475:P518" si="23">IF(M475&gt;I475,1,0)</f>
         <v>0</v>
       </c>
       <c r="Q475" s="10" t="str">
-        <f t="shared" ref="Q475:Q500" si="24">IF(P475=1,(M475-I475), "")</f>
+        <f t="shared" ref="Q475:Q518" si="24">IF(P475=1,(M475-I475), "")</f>
         <v/>
       </c>
       <c r="R475" s="10">
-        <f t="shared" ref="R475:R500" si="25">IF(M475&lt;I475, 1, 0)</f>
+        <f t="shared" ref="R475:R518" si="25">IF(M475&lt;I475, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="S475" s="10">
-        <f t="shared" ref="S475:S500" si="26">IF(R475=1,(I475-M475),"")</f>
+        <f t="shared" ref="S475:S518" si="26">IF(R475=1,(I475-M475),"")</f>
         <v>3.5</v>
       </c>
       <c r="T475" s="10">
-        <f t="shared" ref="T475:T500" si="27">IF(M475=I475,1,0)</f>
+        <f t="shared" ref="T475:T518" si="27">IF(M475=I475,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -35565,6 +35565,1248 @@
         <v>4.5</v>
       </c>
       <c r="T500" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="501" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A501" s="9">
+        <v>45660</v>
+      </c>
+      <c r="B501" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C501" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D501" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E501" s="10">
+        <v>0</v>
+      </c>
+      <c r="F501" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G501" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H501" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="I501" s="10">
+        <v>215.5</v>
+      </c>
+      <c r="J501" s="11">
+        <v>-5</v>
+      </c>
+      <c r="K501" s="10">
+        <v>94</v>
+      </c>
+      <c r="L501" s="10">
+        <v>98</v>
+      </c>
+      <c r="M501" s="10">
+        <f t="shared" si="21"/>
+        <v>192</v>
+      </c>
+      <c r="N501" s="10">
+        <f t="shared" si="22"/>
+        <v>-4</v>
+      </c>
+      <c r="O501" s="10">
+        <v>1</v>
+      </c>
+      <c r="P501" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q501" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R501" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S501" s="10">
+        <f t="shared" si="26"/>
+        <v>23.5</v>
+      </c>
+      <c r="T501" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="502" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A502" s="9">
+        <v>45660</v>
+      </c>
+      <c r="B502" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C502" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D502" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E502" s="10">
+        <v>0</v>
+      </c>
+      <c r="F502" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G502" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H502" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I502" s="10">
+        <v>214.5</v>
+      </c>
+      <c r="J502" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="K502" s="10">
+        <v>106</v>
+      </c>
+      <c r="L502" s="10">
+        <v>97</v>
+      </c>
+      <c r="M502" s="10">
+        <f t="shared" si="21"/>
+        <v>203</v>
+      </c>
+      <c r="N502" s="10">
+        <f t="shared" si="22"/>
+        <v>9</v>
+      </c>
+      <c r="O502" s="10">
+        <v>1</v>
+      </c>
+      <c r="P502" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q502" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R502" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S502" s="10">
+        <f t="shared" si="26"/>
+        <v>11.5</v>
+      </c>
+      <c r="T502" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="503" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A503" s="9">
+        <v>45660</v>
+      </c>
+      <c r="B503" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C503" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D503" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E503" s="10">
+        <v>0</v>
+      </c>
+      <c r="F503" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G503" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H503" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="I503" s="10">
+        <v>220.5</v>
+      </c>
+      <c r="J503" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="K503" s="10">
+        <v>109</v>
+      </c>
+      <c r="L503" s="10">
+        <v>86</v>
+      </c>
+      <c r="M503" s="10">
+        <f t="shared" si="21"/>
+        <v>195</v>
+      </c>
+      <c r="N503" s="10">
+        <f t="shared" si="22"/>
+        <v>23</v>
+      </c>
+      <c r="O503" s="10">
+        <v>1</v>
+      </c>
+      <c r="P503" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q503" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R503" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S503" s="10">
+        <f t="shared" si="26"/>
+        <v>25.5</v>
+      </c>
+      <c r="T503" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="504" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A504" s="9">
+        <v>45660</v>
+      </c>
+      <c r="B504" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C504" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D504" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E504" s="10">
+        <v>0</v>
+      </c>
+      <c r="F504" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G504" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H504" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I504" s="10">
+        <v>231</v>
+      </c>
+      <c r="J504" s="11">
+        <v>-4.5</v>
+      </c>
+      <c r="K504" s="10">
+        <v>120</v>
+      </c>
+      <c r="L504" s="10">
+        <v>132</v>
+      </c>
+      <c r="M504" s="10">
+        <f t="shared" si="21"/>
+        <v>252</v>
+      </c>
+      <c r="N504" s="10">
+        <f t="shared" si="22"/>
+        <v>-12</v>
+      </c>
+      <c r="O504" s="10">
+        <v>1</v>
+      </c>
+      <c r="P504" s="10">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q504" s="10">
+        <f t="shared" si="24"/>
+        <v>21</v>
+      </c>
+      <c r="R504" s="10">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S504" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T504" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="505" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A505" s="9">
+        <v>45660</v>
+      </c>
+      <c r="B505" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C505" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D505" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E505" s="10">
+        <v>0</v>
+      </c>
+      <c r="F505" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G505" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="H505" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I505" s="10">
+        <v>220.5</v>
+      </c>
+      <c r="J505" s="11">
+        <v>-5.5</v>
+      </c>
+      <c r="K505" s="10">
+        <v>107</v>
+      </c>
+      <c r="L505" s="10">
+        <v>117</v>
+      </c>
+      <c r="M505" s="10">
+        <f t="shared" si="21"/>
+        <v>224</v>
+      </c>
+      <c r="N505" s="10">
+        <f t="shared" si="22"/>
+        <v>-10</v>
+      </c>
+      <c r="O505" s="10">
+        <v>1</v>
+      </c>
+      <c r="P505" s="10">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q505" s="10">
+        <f t="shared" si="24"/>
+        <v>3.5</v>
+      </c>
+      <c r="R505" s="10">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S505" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T505" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="506" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A506" s="9">
+        <v>45660</v>
+      </c>
+      <c r="B506" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C506" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D506" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E506" s="10">
+        <v>0</v>
+      </c>
+      <c r="F506" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G506" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H506" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="I506" s="10">
+        <v>229</v>
+      </c>
+      <c r="J506" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="K506" s="10">
+        <v>134</v>
+      </c>
+      <c r="L506" s="10">
+        <v>122</v>
+      </c>
+      <c r="M506" s="10">
+        <f t="shared" si="21"/>
+        <v>256</v>
+      </c>
+      <c r="N506" s="10">
+        <f t="shared" si="22"/>
+        <v>12</v>
+      </c>
+      <c r="O506" s="10">
+        <v>1</v>
+      </c>
+      <c r="P506" s="10">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q506" s="10">
+        <f t="shared" si="24"/>
+        <v>27</v>
+      </c>
+      <c r="R506" s="10">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S506" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T506" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="507" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A507" s="9">
+        <v>45660</v>
+      </c>
+      <c r="B507" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C507" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D507" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E507" s="10">
+        <v>0</v>
+      </c>
+      <c r="F507" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G507" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H507" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I507" s="10">
+        <v>236.5</v>
+      </c>
+      <c r="J507" s="11">
+        <v>-5.5</v>
+      </c>
+      <c r="K507" s="10">
+        <v>113</v>
+      </c>
+      <c r="L507" s="10">
+        <v>110</v>
+      </c>
+      <c r="M507" s="10">
+        <f t="shared" si="21"/>
+        <v>223</v>
+      </c>
+      <c r="N507" s="10">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="O507" s="10">
+        <v>1</v>
+      </c>
+      <c r="P507" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q507" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R507" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S507" s="10">
+        <f t="shared" si="26"/>
+        <v>13.5</v>
+      </c>
+      <c r="T507" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="508" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A508" s="9">
+        <v>45660</v>
+      </c>
+      <c r="B508" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C508" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D508" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E508" s="10">
+        <v>0</v>
+      </c>
+      <c r="F508" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G508" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H508" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I508" s="10">
+        <v>237.5</v>
+      </c>
+      <c r="J508" s="11">
+        <v>-4.5</v>
+      </c>
+      <c r="K508" s="10">
+        <v>133</v>
+      </c>
+      <c r="L508" s="10">
+        <v>138</v>
+      </c>
+      <c r="M508" s="10">
+        <f t="shared" si="21"/>
+        <v>271</v>
+      </c>
+      <c r="N508" s="10">
+        <f t="shared" si="22"/>
+        <v>-5</v>
+      </c>
+      <c r="O508" s="10">
+        <v>1</v>
+      </c>
+      <c r="P508" s="10">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q508" s="10">
+        <f t="shared" si="24"/>
+        <v>33.5</v>
+      </c>
+      <c r="R508" s="10">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S508" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T508" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="509" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A509" s="9">
+        <v>45660</v>
+      </c>
+      <c r="B509" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C509" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D509" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E509" s="10">
+        <v>0</v>
+      </c>
+      <c r="F509" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G509" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H509" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I509" s="10">
+        <v>232</v>
+      </c>
+      <c r="J509" s="11">
+        <v>-4.5</v>
+      </c>
+      <c r="K509" s="10">
+        <v>102</v>
+      </c>
+      <c r="L509" s="10">
+        <v>119</v>
+      </c>
+      <c r="M509" s="10">
+        <f t="shared" si="21"/>
+        <v>221</v>
+      </c>
+      <c r="N509" s="10">
+        <f t="shared" si="22"/>
+        <v>-17</v>
+      </c>
+      <c r="O509" s="10">
+        <v>1</v>
+      </c>
+      <c r="P509" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q509" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R509" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S509" s="10">
+        <f t="shared" si="26"/>
+        <v>11</v>
+      </c>
+      <c r="T509" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="510" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A510" s="6">
+        <v>45661</v>
+      </c>
+      <c r="B510" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C510" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D510" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E510" s="7">
+        <v>0</v>
+      </c>
+      <c r="F510" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G510" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H510" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I510" s="7">
+        <v>216</v>
+      </c>
+      <c r="J510" s="8">
+        <v>6.5</v>
+      </c>
+      <c r="K510" s="7">
+        <v>123</v>
+      </c>
+      <c r="L510" s="7">
+        <v>94</v>
+      </c>
+      <c r="M510" s="7">
+        <f t="shared" si="21"/>
+        <v>217</v>
+      </c>
+      <c r="N510" s="7">
+        <f t="shared" si="22"/>
+        <v>29</v>
+      </c>
+      <c r="O510" s="7">
+        <v>1</v>
+      </c>
+      <c r="P510" s="7">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q510" s="7">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="R510" s="7">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S510" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T510" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="511" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A511" s="6">
+        <v>45661</v>
+      </c>
+      <c r="B511" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C511" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D511" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E511" s="7">
+        <v>0</v>
+      </c>
+      <c r="F511" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G511" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H511" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I511" s="7">
+        <v>234.5</v>
+      </c>
+      <c r="J511" s="8">
+        <v>-2</v>
+      </c>
+      <c r="K511" s="7">
+        <v>108</v>
+      </c>
+      <c r="L511" s="7">
+        <v>126</v>
+      </c>
+      <c r="M511" s="7">
+        <f t="shared" si="21"/>
+        <v>234</v>
+      </c>
+      <c r="N511" s="7">
+        <f t="shared" si="22"/>
+        <v>-18</v>
+      </c>
+      <c r="O511" s="7">
+        <v>1</v>
+      </c>
+      <c r="P511" s="7">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q511" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R511" s="7">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S511" s="7">
+        <f t="shared" si="26"/>
+        <v>0.5</v>
+      </c>
+      <c r="T511" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="512" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A512" s="6">
+        <v>45661</v>
+      </c>
+      <c r="B512" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C512" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D512" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E512" s="7">
+        <v>0</v>
+      </c>
+      <c r="F512" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G512" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H512" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="I512" s="7">
+        <v>218</v>
+      </c>
+      <c r="J512" s="8">
+        <v>6</v>
+      </c>
+      <c r="K512" s="7">
+        <v>105</v>
+      </c>
+      <c r="L512" s="7">
+        <v>119</v>
+      </c>
+      <c r="M512" s="7">
+        <f t="shared" si="21"/>
+        <v>224</v>
+      </c>
+      <c r="N512" s="7">
+        <f t="shared" si="22"/>
+        <v>-14</v>
+      </c>
+      <c r="O512" s="7">
+        <v>1</v>
+      </c>
+      <c r="P512" s="7">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q512" s="7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="R512" s="7">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S512" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T512" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="513" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A513" s="6">
+        <v>45661</v>
+      </c>
+      <c r="B513" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C513" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D513" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E513" s="7">
+        <v>0</v>
+      </c>
+      <c r="F513" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G513" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H513" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="I513" s="7">
+        <v>239</v>
+      </c>
+      <c r="J513" s="8">
+        <v>2</v>
+      </c>
+      <c r="K513" s="7">
+        <v>122</v>
+      </c>
+      <c r="L513" s="7">
+        <v>111</v>
+      </c>
+      <c r="M513" s="7">
+        <f t="shared" si="21"/>
+        <v>233</v>
+      </c>
+      <c r="N513" s="7">
+        <f t="shared" si="22"/>
+        <v>11</v>
+      </c>
+      <c r="O513" s="7">
+        <v>1</v>
+      </c>
+      <c r="P513" s="7">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q513" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R513" s="7">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S513" s="7">
+        <f t="shared" si="26"/>
+        <v>6</v>
+      </c>
+      <c r="T513" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="514" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A514" s="6">
+        <v>45661</v>
+      </c>
+      <c r="B514" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C514" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D514" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E514" s="7">
+        <v>0</v>
+      </c>
+      <c r="F514" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G514" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H514" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I514" s="7">
+        <v>228</v>
+      </c>
+      <c r="J514" s="8">
+        <v>-11.5</v>
+      </c>
+      <c r="K514" s="7">
+        <v>105</v>
+      </c>
+      <c r="L514" s="7">
+        <v>102</v>
+      </c>
+      <c r="M514" s="7">
+        <f t="shared" si="21"/>
+        <v>207</v>
+      </c>
+      <c r="N514" s="7">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="O514" s="7">
+        <v>1</v>
+      </c>
+      <c r="P514" s="7">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q514" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R514" s="7">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S514" s="7">
+        <f t="shared" si="26"/>
+        <v>21</v>
+      </c>
+      <c r="T514" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="515" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A515" s="6">
+        <v>45661</v>
+      </c>
+      <c r="B515" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C515" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D515" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E515" s="7">
+        <v>0</v>
+      </c>
+      <c r="F515" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G515" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H515" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I515" s="7">
+        <v>224.5</v>
+      </c>
+      <c r="J515" s="8">
+        <v>-8.5</v>
+      </c>
+      <c r="K515" s="7">
+        <v>136</v>
+      </c>
+      <c r="L515" s="7">
+        <v>100</v>
+      </c>
+      <c r="M515" s="7">
+        <f t="shared" si="21"/>
+        <v>236</v>
+      </c>
+      <c r="N515" s="7">
+        <f t="shared" si="22"/>
+        <v>36</v>
+      </c>
+      <c r="O515" s="7">
+        <v>1</v>
+      </c>
+      <c r="P515" s="7">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q515" s="7">
+        <f t="shared" si="24"/>
+        <v>11.5</v>
+      </c>
+      <c r="R515" s="7">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S515" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T515" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="516" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A516" s="6">
+        <v>45661</v>
+      </c>
+      <c r="B516" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C516" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D516" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E516" s="7">
+        <v>0</v>
+      </c>
+      <c r="F516" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G516" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H516" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="I516" s="7">
+        <v>233</v>
+      </c>
+      <c r="J516" s="8">
+        <v>6</v>
+      </c>
+      <c r="K516" s="7">
+        <v>126</v>
+      </c>
+      <c r="L516" s="7">
+        <v>139</v>
+      </c>
+      <c r="M516" s="7">
+        <f t="shared" si="21"/>
+        <v>265</v>
+      </c>
+      <c r="N516" s="7">
+        <f t="shared" si="22"/>
+        <v>-13</v>
+      </c>
+      <c r="O516" s="7">
+        <v>1</v>
+      </c>
+      <c r="P516" s="7">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q516" s="7">
+        <f t="shared" si="24"/>
+        <v>32</v>
+      </c>
+      <c r="R516" s="7">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S516" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T516" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="517" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A517" s="6">
+        <v>45661</v>
+      </c>
+      <c r="B517" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C517" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D517" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E517" s="7">
+        <v>0</v>
+      </c>
+      <c r="F517" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G517" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H517" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I517" s="7">
+        <v>238</v>
+      </c>
+      <c r="J517" s="8">
+        <v>-6.5</v>
+      </c>
+      <c r="K517" s="7">
+        <v>113</v>
+      </c>
+      <c r="L517" s="7">
+        <v>121</v>
+      </c>
+      <c r="M517" s="7">
+        <f t="shared" si="21"/>
+        <v>234</v>
+      </c>
+      <c r="N517" s="7">
+        <f t="shared" si="22"/>
+        <v>-8</v>
+      </c>
+      <c r="O517" s="7">
+        <v>1</v>
+      </c>
+      <c r="P517" s="7">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q517" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R517" s="7">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S517" s="7">
+        <f t="shared" si="26"/>
+        <v>4</v>
+      </c>
+      <c r="T517" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="518" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A518" s="6">
+        <v>45661</v>
+      </c>
+      <c r="B518" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C518" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D518" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E518" s="7">
+        <v>0</v>
+      </c>
+      <c r="F518" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G518" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H518" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I518" s="7">
+        <v>229.5</v>
+      </c>
+      <c r="J518" s="8">
+        <v>-3</v>
+      </c>
+      <c r="K518" s="7">
+        <v>105</v>
+      </c>
+      <c r="L518" s="7">
+        <v>131</v>
+      </c>
+      <c r="M518" s="7">
+        <f t="shared" si="21"/>
+        <v>236</v>
+      </c>
+      <c r="N518" s="7">
+        <f t="shared" si="22"/>
+        <v>-26</v>
+      </c>
+      <c r="O518" s="7">
+        <v>1</v>
+      </c>
+      <c r="P518" s="7">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q518" s="7">
+        <f t="shared" si="24"/>
+        <v>6.5</v>
+      </c>
+      <c r="R518" s="7">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S518" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T518" s="7">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added game data, updated EDA notebook
</commit_message>
<xml_diff>
--- a/data/nba_points_2024_2025.xlsx
+++ b/data/nba_points_2024_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Documents/nba-points/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE039625-2A52-9446-B17E-4753E1F41A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40E0E7F-E6EB-C945-877A-691D9342CE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22940" yWindow="500" windowWidth="45860" windowHeight="28300" xr2:uid="{4B944735-6DC1-314A-AF10-68EBB82A81F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3133" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3265" uniqueCount="147">
   <si>
     <t>Date</t>
   </si>
@@ -1001,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78582E2E-5746-944D-860C-ACA920BD70CB}">
-  <dimension ref="A1:Y518"/>
+  <dimension ref="A1:Y540"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A473" workbookViewId="0">
-      <selection activeCell="Q502" sqref="Q502"/>
+    <sheetView tabSelected="1" topLeftCell="A492" workbookViewId="0">
+      <selection activeCell="L544" sqref="L544"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1179,15 +1179,15 @@
       </c>
       <c r="V2" s="7">
         <f>SUM(O:O)</f>
-        <v>515</v>
+        <v>537</v>
       </c>
       <c r="W2" s="12">
         <f>SUM(P:P)</f>
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="X2" s="15">
         <f>SUM(R:R)</f>
-        <v>251</v>
+        <v>266</v>
       </c>
       <c r="Y2" s="20">
         <f>SUM(T:T)</f>
@@ -1342,15 +1342,15 @@
       </c>
       <c r="W4" s="14">
         <f>W2/V2</f>
-        <v>0.51067961165048548</v>
+        <v>0.5027932960893855</v>
       </c>
       <c r="X4" s="16">
         <f>X2/V2</f>
-        <v>0.48737864077669901</v>
+        <v>0.49534450651769085</v>
       </c>
       <c r="Y4" s="21">
         <f>Y2/V2</f>
-        <v>1.9417475728155339E-3</v>
+        <v>1.8621973929236499E-3</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1498,11 +1498,11 @@
       </c>
       <c r="W6" s="22">
         <f>AVERAGE(Q:Q)</f>
-        <v>15.20722433460076</v>
+        <v>15.09074074074074</v>
       </c>
       <c r="X6" s="23">
         <f>AVERAGE(S:S)</f>
-        <v>15.350597609561753</v>
+        <v>15.25187969924812</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -33813,34 +33813,34 @@
         <v>108</v>
       </c>
       <c r="M475" s="10">
-        <f t="shared" ref="M475:M518" si="21">K475+L475</f>
+        <f t="shared" ref="M475:M540" si="21">K475+L475</f>
         <v>223</v>
       </c>
       <c r="N475" s="10">
-        <f t="shared" ref="N475:N518" si="22">(L475-K475)*-1</f>
+        <f t="shared" ref="N475:N540" si="22">(L475-K475)*-1</f>
         <v>7</v>
       </c>
       <c r="O475" s="10">
         <v>1</v>
       </c>
       <c r="P475" s="10">
-        <f t="shared" ref="P475:P518" si="23">IF(M475&gt;I475,1,0)</f>
+        <f t="shared" ref="P475:P540" si="23">IF(M475&gt;I475,1,0)</f>
         <v>0</v>
       </c>
       <c r="Q475" s="10" t="str">
-        <f t="shared" ref="Q475:Q518" si="24">IF(P475=1,(M475-I475), "")</f>
+        <f t="shared" ref="Q475:Q540" si="24">IF(P475=1,(M475-I475), "")</f>
         <v/>
       </c>
       <c r="R475" s="10">
-        <f t="shared" ref="R475:R518" si="25">IF(M475&lt;I475, 1, 0)</f>
+        <f t="shared" ref="R475:R540" si="25">IF(M475&lt;I475, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="S475" s="10">
-        <f t="shared" ref="S475:S518" si="26">IF(R475=1,(I475-M475),"")</f>
+        <f t="shared" ref="S475:S540" si="26">IF(R475=1,(I475-M475),"")</f>
         <v>3.5</v>
       </c>
       <c r="T475" s="10">
-        <f t="shared" ref="T475:T518" si="27">IF(M475=I475,1,0)</f>
+        <f t="shared" ref="T475:T540" si="27">IF(M475=I475,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -36807,6 +36807,1524 @@
         <v/>
       </c>
       <c r="T518" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="519" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A519" s="9">
+        <v>45662</v>
+      </c>
+      <c r="B519" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C519" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D519" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E519" s="10">
+        <v>0</v>
+      </c>
+      <c r="F519" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G519" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H519" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I519" s="10">
+        <v>224</v>
+      </c>
+      <c r="J519" s="11">
+        <v>-2</v>
+      </c>
+      <c r="K519" s="10">
+        <v>92</v>
+      </c>
+      <c r="L519" s="10">
+        <v>105</v>
+      </c>
+      <c r="M519" s="10">
+        <f t="shared" si="21"/>
+        <v>197</v>
+      </c>
+      <c r="N519" s="10">
+        <f t="shared" si="22"/>
+        <v>-13</v>
+      </c>
+      <c r="O519" s="10">
+        <v>1</v>
+      </c>
+      <c r="P519" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q519" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R519" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S519" s="10">
+        <f t="shared" si="26"/>
+        <v>27</v>
+      </c>
+      <c r="T519" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="520" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A520" s="9">
+        <v>45662</v>
+      </c>
+      <c r="B520" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C520" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D520" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E520" s="10">
+        <v>0</v>
+      </c>
+      <c r="F520" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G520" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H520" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I520" s="10">
+        <v>238.5</v>
+      </c>
+      <c r="J520" s="11">
+        <v>4</v>
+      </c>
+      <c r="K520" s="10">
+        <v>110</v>
+      </c>
+      <c r="L520" s="10">
+        <v>98</v>
+      </c>
+      <c r="M520" s="10">
+        <f t="shared" si="21"/>
+        <v>208</v>
+      </c>
+      <c r="N520" s="10">
+        <f t="shared" si="22"/>
+        <v>12</v>
+      </c>
+      <c r="O520" s="10">
+        <v>1</v>
+      </c>
+      <c r="P520" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q520" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R520" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S520" s="10">
+        <f t="shared" si="26"/>
+        <v>30.5</v>
+      </c>
+      <c r="T520" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="521" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A521" s="9">
+        <v>45662</v>
+      </c>
+      <c r="B521" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C521" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D521" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E521" s="10">
+        <v>0</v>
+      </c>
+      <c r="F521" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G521" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H521" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I521" s="10">
+        <v>221.5</v>
+      </c>
+      <c r="J521" s="11">
+        <v>-15.5</v>
+      </c>
+      <c r="K521" s="10">
+        <v>105</v>
+      </c>
+      <c r="L521" s="10">
+        <v>115</v>
+      </c>
+      <c r="M521" s="10">
+        <f t="shared" si="21"/>
+        <v>220</v>
+      </c>
+      <c r="N521" s="10">
+        <f t="shared" si="22"/>
+        <v>-10</v>
+      </c>
+      <c r="O521" s="10">
+        <v>1</v>
+      </c>
+      <c r="P521" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q521" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R521" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S521" s="10">
+        <f t="shared" si="26"/>
+        <v>1.5</v>
+      </c>
+      <c r="T521" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="522" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A522" s="9">
+        <v>45662</v>
+      </c>
+      <c r="B522" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C522" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D522" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E522" s="10">
+        <v>0</v>
+      </c>
+      <c r="F522" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G522" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H522" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I522" s="10">
+        <v>212.5</v>
+      </c>
+      <c r="J522" s="11">
+        <v>-8.5</v>
+      </c>
+      <c r="K522" s="10">
+        <v>105</v>
+      </c>
+      <c r="L522" s="10">
+        <v>92</v>
+      </c>
+      <c r="M522" s="10">
+        <f t="shared" si="21"/>
+        <v>197</v>
+      </c>
+      <c r="N522" s="10">
+        <f t="shared" si="22"/>
+        <v>13</v>
+      </c>
+      <c r="O522" s="10">
+        <v>1</v>
+      </c>
+      <c r="P522" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q522" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R522" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S522" s="10">
+        <f t="shared" si="26"/>
+        <v>15.5</v>
+      </c>
+      <c r="T522" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="523" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A523" s="9">
+        <v>45662</v>
+      </c>
+      <c r="B523" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C523" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D523" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E523" s="10">
+        <v>0</v>
+      </c>
+      <c r="F523" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G523" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H523" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="I523" s="10">
+        <v>221.5</v>
+      </c>
+      <c r="J523" s="11">
+        <v>-4.5</v>
+      </c>
+      <c r="K523" s="10">
+        <v>115</v>
+      </c>
+      <c r="L523" s="10">
+        <v>119</v>
+      </c>
+      <c r="M523" s="10">
+        <f t="shared" si="21"/>
+        <v>234</v>
+      </c>
+      <c r="N523" s="10">
+        <f t="shared" si="22"/>
+        <v>-4</v>
+      </c>
+      <c r="O523" s="10">
+        <v>1</v>
+      </c>
+      <c r="P523" s="10">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q523" s="10">
+        <f t="shared" si="24"/>
+        <v>12.5</v>
+      </c>
+      <c r="R523" s="10">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S523" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T523" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="524" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A524" s="9">
+        <v>45662</v>
+      </c>
+      <c r="B524" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C524" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D524" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E524" s="10">
+        <v>0</v>
+      </c>
+      <c r="F524" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G524" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H524" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I524" s="10">
+        <v>229.5</v>
+      </c>
+      <c r="J524" s="11">
+        <v>-1</v>
+      </c>
+      <c r="K524" s="10">
+        <v>129</v>
+      </c>
+      <c r="L524" s="10">
+        <v>99</v>
+      </c>
+      <c r="M524" s="10">
+        <f t="shared" si="21"/>
+        <v>228</v>
+      </c>
+      <c r="N524" s="10">
+        <f t="shared" si="22"/>
+        <v>30</v>
+      </c>
+      <c r="O524" s="10">
+        <v>1</v>
+      </c>
+      <c r="P524" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q524" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R524" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S524" s="10">
+        <f t="shared" si="26"/>
+        <v>1.5</v>
+      </c>
+      <c r="T524" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="525" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A525" s="6">
+        <v>45663</v>
+      </c>
+      <c r="B525" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C525" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D525" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E525" s="7">
+        <v>0</v>
+      </c>
+      <c r="F525" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G525" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H525" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I525" s="7">
+        <v>227.5</v>
+      </c>
+      <c r="J525" s="8">
+        <v>-3.5</v>
+      </c>
+      <c r="K525" s="7">
+        <v>109</v>
+      </c>
+      <c r="L525" s="7">
+        <v>99</v>
+      </c>
+      <c r="M525" s="7">
+        <f t="shared" si="21"/>
+        <v>208</v>
+      </c>
+      <c r="N525" s="7">
+        <f t="shared" si="22"/>
+        <v>10</v>
+      </c>
+      <c r="O525" s="7">
+        <v>1</v>
+      </c>
+      <c r="P525" s="7">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q525" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R525" s="7">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S525" s="7">
+        <f t="shared" si="26"/>
+        <v>19.5</v>
+      </c>
+      <c r="T525" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="526" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A526" s="6">
+        <v>45663</v>
+      </c>
+      <c r="B526" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C526" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D526" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E526" s="7">
+        <v>0</v>
+      </c>
+      <c r="F526" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G526" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H526" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I526" s="7">
+        <v>225.5</v>
+      </c>
+      <c r="J526" s="8">
+        <v>-5.5</v>
+      </c>
+      <c r="K526" s="7">
+        <v>115</v>
+      </c>
+      <c r="L526" s="7">
+        <v>118</v>
+      </c>
+      <c r="M526" s="7">
+        <f t="shared" si="21"/>
+        <v>233</v>
+      </c>
+      <c r="N526" s="7">
+        <f t="shared" si="22"/>
+        <v>-3</v>
+      </c>
+      <c r="O526" s="7">
+        <v>1</v>
+      </c>
+      <c r="P526" s="7">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q526" s="7">
+        <f t="shared" si="24"/>
+        <v>7.5</v>
+      </c>
+      <c r="R526" s="7">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S526" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T526" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="527" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A527" s="6">
+        <v>45663</v>
+      </c>
+      <c r="B527" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C527" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D527" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E527" s="7">
+        <v>0</v>
+      </c>
+      <c r="F527" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G527" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H527" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="I527" s="7">
+        <v>226</v>
+      </c>
+      <c r="J527" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="K527" s="7">
+        <v>128</v>
+      </c>
+      <c r="L527" s="7">
+        <v>104</v>
+      </c>
+      <c r="M527" s="7">
+        <f t="shared" si="21"/>
+        <v>232</v>
+      </c>
+      <c r="N527" s="7">
+        <f t="shared" si="22"/>
+        <v>24</v>
+      </c>
+      <c r="O527" s="7">
+        <v>1</v>
+      </c>
+      <c r="P527" s="7">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q527" s="7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="R527" s="7">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S527" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T527" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="528" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A528" s="6">
+        <v>45663</v>
+      </c>
+      <c r="B528" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C528" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D528" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E528" s="7">
+        <v>0</v>
+      </c>
+      <c r="F528" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G528" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H528" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="I528" s="7">
+        <v>210</v>
+      </c>
+      <c r="J528" s="8">
+        <v>-11.5</v>
+      </c>
+      <c r="K528" s="7">
+        <v>103</v>
+      </c>
+      <c r="L528" s="7">
+        <v>94</v>
+      </c>
+      <c r="M528" s="7">
+        <f t="shared" si="21"/>
+        <v>197</v>
+      </c>
+      <c r="N528" s="7">
+        <f t="shared" si="22"/>
+        <v>9</v>
+      </c>
+      <c r="O528" s="7">
+        <v>1</v>
+      </c>
+      <c r="P528" s="7">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q528" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R528" s="7">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S528" s="7">
+        <f t="shared" si="26"/>
+        <v>13</v>
+      </c>
+      <c r="T528" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="529" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A529" s="6">
+        <v>45663</v>
+      </c>
+      <c r="B529" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C529" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D529" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E529" s="7">
+        <v>0</v>
+      </c>
+      <c r="F529" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G529" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H529" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I529" s="7">
+        <v>224.5</v>
+      </c>
+      <c r="J529" s="8">
+        <v>8</v>
+      </c>
+      <c r="K529" s="7">
+        <v>113</v>
+      </c>
+      <c r="L529" s="7">
+        <v>99</v>
+      </c>
+      <c r="M529" s="7">
+        <f t="shared" si="21"/>
+        <v>212</v>
+      </c>
+      <c r="N529" s="7">
+        <f t="shared" si="22"/>
+        <v>14</v>
+      </c>
+      <c r="O529" s="7">
+        <v>1</v>
+      </c>
+      <c r="P529" s="7">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q529" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R529" s="7">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S529" s="7">
+        <f t="shared" si="26"/>
+        <v>12.5</v>
+      </c>
+      <c r="T529" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="530" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A530" s="6">
+        <v>45663</v>
+      </c>
+      <c r="B530" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C530" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D530" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E530" s="7">
+        <v>0</v>
+      </c>
+      <c r="F530" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G530" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H530" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="I530" s="7">
+        <v>211.5</v>
+      </c>
+      <c r="J530" s="8">
+        <v>-3</v>
+      </c>
+      <c r="K530" s="7">
+        <v>106</v>
+      </c>
+      <c r="L530" s="7">
+        <v>108</v>
+      </c>
+      <c r="M530" s="7">
+        <f t="shared" si="21"/>
+        <v>214</v>
+      </c>
+      <c r="N530" s="7">
+        <f t="shared" si="22"/>
+        <v>-2</v>
+      </c>
+      <c r="O530" s="7">
+        <v>1</v>
+      </c>
+      <c r="P530" s="7">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q530" s="7">
+        <f t="shared" si="24"/>
+        <v>2.5</v>
+      </c>
+      <c r="R530" s="7">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S530" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T530" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="531" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A531" s="6">
+        <v>45663</v>
+      </c>
+      <c r="B531" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C531" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D531" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E531" s="7">
+        <v>0</v>
+      </c>
+      <c r="F531" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G531" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H531" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I531" s="7">
+        <v>236.5</v>
+      </c>
+      <c r="J531" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="K531" s="7">
+        <v>110</v>
+      </c>
+      <c r="L531" s="7">
+        <v>114</v>
+      </c>
+      <c r="M531" s="7">
+        <f t="shared" si="21"/>
+        <v>224</v>
+      </c>
+      <c r="N531" s="7">
+        <f t="shared" si="22"/>
+        <v>-4</v>
+      </c>
+      <c r="O531" s="7">
+        <v>1</v>
+      </c>
+      <c r="P531" s="7">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q531" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R531" s="7">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S531" s="7">
+        <f t="shared" si="26"/>
+        <v>12.5</v>
+      </c>
+      <c r="T531" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="532" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A532" s="6">
+        <v>45663</v>
+      </c>
+      <c r="B532" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C532" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D532" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E532" s="7">
+        <v>0</v>
+      </c>
+      <c r="F532" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G532" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H532" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I532" s="7">
+        <v>238.5</v>
+      </c>
+      <c r="J532" s="8">
+        <v>-4</v>
+      </c>
+      <c r="K532" s="7">
+        <v>104</v>
+      </c>
+      <c r="L532" s="7">
+        <v>119</v>
+      </c>
+      <c r="M532" s="7">
+        <f t="shared" si="21"/>
+        <v>223</v>
+      </c>
+      <c r="N532" s="7">
+        <f t="shared" si="22"/>
+        <v>-15</v>
+      </c>
+      <c r="O532" s="7">
+        <v>1</v>
+      </c>
+      <c r="P532" s="7">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q532" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R532" s="7">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S532" s="7">
+        <f t="shared" si="26"/>
+        <v>15.5</v>
+      </c>
+      <c r="T532" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="533" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A533" s="6">
+        <v>45663</v>
+      </c>
+      <c r="B533" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C533" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D533" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E533" s="7">
+        <v>0</v>
+      </c>
+      <c r="F533" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G533" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H533" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I533" s="7">
+        <v>224.5</v>
+      </c>
+      <c r="J533" s="8">
+        <v>-2.5</v>
+      </c>
+      <c r="K533" s="7">
+        <v>118</v>
+      </c>
+      <c r="L533" s="7">
+        <v>123</v>
+      </c>
+      <c r="M533" s="7">
+        <f t="shared" si="21"/>
+        <v>241</v>
+      </c>
+      <c r="N533" s="7">
+        <f t="shared" si="22"/>
+        <v>-5</v>
+      </c>
+      <c r="O533" s="7">
+        <v>1</v>
+      </c>
+      <c r="P533" s="7">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q533" s="7">
+        <f t="shared" si="24"/>
+        <v>16.5</v>
+      </c>
+      <c r="R533" s="7">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S533" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T533" s="7">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="534" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A534" s="9">
+        <v>45664</v>
+      </c>
+      <c r="B534" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C534" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D534" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E534" s="10">
+        <v>0</v>
+      </c>
+      <c r="F534" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G534" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H534" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I534" s="10">
+        <v>225.5</v>
+      </c>
+      <c r="J534" s="11">
+        <v>9.5</v>
+      </c>
+      <c r="K534" s="10">
+        <v>135</v>
+      </c>
+      <c r="L534" s="10">
+        <v>112</v>
+      </c>
+      <c r="M534" s="10">
+        <f t="shared" si="21"/>
+        <v>247</v>
+      </c>
+      <c r="N534" s="10">
+        <f t="shared" si="22"/>
+        <v>23</v>
+      </c>
+      <c r="O534" s="10">
+        <v>1</v>
+      </c>
+      <c r="P534" s="10">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q534" s="10">
+        <f t="shared" si="24"/>
+        <v>21.5</v>
+      </c>
+      <c r="R534" s="10">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S534" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T534" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="535" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A535" s="9">
+        <v>45664</v>
+      </c>
+      <c r="B535" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C535" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D535" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E535" s="10">
+        <v>0</v>
+      </c>
+      <c r="F535" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G535" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H535" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I535" s="10">
+        <v>221.5</v>
+      </c>
+      <c r="J535" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="K535" s="10">
+        <v>104</v>
+      </c>
+      <c r="L535" s="10">
+        <v>115</v>
+      </c>
+      <c r="M535" s="10">
+        <f t="shared" si="21"/>
+        <v>219</v>
+      </c>
+      <c r="N535" s="10">
+        <f t="shared" si="22"/>
+        <v>-11</v>
+      </c>
+      <c r="O535" s="10">
+        <v>1</v>
+      </c>
+      <c r="P535" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q535" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R535" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S535" s="10">
+        <f t="shared" si="26"/>
+        <v>2.5</v>
+      </c>
+      <c r="T535" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="536" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A536" s="9">
+        <v>45664</v>
+      </c>
+      <c r="B536" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C536" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D536" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E536" s="10">
+        <v>0</v>
+      </c>
+      <c r="F536" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G536" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H536" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I536" s="10">
+        <v>225.5</v>
+      </c>
+      <c r="J536" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="K536" s="10">
+        <v>97</v>
+      </c>
+      <c r="L536" s="10">
+        <v>118</v>
+      </c>
+      <c r="M536" s="10">
+        <f t="shared" si="21"/>
+        <v>215</v>
+      </c>
+      <c r="N536" s="10">
+        <f t="shared" si="22"/>
+        <v>-21</v>
+      </c>
+      <c r="O536" s="10">
+        <v>1</v>
+      </c>
+      <c r="P536" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q536" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R536" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S536" s="10">
+        <f t="shared" si="26"/>
+        <v>10.5</v>
+      </c>
+      <c r="T536" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="537" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A537" s="9">
+        <v>45664</v>
+      </c>
+      <c r="B537" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C537" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D537" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E537" s="10">
+        <v>0</v>
+      </c>
+      <c r="F537" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G537" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="H537" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="I537" s="10">
+        <v>223</v>
+      </c>
+      <c r="J537" s="11">
+        <v>5</v>
+      </c>
+      <c r="K537" s="10">
+        <v>104</v>
+      </c>
+      <c r="L537" s="10">
+        <v>97</v>
+      </c>
+      <c r="M537" s="10">
+        <f t="shared" si="21"/>
+        <v>201</v>
+      </c>
+      <c r="N537" s="10">
+        <f t="shared" si="22"/>
+        <v>7</v>
+      </c>
+      <c r="O537" s="10">
+        <v>1</v>
+      </c>
+      <c r="P537" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q537" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R537" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S537" s="10">
+        <f t="shared" si="26"/>
+        <v>22</v>
+      </c>
+      <c r="T537" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="538" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A538" s="9">
+        <v>45664</v>
+      </c>
+      <c r="B538" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C538" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D538" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E538" s="10">
+        <v>0</v>
+      </c>
+      <c r="F538" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G538" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H538" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I538" s="10">
+        <v>236.5</v>
+      </c>
+      <c r="J538" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="K538" s="10">
+        <v>124</v>
+      </c>
+      <c r="L538" s="10">
+        <v>121</v>
+      </c>
+      <c r="M538" s="10">
+        <f t="shared" si="21"/>
+        <v>245</v>
+      </c>
+      <c r="N538" s="10">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="O538" s="10">
+        <v>1</v>
+      </c>
+      <c r="P538" s="10">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q538" s="10">
+        <f t="shared" si="24"/>
+        <v>8.5</v>
+      </c>
+      <c r="R538" s="10">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S538" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="T538" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="539" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A539" s="9">
+        <v>45664</v>
+      </c>
+      <c r="B539" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C539" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D539" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E539" s="10">
+        <v>0</v>
+      </c>
+      <c r="F539" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G539" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H539" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="I539" s="10">
+        <v>237.5</v>
+      </c>
+      <c r="J539" s="11">
+        <v>4</v>
+      </c>
+      <c r="K539" s="10">
+        <v>118</v>
+      </c>
+      <c r="L539" s="10">
+        <v>106</v>
+      </c>
+      <c r="M539" s="10">
+        <f t="shared" si="21"/>
+        <v>224</v>
+      </c>
+      <c r="N539" s="10">
+        <f t="shared" si="22"/>
+        <v>12</v>
+      </c>
+      <c r="O539" s="10">
+        <v>1</v>
+      </c>
+      <c r="P539" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q539" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R539" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S539" s="10">
+        <f t="shared" si="26"/>
+        <v>13.5</v>
+      </c>
+      <c r="T539" s="10">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="540" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A540" s="9">
+        <v>45664</v>
+      </c>
+      <c r="B540" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C540" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D540" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E540" s="10">
+        <v>0</v>
+      </c>
+      <c r="F540" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G540" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H540" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I540" s="10">
+        <v>218.5</v>
+      </c>
+      <c r="J540" s="11">
+        <v>-7</v>
+      </c>
+      <c r="K540" s="10">
+        <v>114</v>
+      </c>
+      <c r="L540" s="10">
+        <v>98</v>
+      </c>
+      <c r="M540" s="10">
+        <f t="shared" si="21"/>
+        <v>212</v>
+      </c>
+      <c r="N540" s="10">
+        <f t="shared" si="22"/>
+        <v>16</v>
+      </c>
+      <c r="O540" s="10">
+        <v>1</v>
+      </c>
+      <c r="P540" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q540" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="R540" s="10">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="S540" s="10">
+        <f t="shared" si="26"/>
+        <v>6.5</v>
+      </c>
+      <c r="T540" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added some game data
</commit_message>
<xml_diff>
--- a/data/nba_points_2024_2025.xlsx
+++ b/data/nba_points_2024_2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Documents/nba-points/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E19977-EB09-4F48-AE87-78DF82E7C6E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4404DD9D-6FA4-2245-A52B-CD0C3B777A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22940" yWindow="500" windowWidth="45860" windowHeight="28300" xr2:uid="{4B944735-6DC1-314A-AF10-68EBB82A81F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3559" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3754" uniqueCount="148">
   <si>
     <t>Date</t>
   </si>
@@ -528,7 +528,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -565,6 +565,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -593,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -677,6 +683,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1013,10 +1031,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78582E2E-5746-944D-860C-ACA920BD70CB}">
-  <dimension ref="A1:Y589"/>
+  <dimension ref="A1:Y649"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K597" sqref="K597"/>
+      <pane ySplit="1" topLeftCell="A598" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G618" sqref="G618"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1191,15 +1210,15 @@
       </c>
       <c r="V2" s="7">
         <f>SUM(O:O)</f>
-        <v>584</v>
+        <v>634</v>
       </c>
       <c r="W2" s="12">
         <f>SUM(P:P)</f>
-        <v>297</v>
+        <v>326</v>
       </c>
       <c r="X2" s="15">
         <f>SUM(R:R)</f>
-        <v>286</v>
+        <v>308</v>
       </c>
       <c r="Y2" s="20">
         <f>SUM(T:T)</f>
@@ -1354,15 +1373,15 @@
       </c>
       <c r="W4" s="14">
         <f>W2/V2</f>
-        <v>0.50856164383561642</v>
+        <v>0.51419558359621453</v>
       </c>
       <c r="X4" s="16">
         <f>X2/V2</f>
-        <v>0.48972602739726029</v>
+        <v>0.48580441640378547</v>
       </c>
       <c r="Y4" s="21">
         <f>Y2/V2</f>
-        <v>1.7123287671232876E-3</v>
+        <v>1.5772870662460567E-3</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1510,11 +1529,11 @@
       </c>
       <c r="W6" s="22">
         <f>AVERAGE(Q:Q)</f>
-        <v>14.54040404040404</v>
+        <v>15.032208588957054</v>
       </c>
       <c r="X6" s="23">
         <f>AVERAGE(S:S)</f>
-        <v>15.017482517482517</v>
+        <v>15.102272727272727</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1662,7 +1681,7 @@
       </c>
       <c r="W8" s="22">
         <f>MEDIAN(Q:Q)</f>
-        <v>11.5</v>
+        <v>12</v>
       </c>
       <c r="X8" s="23">
         <f>MEDIAN(S:S)</f>
@@ -39605,23 +39624,23 @@
         <v>1</v>
       </c>
       <c r="P559" s="7">
-        <f t="shared" ref="P559:P589" si="28">IF(M559&gt;I559,1,0)</f>
+        <f t="shared" ref="P559:P640" si="28">IF(M559&gt;I559,1,0)</f>
         <v>1</v>
       </c>
       <c r="Q559" s="7">
-        <f t="shared" ref="Q559:Q589" si="29">IF(P559=1,(M559-I559), "")</f>
+        <f t="shared" ref="Q559:Q640" si="29">IF(P559=1,(M559-I559), "")</f>
         <v>18.5</v>
       </c>
       <c r="R559" s="7">
-        <f t="shared" ref="R559:R589" si="30">IF(M559&lt;I559, 1, 0)</f>
+        <f t="shared" ref="R559:R640" si="30">IF(M559&lt;I559, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="S559" s="7" t="str">
-        <f t="shared" ref="S559:S589" si="31">IF(R559=1,(I559-M559),"")</f>
+        <f t="shared" ref="S559:S640" si="31">IF(R559=1,(I559-M559),"")</f>
         <v/>
       </c>
       <c r="T559" s="7">
-        <f t="shared" ref="T559:T589" si="32">IF(M559=I559,1,0)</f>
+        <f t="shared" ref="T559:T640" si="32">IF(M559=I559,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -41505,11 +41524,11 @@
         <v>113</v>
       </c>
       <c r="M587" s="7">
-        <f t="shared" ref="M587:M589" si="33">K587+L587</f>
+        <f t="shared" ref="M587:M640" si="33">K587+L587</f>
         <v>232</v>
       </c>
       <c r="N587" s="7">
-        <f t="shared" ref="N587:N589" si="34">(L587-K587)*-1</f>
+        <f t="shared" ref="N587:N640" si="34">(L587-K587)*-1</f>
         <v>6</v>
       </c>
       <c r="O587" s="7">
@@ -41673,6 +41692,3472 @@
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="590" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A590" s="9">
+        <v>45672</v>
+      </c>
+      <c r="B590" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C590" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D590" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E590" s="10">
+        <v>0</v>
+      </c>
+      <c r="F590" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G590" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H590" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="I590" s="10">
+        <v>222.5</v>
+      </c>
+      <c r="J590" s="11">
+        <v>9</v>
+      </c>
+      <c r="K590" s="10">
+        <v>125</v>
+      </c>
+      <c r="L590" s="10">
+        <v>119</v>
+      </c>
+      <c r="M590" s="10">
+        <f t="shared" si="33"/>
+        <v>244</v>
+      </c>
+      <c r="N590" s="10">
+        <f t="shared" si="34"/>
+        <v>6</v>
+      </c>
+      <c r="O590" s="10">
+        <v>1</v>
+      </c>
+      <c r="P590" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q590" s="10">
+        <f t="shared" si="29"/>
+        <v>21.5</v>
+      </c>
+      <c r="R590" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S590" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T590" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="591" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A591" s="9">
+        <v>45672</v>
+      </c>
+      <c r="B591" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C591" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D591" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E591" s="10">
+        <v>0</v>
+      </c>
+      <c r="F591" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G591" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H591" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I591" s="10">
+        <v>229</v>
+      </c>
+      <c r="J591" s="11">
+        <v>12.5</v>
+      </c>
+      <c r="K591" s="10">
+        <v>97</v>
+      </c>
+      <c r="L591" s="10">
+        <v>110</v>
+      </c>
+      <c r="M591" s="10">
+        <f t="shared" si="33"/>
+        <v>207</v>
+      </c>
+      <c r="N591" s="10">
+        <f t="shared" si="34"/>
+        <v>-13</v>
+      </c>
+      <c r="O591" s="10">
+        <v>1</v>
+      </c>
+      <c r="P591" s="10">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q591" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R591" s="10">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S591" s="10">
+        <f t="shared" si="31"/>
+        <v>22</v>
+      </c>
+      <c r="T591" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="592" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A592" s="9">
+        <v>45672</v>
+      </c>
+      <c r="B592" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C592" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D592" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E592" s="10">
+        <v>0</v>
+      </c>
+      <c r="F592" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G592" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H592" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I592" s="10">
+        <v>224.5</v>
+      </c>
+      <c r="J592" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="K592" s="10">
+        <v>116</v>
+      </c>
+      <c r="L592" s="10">
+        <v>119</v>
+      </c>
+      <c r="M592" s="10">
+        <f t="shared" si="33"/>
+        <v>235</v>
+      </c>
+      <c r="N592" s="10">
+        <f t="shared" si="34"/>
+        <v>-3</v>
+      </c>
+      <c r="O592" s="10">
+        <v>1</v>
+      </c>
+      <c r="P592" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q592" s="10">
+        <f t="shared" si="29"/>
+        <v>10.5</v>
+      </c>
+      <c r="R592" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S592" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T592" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="593" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A593" s="9">
+        <v>45672</v>
+      </c>
+      <c r="B593" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C593" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D593" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E593" s="10">
+        <v>0</v>
+      </c>
+      <c r="F593" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G593" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H593" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I593" s="10">
+        <v>211.5</v>
+      </c>
+      <c r="J593" s="11">
+        <v>-6.5</v>
+      </c>
+      <c r="K593" s="10">
+        <v>93</v>
+      </c>
+      <c r="L593" s="10">
+        <v>122</v>
+      </c>
+      <c r="M593" s="10">
+        <f t="shared" si="33"/>
+        <v>215</v>
+      </c>
+      <c r="N593" s="10">
+        <f t="shared" si="34"/>
+        <v>-29</v>
+      </c>
+      <c r="O593" s="10">
+        <v>1</v>
+      </c>
+      <c r="P593" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q593" s="10">
+        <f t="shared" si="29"/>
+        <v>3.5</v>
+      </c>
+      <c r="R593" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S593" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T593" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="594" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A594" s="9">
+        <v>45672</v>
+      </c>
+      <c r="B594" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C594" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D594" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E594" s="10">
+        <v>0</v>
+      </c>
+      <c r="F594" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G594" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H594" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="I594" s="10">
+        <v>244.5</v>
+      </c>
+      <c r="J594" s="11">
+        <v>-2.5</v>
+      </c>
+      <c r="K594" s="10">
+        <v>110</v>
+      </c>
+      <c r="L594" s="10">
+        <v>94</v>
+      </c>
+      <c r="M594" s="10">
+        <f t="shared" si="33"/>
+        <v>204</v>
+      </c>
+      <c r="N594" s="10">
+        <f t="shared" si="34"/>
+        <v>16</v>
+      </c>
+      <c r="O594" s="10">
+        <v>1</v>
+      </c>
+      <c r="P594" s="10">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q594" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R594" s="10">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S594" s="10">
+        <f t="shared" si="31"/>
+        <v>40.5</v>
+      </c>
+      <c r="T594" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="595" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A595" s="9">
+        <v>45672</v>
+      </c>
+      <c r="B595" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C595" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D595" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E595" s="10">
+        <v>0</v>
+      </c>
+      <c r="F595" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G595" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H595" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I595" s="10">
+        <v>236.5</v>
+      </c>
+      <c r="J595" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="K595" s="10">
+        <v>129</v>
+      </c>
+      <c r="L595" s="10">
+        <v>115</v>
+      </c>
+      <c r="M595" s="10">
+        <f t="shared" si="33"/>
+        <v>244</v>
+      </c>
+      <c r="N595" s="10">
+        <f t="shared" si="34"/>
+        <v>14</v>
+      </c>
+      <c r="O595" s="10">
+        <v>1</v>
+      </c>
+      <c r="P595" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q595" s="10">
+        <f t="shared" si="29"/>
+        <v>7.5</v>
+      </c>
+      <c r="R595" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S595" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T595" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="596" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A596" s="9">
+        <v>45672</v>
+      </c>
+      <c r="B596" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C596" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D596" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E596" s="10">
+        <v>0</v>
+      </c>
+      <c r="F596" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G596" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H596" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I596" s="10">
+        <v>232.5</v>
+      </c>
+      <c r="J596" s="11">
+        <v>-1.5</v>
+      </c>
+      <c r="K596" s="10">
+        <v>128</v>
+      </c>
+      <c r="L596" s="10">
+        <v>108</v>
+      </c>
+      <c r="M596" s="10">
+        <f t="shared" si="33"/>
+        <v>236</v>
+      </c>
+      <c r="N596" s="10">
+        <f t="shared" si="34"/>
+        <v>20</v>
+      </c>
+      <c r="O596" s="10">
+        <v>1</v>
+      </c>
+      <c r="P596" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q596" s="10">
+        <f t="shared" si="29"/>
+        <v>3.5</v>
+      </c>
+      <c r="R596" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S596" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T596" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="597" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A597" s="9">
+        <v>45672</v>
+      </c>
+      <c r="B597" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C597" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D597" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E597" s="10">
+        <v>0</v>
+      </c>
+      <c r="F597" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G597" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H597" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I597" s="10">
+        <v>220.5</v>
+      </c>
+      <c r="J597" s="11">
+        <v>-1.5</v>
+      </c>
+      <c r="K597" s="10">
+        <v>117</v>
+      </c>
+      <c r="L597" s="10">
+        <v>112</v>
+      </c>
+      <c r="M597" s="10">
+        <f t="shared" si="33"/>
+        <v>229</v>
+      </c>
+      <c r="N597" s="10">
+        <f t="shared" si="34"/>
+        <v>5</v>
+      </c>
+      <c r="O597" s="10">
+        <v>1</v>
+      </c>
+      <c r="P597" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q597" s="10">
+        <f t="shared" si="29"/>
+        <v>8.5</v>
+      </c>
+      <c r="R597" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S597" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T597" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="598" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A598" s="9">
+        <v>45672</v>
+      </c>
+      <c r="B598" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C598" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D598" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E598" s="10">
+        <v>0</v>
+      </c>
+      <c r="F598" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G598" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H598" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="I598" s="10">
+        <v>215.5</v>
+      </c>
+      <c r="J598" s="11">
+        <v>-5.5</v>
+      </c>
+      <c r="K598" s="10">
+        <v>116</v>
+      </c>
+      <c r="L598" s="10">
+        <v>115</v>
+      </c>
+      <c r="M598" s="10">
+        <f t="shared" si="33"/>
+        <v>231</v>
+      </c>
+      <c r="N598" s="10">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+      <c r="O598" s="10">
+        <v>1</v>
+      </c>
+      <c r="P598" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q598" s="10">
+        <f t="shared" si="29"/>
+        <v>15.5</v>
+      </c>
+      <c r="R598" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S598" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T598" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="599" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A599" s="9">
+        <v>45672</v>
+      </c>
+      <c r="B599" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C599" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D599" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E599" s="10">
+        <v>0</v>
+      </c>
+      <c r="F599" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G599" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H599" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I599" s="10">
+        <v>218</v>
+      </c>
+      <c r="J599" s="11">
+        <v>-3.5</v>
+      </c>
+      <c r="K599" s="10">
+        <v>108</v>
+      </c>
+      <c r="L599" s="10">
+        <v>117</v>
+      </c>
+      <c r="M599" s="10">
+        <f t="shared" si="33"/>
+        <v>225</v>
+      </c>
+      <c r="N599" s="10">
+        <f t="shared" si="34"/>
+        <v>-9</v>
+      </c>
+      <c r="O599" s="10">
+        <v>1</v>
+      </c>
+      <c r="P599" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q599" s="10">
+        <f t="shared" si="29"/>
+        <v>7</v>
+      </c>
+      <c r="R599" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S599" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T599" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="600" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A600" s="9">
+        <v>45672</v>
+      </c>
+      <c r="B600" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C600" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D600" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E600" s="10">
+        <v>0</v>
+      </c>
+      <c r="F600" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G600" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H600" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I600" s="10">
+        <v>211.5</v>
+      </c>
+      <c r="J600" s="11">
+        <v>-14.5</v>
+      </c>
+      <c r="K600" s="10">
+        <v>67</v>
+      </c>
+      <c r="L600" s="10">
+        <v>126</v>
+      </c>
+      <c r="M600" s="10">
+        <f t="shared" si="33"/>
+        <v>193</v>
+      </c>
+      <c r="N600" s="10">
+        <f t="shared" si="34"/>
+        <v>-59</v>
+      </c>
+      <c r="O600" s="10">
+        <v>1</v>
+      </c>
+      <c r="P600" s="10">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q600" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R600" s="10">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S600" s="10">
+        <f t="shared" si="31"/>
+        <v>18.5</v>
+      </c>
+      <c r="T600" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="601" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A601" s="25">
+        <v>45673</v>
+      </c>
+      <c r="B601" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C601" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D601" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E601" s="26">
+        <v>0</v>
+      </c>
+      <c r="F601" s="26"/>
+      <c r="G601" s="26"/>
+      <c r="H601" s="26"/>
+      <c r="I601" s="26">
+        <v>0</v>
+      </c>
+      <c r="J601" s="27">
+        <v>0</v>
+      </c>
+      <c r="K601" s="26">
+        <v>111</v>
+      </c>
+      <c r="L601" s="26">
+        <v>100</v>
+      </c>
+      <c r="M601" s="26">
+        <f t="shared" si="33"/>
+        <v>211</v>
+      </c>
+      <c r="N601" s="26">
+        <f t="shared" si="34"/>
+        <v>11</v>
+      </c>
+      <c r="O601" s="26"/>
+      <c r="P601" s="26">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q601" s="26">
+        <f t="shared" si="29"/>
+        <v>211</v>
+      </c>
+      <c r="R601" s="26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S601" s="26" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T601" s="26">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="602" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A602" s="29">
+        <v>45673</v>
+      </c>
+      <c r="B602" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C602" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D602" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E602" s="30">
+        <v>0</v>
+      </c>
+      <c r="F602" s="30"/>
+      <c r="G602" s="30"/>
+      <c r="H602" s="30"/>
+      <c r="I602" s="30">
+        <v>233</v>
+      </c>
+      <c r="J602" s="31">
+        <v>11.5</v>
+      </c>
+      <c r="K602" s="30">
+        <v>130</v>
+      </c>
+      <c r="L602" s="30">
+        <v>123</v>
+      </c>
+      <c r="M602" s="30">
+        <f t="shared" si="33"/>
+        <v>253</v>
+      </c>
+      <c r="N602" s="30">
+        <f t="shared" si="34"/>
+        <v>7</v>
+      </c>
+      <c r="O602" s="30">
+        <v>1</v>
+      </c>
+      <c r="P602" s="30">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q602" s="30">
+        <f t="shared" si="29"/>
+        <v>20</v>
+      </c>
+      <c r="R602" s="30">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S602" s="30" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T602" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="603" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A603" s="29">
+        <v>45673</v>
+      </c>
+      <c r="B603" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C603" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D603" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E603" s="30">
+        <v>0</v>
+      </c>
+      <c r="F603" s="30"/>
+      <c r="G603" s="30"/>
+      <c r="H603" s="30"/>
+      <c r="I603" s="30">
+        <v>232.5</v>
+      </c>
+      <c r="J603" s="31">
+        <v>-2.5</v>
+      </c>
+      <c r="K603" s="30">
+        <v>114</v>
+      </c>
+      <c r="L603" s="30">
+        <v>134</v>
+      </c>
+      <c r="M603" s="30">
+        <f t="shared" si="33"/>
+        <v>248</v>
+      </c>
+      <c r="N603" s="30">
+        <f t="shared" si="34"/>
+        <v>-20</v>
+      </c>
+      <c r="O603" s="30">
+        <v>1</v>
+      </c>
+      <c r="P603" s="30">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q603" s="30">
+        <f t="shared" si="29"/>
+        <v>15.5</v>
+      </c>
+      <c r="R603" s="30">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S603" s="30" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T603" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="604" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A604" s="29">
+        <v>45673</v>
+      </c>
+      <c r="B604" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C604" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D604" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E604" s="30">
+        <v>0</v>
+      </c>
+      <c r="F604" s="30"/>
+      <c r="G604" s="30"/>
+      <c r="H604" s="30"/>
+      <c r="I604" s="30">
+        <v>227</v>
+      </c>
+      <c r="J604" s="31">
+        <v>-2.5</v>
+      </c>
+      <c r="K604" s="30">
+        <v>118</v>
+      </c>
+      <c r="L604" s="30">
+        <v>89</v>
+      </c>
+      <c r="M604" s="30">
+        <f t="shared" si="33"/>
+        <v>207</v>
+      </c>
+      <c r="N604" s="30">
+        <f t="shared" si="34"/>
+        <v>29</v>
+      </c>
+      <c r="O604" s="30">
+        <v>1</v>
+      </c>
+      <c r="P604" s="30">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q604" s="30" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R604" s="30">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S604" s="30">
+        <f t="shared" si="31"/>
+        <v>20</v>
+      </c>
+      <c r="T604" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="605" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A605" s="29">
+        <v>45673</v>
+      </c>
+      <c r="B605" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C605" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D605" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E605" s="30">
+        <v>0</v>
+      </c>
+      <c r="F605" s="30"/>
+      <c r="G605" s="30"/>
+      <c r="H605" s="30"/>
+      <c r="I605" s="30">
+        <v>227.5</v>
+      </c>
+      <c r="J605" s="31">
+        <v>-2.5</v>
+      </c>
+      <c r="K605" s="30">
+        <v>127</v>
+      </c>
+      <c r="L605" s="30">
+        <v>132</v>
+      </c>
+      <c r="M605" s="30">
+        <f t="shared" si="33"/>
+        <v>259</v>
+      </c>
+      <c r="N605" s="30">
+        <f t="shared" si="34"/>
+        <v>-5</v>
+      </c>
+      <c r="O605" s="30">
+        <v>1</v>
+      </c>
+      <c r="P605" s="30">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q605" s="30">
+        <f t="shared" si="29"/>
+        <v>31.5</v>
+      </c>
+      <c r="R605" s="30">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S605" s="30" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T605" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="606" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A606" s="9">
+        <v>45674</v>
+      </c>
+      <c r="B606" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C606" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D606" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E606" s="10">
+        <v>0</v>
+      </c>
+      <c r="I606" s="10">
+        <v>210</v>
+      </c>
+      <c r="J606" s="11">
+        <v>-11.5</v>
+      </c>
+      <c r="K606" s="10">
+        <v>94</v>
+      </c>
+      <c r="L606" s="10">
+        <v>121</v>
+      </c>
+      <c r="M606" s="10">
+        <f t="shared" si="33"/>
+        <v>215</v>
+      </c>
+      <c r="N606" s="10">
+        <f t="shared" si="34"/>
+        <v>-27</v>
+      </c>
+      <c r="O606" s="10">
+        <v>1</v>
+      </c>
+      <c r="P606" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q606" s="10">
+        <f t="shared" si="29"/>
+        <v>5</v>
+      </c>
+      <c r="R606" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S606" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T606" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="607" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A607" s="9">
+        <v>45674</v>
+      </c>
+      <c r="B607" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C607" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D607" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E607" s="10">
+        <v>0</v>
+      </c>
+      <c r="I607" s="10">
+        <v>221</v>
+      </c>
+      <c r="J607" s="11">
+        <v>-3.5</v>
+      </c>
+      <c r="K607" s="10">
+        <v>116</v>
+      </c>
+      <c r="L607" s="10">
+        <v>99</v>
+      </c>
+      <c r="M607" s="10">
+        <f t="shared" si="33"/>
+        <v>215</v>
+      </c>
+      <c r="N607" s="10">
+        <f t="shared" si="34"/>
+        <v>17</v>
+      </c>
+      <c r="O607" s="10">
+        <v>1</v>
+      </c>
+      <c r="P607" s="10">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q607" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R607" s="10">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S607" s="10">
+        <f t="shared" si="31"/>
+        <v>6</v>
+      </c>
+      <c r="T607" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="608" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A608" s="9">
+        <v>45674</v>
+      </c>
+      <c r="B608" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C608" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D608" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E608" s="10">
+        <v>0</v>
+      </c>
+      <c r="I608" s="10">
+        <v>232.5</v>
+      </c>
+      <c r="J608" s="11">
+        <v>-11.5</v>
+      </c>
+      <c r="K608" s="10">
+        <v>112</v>
+      </c>
+      <c r="L608" s="10">
+        <v>130</v>
+      </c>
+      <c r="M608" s="10">
+        <f t="shared" si="33"/>
+        <v>242</v>
+      </c>
+      <c r="N608" s="10">
+        <f t="shared" si="34"/>
+        <v>-18</v>
+      </c>
+      <c r="O608" s="10">
+        <v>1</v>
+      </c>
+      <c r="P608" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q608" s="10">
+        <f t="shared" si="29"/>
+        <v>9.5</v>
+      </c>
+      <c r="R608" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S608" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T608" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="609" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A609" s="9">
+        <v>45674</v>
+      </c>
+      <c r="B609" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C609" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D609" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E609" s="10">
+        <v>0</v>
+      </c>
+      <c r="I609" s="10">
+        <v>228.5</v>
+      </c>
+      <c r="J609" s="11">
+        <v>-8.5</v>
+      </c>
+      <c r="K609" s="10">
+        <v>123</v>
+      </c>
+      <c r="L609" s="10">
+        <v>136</v>
+      </c>
+      <c r="M609" s="10">
+        <f t="shared" si="33"/>
+        <v>259</v>
+      </c>
+      <c r="N609" s="10">
+        <f t="shared" si="34"/>
+        <v>-13</v>
+      </c>
+      <c r="O609" s="10">
+        <v>1</v>
+      </c>
+      <c r="P609" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q609" s="10">
+        <f t="shared" si="29"/>
+        <v>30.5</v>
+      </c>
+      <c r="R609" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S609" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T609" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="610" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A610" s="9">
+        <v>45674</v>
+      </c>
+      <c r="B610" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C610" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D610" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E610" s="10">
+        <v>0</v>
+      </c>
+      <c r="I610" s="10">
+        <v>224.5</v>
+      </c>
+      <c r="J610" s="11">
+        <v>-3.5</v>
+      </c>
+      <c r="K610" s="10">
+        <v>133</v>
+      </c>
+      <c r="L610" s="10">
+        <v>113</v>
+      </c>
+      <c r="M610" s="10">
+        <f t="shared" si="33"/>
+        <v>246</v>
+      </c>
+      <c r="N610" s="10">
+        <f t="shared" si="34"/>
+        <v>20</v>
+      </c>
+      <c r="O610" s="10">
+        <v>1</v>
+      </c>
+      <c r="P610" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q610" s="10">
+        <f t="shared" si="29"/>
+        <v>21.5</v>
+      </c>
+      <c r="R610" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S610" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T610" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="611" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A611" s="9">
+        <v>45674</v>
+      </c>
+      <c r="B611" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C611" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D611" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E611" s="10">
+        <v>0</v>
+      </c>
+      <c r="I611" s="10">
+        <v>235</v>
+      </c>
+      <c r="J611" s="11">
+        <v>-4.5</v>
+      </c>
+      <c r="K611" s="10">
+        <v>125</v>
+      </c>
+      <c r="L611" s="10">
+        <v>123</v>
+      </c>
+      <c r="M611" s="10">
+        <f t="shared" si="33"/>
+        <v>248</v>
+      </c>
+      <c r="N611" s="10">
+        <f t="shared" si="34"/>
+        <v>2</v>
+      </c>
+      <c r="O611" s="10">
+        <v>1</v>
+      </c>
+      <c r="P611" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q611" s="10">
+        <f t="shared" si="29"/>
+        <v>13</v>
+      </c>
+      <c r="R611" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S611" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T611" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="612" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A612" s="9">
+        <v>45674</v>
+      </c>
+      <c r="B612" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C612" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D612" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E612" s="10">
+        <v>0</v>
+      </c>
+      <c r="I612" s="10">
+        <v>221</v>
+      </c>
+      <c r="J612" s="11">
+        <v>6</v>
+      </c>
+      <c r="K612" s="10">
+        <v>98</v>
+      </c>
+      <c r="L612" s="10">
+        <v>106</v>
+      </c>
+      <c r="M612" s="10">
+        <f t="shared" si="33"/>
+        <v>204</v>
+      </c>
+      <c r="N612" s="10">
+        <f t="shared" si="34"/>
+        <v>-8</v>
+      </c>
+      <c r="O612" s="10">
+        <v>1</v>
+      </c>
+      <c r="P612" s="10">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q612" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R612" s="10">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S612" s="10">
+        <f t="shared" si="31"/>
+        <v>17</v>
+      </c>
+      <c r="T612" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="613" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A613" s="9">
+        <v>45674</v>
+      </c>
+      <c r="B613" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C613" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D613" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E613" s="10">
+        <v>0</v>
+      </c>
+      <c r="I613" s="10">
+        <v>239.5</v>
+      </c>
+      <c r="J613" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="K613" s="10">
+        <v>140</v>
+      </c>
+      <c r="L613" s="10">
+        <v>112</v>
+      </c>
+      <c r="M613" s="10">
+        <f t="shared" si="33"/>
+        <v>252</v>
+      </c>
+      <c r="N613" s="10">
+        <f t="shared" si="34"/>
+        <v>28</v>
+      </c>
+      <c r="O613" s="10">
+        <v>1</v>
+      </c>
+      <c r="P613" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q613" s="10">
+        <f t="shared" si="29"/>
+        <v>12.5</v>
+      </c>
+      <c r="R613" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S613" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T613" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="614" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A614" s="9">
+        <v>45674</v>
+      </c>
+      <c r="B614" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C614" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D614" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E614" s="10">
+        <v>0</v>
+      </c>
+      <c r="I614" s="10">
+        <v>219.5</v>
+      </c>
+      <c r="J614" s="11">
+        <v>-11.5</v>
+      </c>
+      <c r="K614" s="10">
+        <v>101</v>
+      </c>
+      <c r="L614" s="10">
+        <v>102</v>
+      </c>
+      <c r="M614" s="10">
+        <f t="shared" si="33"/>
+        <v>203</v>
+      </c>
+      <c r="N614" s="10">
+        <f t="shared" si="34"/>
+        <v>-1</v>
+      </c>
+      <c r="O614" s="10">
+        <v>1</v>
+      </c>
+      <c r="P614" s="10">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q614" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R614" s="10">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S614" s="10">
+        <f t="shared" si="31"/>
+        <v>16.5</v>
+      </c>
+      <c r="T614" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="615" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A615" s="29">
+        <v>45675</v>
+      </c>
+      <c r="B615" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C615" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D615" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E615" s="30">
+        <v>0</v>
+      </c>
+      <c r="F615" s="30"/>
+      <c r="G615" s="30"/>
+      <c r="H615" s="30"/>
+      <c r="I615" s="30">
+        <v>227.5</v>
+      </c>
+      <c r="J615" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="K615" s="30">
+        <v>125</v>
+      </c>
+      <c r="L615" s="30">
+        <v>121</v>
+      </c>
+      <c r="M615" s="30">
+        <f t="shared" si="33"/>
+        <v>246</v>
+      </c>
+      <c r="N615" s="30">
+        <f t="shared" si="34"/>
+        <v>4</v>
+      </c>
+      <c r="O615" s="30">
+        <v>1</v>
+      </c>
+      <c r="P615" s="30">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q615" s="30">
+        <f t="shared" si="29"/>
+        <v>18.5</v>
+      </c>
+      <c r="R615" s="30">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S615" s="30" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T615" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="616" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A616" s="29">
+        <v>45675</v>
+      </c>
+      <c r="B616" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C616" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D616" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E616" s="30">
+        <v>0</v>
+      </c>
+      <c r="F616" s="30"/>
+      <c r="G616" s="30"/>
+      <c r="H616" s="30"/>
+      <c r="I616" s="30">
+        <v>223.5</v>
+      </c>
+      <c r="J616" s="31">
+        <v>-7.5</v>
+      </c>
+      <c r="K616" s="30">
+        <v>102</v>
+      </c>
+      <c r="L616" s="30">
+        <v>115</v>
+      </c>
+      <c r="M616" s="30">
+        <f t="shared" si="33"/>
+        <v>217</v>
+      </c>
+      <c r="N616" s="30">
+        <f t="shared" si="34"/>
+        <v>-13</v>
+      </c>
+      <c r="O616" s="30">
+        <v>1</v>
+      </c>
+      <c r="P616" s="30">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q616" s="30" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R616" s="30">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S616" s="30">
+        <f t="shared" si="31"/>
+        <v>6.5</v>
+      </c>
+      <c r="T616" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="617" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A617" s="29">
+        <v>45675</v>
+      </c>
+      <c r="B617" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C617" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D617" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E617" s="30">
+        <v>0</v>
+      </c>
+      <c r="F617" s="30"/>
+      <c r="G617" s="30"/>
+      <c r="H617" s="30"/>
+      <c r="I617" s="30">
+        <v>234.5</v>
+      </c>
+      <c r="J617" s="31">
+        <v>-11.5</v>
+      </c>
+      <c r="K617" s="30">
+        <v>119</v>
+      </c>
+      <c r="L617" s="30">
+        <v>115</v>
+      </c>
+      <c r="M617" s="30">
+        <f t="shared" si="33"/>
+        <v>234</v>
+      </c>
+      <c r="N617" s="30">
+        <f t="shared" si="34"/>
+        <v>4</v>
+      </c>
+      <c r="O617" s="30">
+        <v>1</v>
+      </c>
+      <c r="P617" s="30">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q617" s="30" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R617" s="30">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S617" s="30">
+        <f t="shared" si="31"/>
+        <v>0.5</v>
+      </c>
+      <c r="T617" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="618" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A618" s="29">
+        <v>45675</v>
+      </c>
+      <c r="B618" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C618" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D618" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E618" s="30">
+        <v>0</v>
+      </c>
+      <c r="F618" s="30"/>
+      <c r="G618" s="30"/>
+      <c r="H618" s="30"/>
+      <c r="I618" s="30">
+        <v>230.5</v>
+      </c>
+      <c r="J618" s="31">
+        <v>-14.5</v>
+      </c>
+      <c r="K618" s="30">
+        <v>114</v>
+      </c>
+      <c r="L618" s="30">
+        <v>122</v>
+      </c>
+      <c r="M618" s="30">
+        <f t="shared" si="33"/>
+        <v>236</v>
+      </c>
+      <c r="N618" s="30">
+        <f t="shared" si="34"/>
+        <v>-8</v>
+      </c>
+      <c r="O618" s="30">
+        <v>1</v>
+      </c>
+      <c r="P618" s="30">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q618" s="30">
+        <f t="shared" si="29"/>
+        <v>5.5</v>
+      </c>
+      <c r="R618" s="30">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S618" s="30" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T618" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="619" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A619" s="29">
+        <v>45675</v>
+      </c>
+      <c r="B619" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C619" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D619" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E619" s="30">
+        <v>0</v>
+      </c>
+      <c r="F619" s="30"/>
+      <c r="G619" s="30"/>
+      <c r="H619" s="30"/>
+      <c r="I619" s="30">
+        <v>227.5</v>
+      </c>
+      <c r="J619" s="31">
+        <v>5</v>
+      </c>
+      <c r="K619" s="30">
+        <v>124</v>
+      </c>
+      <c r="L619" s="30">
+        <v>117</v>
+      </c>
+      <c r="M619" s="30">
+        <f t="shared" si="33"/>
+        <v>241</v>
+      </c>
+      <c r="N619" s="30">
+        <f t="shared" si="34"/>
+        <v>7</v>
+      </c>
+      <c r="O619" s="30">
+        <v>1</v>
+      </c>
+      <c r="P619" s="30">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q619" s="30">
+        <f t="shared" si="29"/>
+        <v>13.5</v>
+      </c>
+      <c r="R619" s="30">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S619" s="30" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T619" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="620" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A620" s="29">
+        <v>45675</v>
+      </c>
+      <c r="B620" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C620" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D620" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E620" s="30">
+        <v>0</v>
+      </c>
+      <c r="F620" s="30"/>
+      <c r="G620" s="30"/>
+      <c r="H620" s="30"/>
+      <c r="I620" s="30">
+        <v>223</v>
+      </c>
+      <c r="J620" s="31">
+        <v>9.5</v>
+      </c>
+      <c r="K620" s="30">
+        <v>125</v>
+      </c>
+      <c r="L620" s="30">
+        <v>103</v>
+      </c>
+      <c r="M620" s="30">
+        <f t="shared" si="33"/>
+        <v>228</v>
+      </c>
+      <c r="N620" s="30">
+        <f t="shared" si="34"/>
+        <v>22</v>
+      </c>
+      <c r="O620" s="30">
+        <v>1</v>
+      </c>
+      <c r="P620" s="30">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q620" s="30">
+        <f t="shared" si="29"/>
+        <v>5</v>
+      </c>
+      <c r="R620" s="30">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S620" s="30" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T620" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="621" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A621" s="9">
+        <v>45676</v>
+      </c>
+      <c r="B621" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C621" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D621" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E621" s="10">
+        <v>0</v>
+      </c>
+      <c r="I621" s="10">
+        <v>219</v>
+      </c>
+      <c r="J621" s="11">
+        <v>-2.5</v>
+      </c>
+      <c r="K621" s="10">
+        <v>107</v>
+      </c>
+      <c r="L621" s="10">
+        <v>128</v>
+      </c>
+      <c r="M621" s="10">
+        <f t="shared" si="33"/>
+        <v>235</v>
+      </c>
+      <c r="N621" s="10">
+        <f t="shared" si="34"/>
+        <v>-21</v>
+      </c>
+      <c r="O621" s="10">
+        <v>1</v>
+      </c>
+      <c r="P621" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q621" s="10">
+        <f t="shared" si="29"/>
+        <v>16</v>
+      </c>
+      <c r="R621" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S621" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T621" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="622" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A622" s="9">
+        <v>45676</v>
+      </c>
+      <c r="B622" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C622" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D622" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E622" s="10">
+        <v>0</v>
+      </c>
+      <c r="I622" s="10">
+        <v>221.5</v>
+      </c>
+      <c r="J622" s="11">
+        <v>3</v>
+      </c>
+      <c r="K622" s="10">
+        <v>113</v>
+      </c>
+      <c r="L622" s="10">
+        <v>100</v>
+      </c>
+      <c r="M622" s="10">
+        <f t="shared" si="33"/>
+        <v>213</v>
+      </c>
+      <c r="N622" s="10">
+        <f t="shared" si="34"/>
+        <v>13</v>
+      </c>
+      <c r="O622" s="10">
+        <v>1</v>
+      </c>
+      <c r="P622" s="10">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q622" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R622" s="10">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S622" s="10">
+        <f t="shared" si="31"/>
+        <v>8.5</v>
+      </c>
+      <c r="T622" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="623" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A623" s="9">
+        <v>45676</v>
+      </c>
+      <c r="B623" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C623" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D623" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E623" s="10">
+        <v>0</v>
+      </c>
+      <c r="I623" s="10">
+        <v>221</v>
+      </c>
+      <c r="J623" s="11">
+        <v>-9.5</v>
+      </c>
+      <c r="K623" s="10">
+        <v>109</v>
+      </c>
+      <c r="L623" s="10">
+        <v>123</v>
+      </c>
+      <c r="M623" s="10">
+        <f t="shared" si="33"/>
+        <v>232</v>
+      </c>
+      <c r="N623" s="10">
+        <f t="shared" si="34"/>
+        <v>-14</v>
+      </c>
+      <c r="O623" s="10">
+        <v>1</v>
+      </c>
+      <c r="P623" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q623" s="10">
+        <f t="shared" si="29"/>
+        <v>11</v>
+      </c>
+      <c r="R623" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S623" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T623" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="624" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A624" s="9">
+        <v>45676</v>
+      </c>
+      <c r="B624" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C624" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D624" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E624" s="10">
+        <v>0</v>
+      </c>
+      <c r="I624" s="10">
+        <v>212.5</v>
+      </c>
+      <c r="J624" s="11">
+        <v>-13.5</v>
+      </c>
+      <c r="K624" s="10">
+        <v>101</v>
+      </c>
+      <c r="L624" s="10">
+        <v>127</v>
+      </c>
+      <c r="M624" s="10">
+        <f t="shared" si="33"/>
+        <v>228</v>
+      </c>
+      <c r="N624" s="10">
+        <f t="shared" si="34"/>
+        <v>-26</v>
+      </c>
+      <c r="O624" s="10">
+        <v>1</v>
+      </c>
+      <c r="P624" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q624" s="10">
+        <f t="shared" si="29"/>
+        <v>15.5</v>
+      </c>
+      <c r="R624" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S624" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T624" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="625" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A625" s="9">
+        <v>45676</v>
+      </c>
+      <c r="B625" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C625" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D625" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E625" s="10">
+        <v>0</v>
+      </c>
+      <c r="I625" s="10">
+        <v>234.5</v>
+      </c>
+      <c r="J625" s="11">
+        <v>-16.5</v>
+      </c>
+      <c r="K625" s="10">
+        <v>100</v>
+      </c>
+      <c r="L625" s="10">
+        <v>123</v>
+      </c>
+      <c r="M625" s="10">
+        <f t="shared" si="33"/>
+        <v>223</v>
+      </c>
+      <c r="N625" s="10">
+        <f t="shared" si="34"/>
+        <v>-23</v>
+      </c>
+      <c r="O625" s="10">
+        <v>1</v>
+      </c>
+      <c r="P625" s="10">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q625" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R625" s="10">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S625" s="10">
+        <f t="shared" si="31"/>
+        <v>11.5</v>
+      </c>
+      <c r="T625" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="626" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A626" s="9">
+        <v>45676</v>
+      </c>
+      <c r="B626" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C626" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D626" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E626" s="10">
+        <v>0</v>
+      </c>
+      <c r="I626" s="10">
+        <v>232.5</v>
+      </c>
+      <c r="J626" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="K626" s="10">
+        <v>102</v>
+      </c>
+      <c r="L626" s="10">
+        <v>113</v>
+      </c>
+      <c r="M626" s="10">
+        <f t="shared" si="33"/>
+        <v>215</v>
+      </c>
+      <c r="N626" s="10">
+        <f t="shared" si="34"/>
+        <v>-11</v>
+      </c>
+      <c r="O626" s="10">
+        <v>1</v>
+      </c>
+      <c r="P626" s="10">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q626" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R626" s="10">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S626" s="10">
+        <f t="shared" si="31"/>
+        <v>17.5</v>
+      </c>
+      <c r="T626" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="627" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A627" s="9">
+        <v>45676</v>
+      </c>
+      <c r="B627" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C627" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D627" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E627" s="10">
+        <v>0</v>
+      </c>
+      <c r="I627" s="10">
+        <v>218.5</v>
+      </c>
+      <c r="J627" s="11">
+        <v>-4.5</v>
+      </c>
+      <c r="K627" s="10">
+        <v>102</v>
+      </c>
+      <c r="L627" s="10">
+        <v>116</v>
+      </c>
+      <c r="M627" s="10">
+        <f t="shared" si="33"/>
+        <v>218</v>
+      </c>
+      <c r="N627" s="10">
+        <f t="shared" si="34"/>
+        <v>-14</v>
+      </c>
+      <c r="O627" s="10">
+        <v>1</v>
+      </c>
+      <c r="P627" s="10">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q627" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R627" s="10">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S627" s="10">
+        <f t="shared" si="31"/>
+        <v>0.5</v>
+      </c>
+      <c r="T627" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="628" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A628" s="29">
+        <v>45677</v>
+      </c>
+      <c r="B628" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C628" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D628" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E628" s="30">
+        <v>0</v>
+      </c>
+      <c r="F628" s="30"/>
+      <c r="G628" s="30"/>
+      <c r="H628" s="30"/>
+      <c r="I628" s="30">
+        <v>232.5</v>
+      </c>
+      <c r="J628" s="31">
+        <v>7</v>
+      </c>
+      <c r="K628" s="30">
+        <v>105</v>
+      </c>
+      <c r="L628" s="30">
+        <v>110</v>
+      </c>
+      <c r="M628" s="30">
+        <f t="shared" si="33"/>
+        <v>215</v>
+      </c>
+      <c r="N628" s="30">
+        <f t="shared" si="34"/>
+        <v>-5</v>
+      </c>
+      <c r="O628" s="30">
+        <v>1</v>
+      </c>
+      <c r="P628" s="30">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q628" s="30" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R628" s="30">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S628" s="30">
+        <f t="shared" si="31"/>
+        <v>17.5</v>
+      </c>
+      <c r="T628" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="629" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A629" s="29">
+        <v>45677</v>
+      </c>
+      <c r="B629" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C629" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D629" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E629" s="30">
+        <v>0</v>
+      </c>
+      <c r="F629" s="30"/>
+      <c r="G629" s="30"/>
+      <c r="H629" s="30"/>
+      <c r="I629" s="30">
+        <v>228.5</v>
+      </c>
+      <c r="J629" s="31">
+        <v>-7</v>
+      </c>
+      <c r="K629" s="30">
+        <v>107</v>
+      </c>
+      <c r="L629" s="30">
+        <v>96</v>
+      </c>
+      <c r="M629" s="30">
+        <f t="shared" si="33"/>
+        <v>203</v>
+      </c>
+      <c r="N629" s="30">
+        <f t="shared" si="34"/>
+        <v>11</v>
+      </c>
+      <c r="O629" s="30">
+        <v>1</v>
+      </c>
+      <c r="P629" s="30">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q629" s="30" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R629" s="30">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S629" s="30">
+        <f t="shared" si="31"/>
+        <v>25.5</v>
+      </c>
+      <c r="T629" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="630" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A630" s="29">
+        <v>45677</v>
+      </c>
+      <c r="B630" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C630" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D630" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E630" s="30">
+        <v>0</v>
+      </c>
+      <c r="F630" s="30"/>
+      <c r="G630" s="30"/>
+      <c r="H630" s="30"/>
+      <c r="I630" s="30">
+        <v>218.5</v>
+      </c>
+      <c r="J630" s="31">
+        <v>-1</v>
+      </c>
+      <c r="K630" s="30">
+        <v>106</v>
+      </c>
+      <c r="L630" s="30">
+        <v>108</v>
+      </c>
+      <c r="M630" s="30">
+        <f t="shared" si="33"/>
+        <v>214</v>
+      </c>
+      <c r="N630" s="30">
+        <f t="shared" si="34"/>
+        <v>-2</v>
+      </c>
+      <c r="O630" s="30">
+        <v>1</v>
+      </c>
+      <c r="P630" s="30">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q630" s="30" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R630" s="30">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S630" s="30">
+        <f t="shared" si="31"/>
+        <v>4.5</v>
+      </c>
+      <c r="T630" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="631" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A631" s="29">
+        <v>45677</v>
+      </c>
+      <c r="B631" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C631" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D631" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E631" s="30">
+        <v>0</v>
+      </c>
+      <c r="F631" s="30"/>
+      <c r="G631" s="30"/>
+      <c r="H631" s="30"/>
+      <c r="I631" s="30">
+        <v>222</v>
+      </c>
+      <c r="J631" s="31">
+        <v>-9</v>
+      </c>
+      <c r="K631" s="30">
+        <v>110</v>
+      </c>
+      <c r="L631" s="30">
+        <v>119</v>
+      </c>
+      <c r="M631" s="30">
+        <f t="shared" si="33"/>
+        <v>229</v>
+      </c>
+      <c r="N631" s="30">
+        <f t="shared" si="34"/>
+        <v>-9</v>
+      </c>
+      <c r="O631" s="30">
+        <v>1</v>
+      </c>
+      <c r="P631" s="30">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q631" s="30">
+        <f t="shared" si="29"/>
+        <v>7</v>
+      </c>
+      <c r="R631" s="30">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S631" s="30" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T631" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="632" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A632" s="29">
+        <v>45677</v>
+      </c>
+      <c r="B632" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C632" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D632" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E632" s="30">
+        <v>0</v>
+      </c>
+      <c r="F632" s="30"/>
+      <c r="G632" s="30"/>
+      <c r="H632" s="30"/>
+      <c r="I632" s="30">
+        <v>223.5</v>
+      </c>
+      <c r="J632" s="31">
+        <v>-2.5</v>
+      </c>
+      <c r="K632" s="30">
+        <v>92</v>
+      </c>
+      <c r="L632" s="30">
+        <v>118</v>
+      </c>
+      <c r="M632" s="30">
+        <f t="shared" si="33"/>
+        <v>210</v>
+      </c>
+      <c r="N632" s="30">
+        <f t="shared" si="34"/>
+        <v>-26</v>
+      </c>
+      <c r="O632" s="30">
+        <v>1</v>
+      </c>
+      <c r="P632" s="30">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q632" s="30" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R632" s="30">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S632" s="30">
+        <f t="shared" si="31"/>
+        <v>13.5</v>
+      </c>
+      <c r="T632" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="633" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A633" s="29">
+        <v>45677</v>
+      </c>
+      <c r="B633" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C633" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D633" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E633" s="30">
+        <v>0</v>
+      </c>
+      <c r="F633" s="30"/>
+      <c r="G633" s="30"/>
+      <c r="H633" s="30"/>
+      <c r="I633" s="30">
+        <v>223.5</v>
+      </c>
+      <c r="J633" s="31">
+        <v>5</v>
+      </c>
+      <c r="K633" s="30">
+        <v>125</v>
+      </c>
+      <c r="L633" s="30">
+        <v>85</v>
+      </c>
+      <c r="M633" s="30">
+        <f t="shared" si="33"/>
+        <v>210</v>
+      </c>
+      <c r="N633" s="30">
+        <f t="shared" si="34"/>
+        <v>40</v>
+      </c>
+      <c r="O633" s="30">
+        <v>1</v>
+      </c>
+      <c r="P633" s="30">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q633" s="30" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R633" s="30">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S633" s="30">
+        <f t="shared" si="31"/>
+        <v>13.5</v>
+      </c>
+      <c r="T633" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="634" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A634" s="29">
+        <v>45677</v>
+      </c>
+      <c r="B634" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C634" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D634" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E634" s="30">
+        <v>0</v>
+      </c>
+      <c r="F634" s="30"/>
+      <c r="G634" s="30"/>
+      <c r="H634" s="30"/>
+      <c r="I634" s="30">
+        <v>226.5</v>
+      </c>
+      <c r="J634" s="31">
+        <v>-7.5</v>
+      </c>
+      <c r="K634" s="30">
+        <v>119</v>
+      </c>
+      <c r="L634" s="30">
+        <v>123</v>
+      </c>
+      <c r="M634" s="30">
+        <f t="shared" si="33"/>
+        <v>242</v>
+      </c>
+      <c r="N634" s="30">
+        <f t="shared" si="34"/>
+        <v>-4</v>
+      </c>
+      <c r="O634" s="30">
+        <v>1</v>
+      </c>
+      <c r="P634" s="30">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q634" s="30">
+        <f t="shared" si="29"/>
+        <v>15.5</v>
+      </c>
+      <c r="R634" s="30">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S634" s="30" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T634" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="635" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A635" s="29">
+        <v>45677</v>
+      </c>
+      <c r="B635" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C635" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D635" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E635" s="30">
+        <v>0</v>
+      </c>
+      <c r="F635" s="30"/>
+      <c r="G635" s="30"/>
+      <c r="H635" s="30"/>
+      <c r="I635" s="30">
+        <v>233.5</v>
+      </c>
+      <c r="J635" s="31">
+        <v>-6.5</v>
+      </c>
+      <c r="K635" s="30">
+        <v>112</v>
+      </c>
+      <c r="L635" s="30">
+        <v>99</v>
+      </c>
+      <c r="M635" s="30">
+        <f t="shared" si="33"/>
+        <v>211</v>
+      </c>
+      <c r="N635" s="30">
+        <f t="shared" si="34"/>
+        <v>13</v>
+      </c>
+      <c r="O635" s="30">
+        <v>1</v>
+      </c>
+      <c r="P635" s="30">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q635" s="30" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R635" s="30">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S635" s="30">
+        <f t="shared" si="31"/>
+        <v>22.5</v>
+      </c>
+      <c r="T635" s="30">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="636" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A636" s="9">
+        <v>45678</v>
+      </c>
+      <c r="B636" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C636" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D636" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E636" s="10">
+        <v>0</v>
+      </c>
+      <c r="I636" s="10">
+        <v>219.5</v>
+      </c>
+      <c r="J636" s="11">
+        <v>-11.5</v>
+      </c>
+      <c r="K636" s="10">
+        <v>116</v>
+      </c>
+      <c r="L636" s="10">
+        <v>107</v>
+      </c>
+      <c r="M636" s="10">
+        <f t="shared" si="33"/>
+        <v>223</v>
+      </c>
+      <c r="N636" s="10">
+        <f t="shared" si="34"/>
+        <v>9</v>
+      </c>
+      <c r="O636" s="10">
+        <v>1</v>
+      </c>
+      <c r="P636" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q636" s="10">
+        <f t="shared" si="29"/>
+        <v>3.5</v>
+      </c>
+      <c r="R636" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S636" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T636" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="637" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A637" s="9">
+        <v>45678</v>
+      </c>
+      <c r="B637" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C637" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D637" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E637" s="10">
+        <v>0</v>
+      </c>
+      <c r="I637" s="10">
+        <v>215.5</v>
+      </c>
+      <c r="J637" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="K637" s="10">
+        <v>93</v>
+      </c>
+      <c r="L637" s="10">
+        <v>109</v>
+      </c>
+      <c r="M637" s="10">
+        <f t="shared" si="33"/>
+        <v>202</v>
+      </c>
+      <c r="N637" s="10">
+        <f t="shared" si="34"/>
+        <v>-16</v>
+      </c>
+      <c r="O637" s="10">
+        <v>1</v>
+      </c>
+      <c r="P637" s="10">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q637" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R637" s="10">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S637" s="10">
+        <f t="shared" si="31"/>
+        <v>13.5</v>
+      </c>
+      <c r="T637" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="638" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A638" s="9">
+        <v>45678</v>
+      </c>
+      <c r="B638" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C638" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D638" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E638" s="10">
+        <v>0</v>
+      </c>
+      <c r="I638" s="10">
+        <v>222.5</v>
+      </c>
+      <c r="J638" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="K638" s="10">
+        <v>99</v>
+      </c>
+      <c r="L638" s="10">
+        <v>95</v>
+      </c>
+      <c r="M638" s="10">
+        <f t="shared" si="33"/>
+        <v>194</v>
+      </c>
+      <c r="N638" s="10">
+        <f t="shared" si="34"/>
+        <v>4</v>
+      </c>
+      <c r="O638" s="10">
+        <v>1</v>
+      </c>
+      <c r="P638" s="10">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q638" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R638" s="10">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S638" s="10">
+        <f t="shared" si="31"/>
+        <v>28.5</v>
+      </c>
+      <c r="T638" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="639" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A639" s="9">
+        <v>45678</v>
+      </c>
+      <c r="B639" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C639" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D639" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E639" s="10">
+        <v>0</v>
+      </c>
+      <c r="I639" s="10">
+        <v>229.5</v>
+      </c>
+      <c r="J639" s="11">
+        <v>-10.5</v>
+      </c>
+      <c r="K639" s="10">
+        <v>109</v>
+      </c>
+      <c r="L639" s="10">
+        <v>144</v>
+      </c>
+      <c r="M639" s="10">
+        <f t="shared" si="33"/>
+        <v>253</v>
+      </c>
+      <c r="N639" s="10">
+        <f t="shared" si="34"/>
+        <v>-35</v>
+      </c>
+      <c r="O639" s="10">
+        <v>1</v>
+      </c>
+      <c r="P639" s="10">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q639" s="10">
+        <f t="shared" si="29"/>
+        <v>23.5</v>
+      </c>
+      <c r="R639" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S639" s="10" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="T639" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="640" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A640" s="9">
+        <v>45678</v>
+      </c>
+      <c r="B640" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C640" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D640" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E640" s="10">
+        <v>0</v>
+      </c>
+      <c r="I640" s="10">
+        <v>231</v>
+      </c>
+      <c r="J640" s="11">
+        <v>-14.5</v>
+      </c>
+      <c r="K640" s="10">
+        <v>88</v>
+      </c>
+      <c r="L640" s="10">
+        <v>111</v>
+      </c>
+      <c r="M640" s="10">
+        <f t="shared" si="33"/>
+        <v>199</v>
+      </c>
+      <c r="N640" s="10">
+        <f t="shared" si="34"/>
+        <v>-23</v>
+      </c>
+      <c r="O640" s="10">
+        <v>1</v>
+      </c>
+      <c r="P640" s="10">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q640" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="R640" s="10">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="S640" s="10">
+        <f t="shared" si="31"/>
+        <v>32</v>
+      </c>
+      <c r="T640" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="641" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A641" s="29">
+        <v>45679</v>
+      </c>
+      <c r="B641" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C641" s="30"/>
+      <c r="D641" s="30"/>
+      <c r="E641" s="30">
+        <v>0</v>
+      </c>
+      <c r="F641" s="30"/>
+      <c r="G641" s="30"/>
+      <c r="H641" s="30"/>
+      <c r="I641" s="30"/>
+      <c r="J641" s="31"/>
+      <c r="K641" s="30"/>
+      <c r="L641" s="30"/>
+      <c r="M641" s="30"/>
+      <c r="N641" s="30"/>
+      <c r="O641" s="30"/>
+      <c r="P641" s="30"/>
+      <c r="Q641" s="30"/>
+      <c r="R641" s="30"/>
+      <c r="S641" s="30"/>
+      <c r="T641" s="30"/>
+    </row>
+    <row r="642" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A642" s="29">
+        <v>45679</v>
+      </c>
+      <c r="B642" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C642" s="30"/>
+      <c r="D642" s="30"/>
+      <c r="E642" s="30">
+        <v>0</v>
+      </c>
+      <c r="F642" s="30"/>
+      <c r="G642" s="30"/>
+      <c r="H642" s="30"/>
+      <c r="I642" s="30"/>
+      <c r="J642" s="31"/>
+      <c r="K642" s="30"/>
+      <c r="L642" s="30"/>
+      <c r="M642" s="30"/>
+      <c r="N642" s="30"/>
+      <c r="O642" s="30"/>
+      <c r="P642" s="30"/>
+      <c r="Q642" s="30"/>
+      <c r="R642" s="30"/>
+      <c r="S642" s="30"/>
+      <c r="T642" s="30"/>
+    </row>
+    <row r="643" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A643" s="29">
+        <v>45679</v>
+      </c>
+      <c r="B643" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C643" s="30"/>
+      <c r="D643" s="30"/>
+      <c r="E643" s="30">
+        <v>0</v>
+      </c>
+      <c r="F643" s="30"/>
+      <c r="G643" s="30"/>
+      <c r="H643" s="30"/>
+      <c r="I643" s="30"/>
+      <c r="J643" s="31"/>
+      <c r="K643" s="30"/>
+      <c r="L643" s="30"/>
+      <c r="M643" s="30"/>
+      <c r="N643" s="30"/>
+      <c r="O643" s="30"/>
+      <c r="P643" s="30"/>
+      <c r="Q643" s="30"/>
+      <c r="R643" s="30"/>
+      <c r="S643" s="30"/>
+      <c r="T643" s="30"/>
+    </row>
+    <row r="644" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A644" s="29">
+        <v>45679</v>
+      </c>
+      <c r="B644" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C644" s="30"/>
+      <c r="D644" s="30"/>
+      <c r="E644" s="30">
+        <v>0</v>
+      </c>
+      <c r="F644" s="30"/>
+      <c r="G644" s="30"/>
+      <c r="H644" s="30"/>
+      <c r="I644" s="30"/>
+      <c r="J644" s="31"/>
+      <c r="K644" s="30"/>
+      <c r="L644" s="30"/>
+      <c r="M644" s="30"/>
+      <c r="N644" s="30"/>
+      <c r="O644" s="30"/>
+      <c r="P644" s="30"/>
+      <c r="Q644" s="30"/>
+      <c r="R644" s="30"/>
+      <c r="S644" s="30"/>
+      <c r="T644" s="30"/>
+    </row>
+    <row r="645" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A645" s="29">
+        <v>45679</v>
+      </c>
+      <c r="B645" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C645" s="30"/>
+      <c r="D645" s="30"/>
+      <c r="E645" s="30">
+        <v>0</v>
+      </c>
+      <c r="F645" s="30"/>
+      <c r="G645" s="30"/>
+      <c r="H645" s="30"/>
+      <c r="I645" s="30"/>
+      <c r="J645" s="31"/>
+      <c r="K645" s="30"/>
+      <c r="L645" s="30"/>
+      <c r="M645" s="30"/>
+      <c r="N645" s="30"/>
+      <c r="O645" s="30"/>
+      <c r="P645" s="30"/>
+      <c r="Q645" s="30"/>
+      <c r="R645" s="30"/>
+      <c r="S645" s="30"/>
+      <c r="T645" s="30"/>
+    </row>
+    <row r="646" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A646" s="29">
+        <v>45679</v>
+      </c>
+      <c r="B646" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C646" s="30"/>
+      <c r="D646" s="30"/>
+      <c r="E646" s="30">
+        <v>0</v>
+      </c>
+      <c r="F646" s="30"/>
+      <c r="G646" s="30"/>
+      <c r="H646" s="30"/>
+      <c r="I646" s="30"/>
+      <c r="J646" s="31"/>
+      <c r="K646" s="30"/>
+      <c r="L646" s="30"/>
+      <c r="M646" s="30"/>
+      <c r="N646" s="30"/>
+      <c r="O646" s="30"/>
+      <c r="P646" s="30"/>
+      <c r="Q646" s="30"/>
+      <c r="R646" s="30"/>
+      <c r="S646" s="30"/>
+      <c r="T646" s="30"/>
+    </row>
+    <row r="647" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A647" s="29">
+        <v>45679</v>
+      </c>
+      <c r="B647" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C647" s="30"/>
+      <c r="D647" s="30"/>
+      <c r="E647" s="30">
+        <v>0</v>
+      </c>
+      <c r="F647" s="30"/>
+      <c r="G647" s="30"/>
+      <c r="H647" s="30"/>
+      <c r="I647" s="30"/>
+      <c r="J647" s="31"/>
+      <c r="K647" s="30"/>
+      <c r="L647" s="30"/>
+      <c r="M647" s="30"/>
+      <c r="N647" s="30"/>
+      <c r="O647" s="30"/>
+      <c r="P647" s="30"/>
+      <c r="Q647" s="30"/>
+      <c r="R647" s="30"/>
+      <c r="S647" s="30"/>
+      <c r="T647" s="30"/>
+    </row>
+    <row r="648" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A648" s="29">
+        <v>45679</v>
+      </c>
+      <c r="B648" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C648" s="30"/>
+      <c r="D648" s="30"/>
+      <c r="E648" s="30">
+        <v>0</v>
+      </c>
+      <c r="F648" s="30"/>
+      <c r="G648" s="30"/>
+      <c r="H648" s="30"/>
+      <c r="I648" s="30"/>
+      <c r="J648" s="31"/>
+      <c r="K648" s="30"/>
+      <c r="L648" s="30"/>
+      <c r="M648" s="30"/>
+      <c r="N648" s="30"/>
+      <c r="O648" s="30"/>
+      <c r="P648" s="30"/>
+      <c r="Q648" s="30"/>
+      <c r="R648" s="30"/>
+      <c r="S648" s="30"/>
+      <c r="T648" s="30"/>
+    </row>
+    <row r="649" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A649" s="29">
+        <v>45679</v>
+      </c>
+      <c r="B649" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C649" s="30"/>
+      <c r="D649" s="30"/>
+      <c r="E649" s="30">
+        <v>0</v>
+      </c>
+      <c r="F649" s="30"/>
+      <c r="G649" s="30"/>
+      <c r="H649" s="30"/>
+      <c r="I649" s="30"/>
+      <c r="J649" s="31"/>
+      <c r="K649" s="30"/>
+      <c r="L649" s="30"/>
+      <c r="M649" s="30"/>
+      <c r="N649" s="30"/>
+      <c r="O649" s="30"/>
+      <c r="P649" s="30"/>
+      <c r="Q649" s="30"/>
+      <c r="R649" s="30"/>
+      <c r="S649" s="30"/>
+      <c r="T649" s="30"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
added game data for february 12, 2025
</commit_message>
<xml_diff>
--- a/data/nba_points_2024_2025.xlsx
+++ b/data/nba_points_2024_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Documents/nba-points/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7660420B-C7EC-8D49-96BC-516D854D7AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45C25B0-C79A-074E-B98C-495143C01F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22940" yWindow="500" windowWidth="45860" windowHeight="28300" xr2:uid="{4B944735-6DC1-314A-AF10-68EBB82A81F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4810" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4900" uniqueCount="148">
   <si>
     <t>Date</t>
   </si>
@@ -1028,11 +1028,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78582E2E-5746-944D-860C-ACA920BD70CB}">
-  <dimension ref="A1:Y799"/>
+  <dimension ref="A1:Y814"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A757" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I802" sqref="I802"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V803" sqref="V803"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1207,15 +1207,15 @@
       </c>
       <c r="V2" s="7">
         <f>SUM(O:O)</f>
-        <v>791</v>
+        <v>806</v>
       </c>
       <c r="W2" s="12">
         <f>SUM(P:P)</f>
-        <v>420</v>
+        <v>428</v>
       </c>
       <c r="X2" s="15">
         <f>SUM(R:R)</f>
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="Y2" s="20">
         <f>SUM(T:T)</f>
@@ -1370,15 +1370,15 @@
       </c>
       <c r="W4" s="14">
         <f>W2/V2</f>
-        <v>0.53097345132743368</v>
+        <v>0.53101736972704716</v>
       </c>
       <c r="X4" s="16">
         <f>X2/V2</f>
-        <v>0.46902654867256638</v>
+        <v>0.46898263027295284</v>
       </c>
       <c r="Y4" s="21">
         <f>Y2/V2</f>
-        <v>3.7926675094816687E-3</v>
+        <v>3.7220843672456576E-3</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1526,11 +1526,11 @@
       </c>
       <c r="W6" s="22">
         <f>AVERAGE(Q:Q)</f>
-        <v>14.773809523809524</v>
+        <v>14.809579439252337</v>
       </c>
       <c r="X6" s="23">
         <f>AVERAGE(S:S)</f>
-        <v>15.024258760107816</v>
+        <v>15.002645502645503</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -41521,7 +41521,7 @@
         <v>113</v>
       </c>
       <c r="M587" s="7">
-        <f t="shared" ref="M587:M799" si="33">K587+L587</f>
+        <f t="shared" ref="M587:M814" si="33">K587+L587</f>
         <v>232</v>
       </c>
       <c r="N587" s="7">
@@ -46005,7 +46005,7 @@
         <v>1</v>
       </c>
       <c r="Q652" s="10">
-        <f t="shared" ref="Q652:Q799" si="35">IF(P652=1,(M652-I652), "")</f>
+        <f t="shared" ref="Q652:Q814" si="35">IF(P652=1,(M652-I652), "")</f>
         <v>4</v>
       </c>
       <c r="R652" s="10">
@@ -46063,14 +46063,14 @@
         <v>236</v>
       </c>
       <c r="N653" s="10">
-        <f t="shared" ref="N653:N799" si="36">(L653-K653)*-1</f>
+        <f t="shared" ref="N653:N814" si="36">(L653-K653)*-1</f>
         <v>6</v>
       </c>
       <c r="O653" s="10">
         <v>1</v>
       </c>
       <c r="P653" s="10">
-        <f t="shared" ref="P653:P799" si="37">IF(M653&gt;I653,1,0)</f>
+        <f t="shared" ref="P653:P814" si="37">IF(M653&gt;I653,1,0)</f>
         <v>1</v>
       </c>
       <c r="Q653" s="10">
@@ -46078,15 +46078,15 @@
         <v>17.5</v>
       </c>
       <c r="R653" s="10">
-        <f t="shared" ref="R653:R799" si="38">IF(M653&lt;I653, 1, 0)</f>
+        <f t="shared" ref="R653:R814" si="38">IF(M653&lt;I653, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="S653" s="10" t="str">
-        <f t="shared" ref="S653:S799" si="39">IF(R653=1,(I653-M653),"")</f>
+        <f t="shared" ref="S653:S814" si="39">IF(R653=1,(I653-M653),"")</f>
         <v/>
       </c>
       <c r="T653" s="10">
-        <f t="shared" ref="T653:T799" si="40">IF(M653=I653,1,0)</f>
+        <f t="shared" ref="T653:T814" si="40">IF(M653=I653,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -56152,6 +56152,1041 @@
         <v>10.5</v>
       </c>
       <c r="T799" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="800" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A800" s="9">
+        <v>45700</v>
+      </c>
+      <c r="B800" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C800" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D800" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E800" s="10">
+        <v>0</v>
+      </c>
+      <c r="F800" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G800" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H800" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I800" s="10">
+        <v>208</v>
+      </c>
+      <c r="J800" s="11">
+        <v>-10.5</v>
+      </c>
+      <c r="K800" s="10">
+        <v>86</v>
+      </c>
+      <c r="L800" s="10">
+        <v>102</v>
+      </c>
+      <c r="M800" s="10">
+        <f t="shared" si="33"/>
+        <v>188</v>
+      </c>
+      <c r="N800" s="10">
+        <f t="shared" si="36"/>
+        <v>-16</v>
+      </c>
+      <c r="O800" s="10">
+        <v>1</v>
+      </c>
+      <c r="P800" s="10">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q800" s="10" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R800" s="10">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S800" s="10">
+        <f t="shared" si="39"/>
+        <v>20</v>
+      </c>
+      <c r="T800" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="801" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A801" s="9">
+        <v>45700</v>
+      </c>
+      <c r="B801" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C801" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D801" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E801" s="10">
+        <v>0</v>
+      </c>
+      <c r="F801" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G801" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H801" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I801" s="10">
+        <v>239.5</v>
+      </c>
+      <c r="J801" s="11">
+        <v>10</v>
+      </c>
+      <c r="K801" s="10">
+        <v>134</v>
+      </c>
+      <c r="L801" s="10">
+        <v>130</v>
+      </c>
+      <c r="M801" s="10">
+        <f t="shared" si="33"/>
+        <v>264</v>
+      </c>
+      <c r="N801" s="10">
+        <f t="shared" si="36"/>
+        <v>4</v>
+      </c>
+      <c r="O801" s="10">
+        <v>1</v>
+      </c>
+      <c r="P801" s="10">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q801" s="10">
+        <f t="shared" si="35"/>
+        <v>24.5</v>
+      </c>
+      <c r="R801" s="10">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S801" s="10" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T801" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="802" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A802" s="9">
+        <v>45700</v>
+      </c>
+      <c r="B802" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C802" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D802" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E802" s="10">
+        <v>0</v>
+      </c>
+      <c r="F802" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G802" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H802" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I802" s="10">
+        <v>231.5</v>
+      </c>
+      <c r="J802" s="11">
+        <v>-9.5</v>
+      </c>
+      <c r="K802" s="10">
+        <v>103</v>
+      </c>
+      <c r="L802" s="10">
+        <v>116</v>
+      </c>
+      <c r="M802" s="10">
+        <f t="shared" si="33"/>
+        <v>219</v>
+      </c>
+      <c r="N802" s="10">
+        <f t="shared" si="36"/>
+        <v>-13</v>
+      </c>
+      <c r="O802" s="10">
+        <v>1</v>
+      </c>
+      <c r="P802" s="10">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q802" s="10" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R802" s="10">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S802" s="10">
+        <f t="shared" si="39"/>
+        <v>12.5</v>
+      </c>
+      <c r="T802" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="803" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A803" s="9">
+        <v>45700</v>
+      </c>
+      <c r="B803" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C803" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D803" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E803" s="10">
+        <v>0</v>
+      </c>
+      <c r="F803" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G803" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H803" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I803" s="10">
+        <v>212</v>
+      </c>
+      <c r="J803" s="11">
+        <v>2</v>
+      </c>
+      <c r="K803" s="10">
+        <v>96</v>
+      </c>
+      <c r="L803" s="10">
+        <v>100</v>
+      </c>
+      <c r="M803" s="10">
+        <f t="shared" si="33"/>
+        <v>196</v>
+      </c>
+      <c r="N803" s="10">
+        <f t="shared" si="36"/>
+        <v>-4</v>
+      </c>
+      <c r="O803" s="10">
+        <v>1</v>
+      </c>
+      <c r="P803" s="10">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q803" s="10" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R803" s="10">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S803" s="10">
+        <f t="shared" si="39"/>
+        <v>16</v>
+      </c>
+      <c r="T803" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="804" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A804" s="9">
+        <v>45700</v>
+      </c>
+      <c r="B804" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C804" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D804" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E804" s="10">
+        <v>0</v>
+      </c>
+      <c r="F804" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G804" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H804" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I804" s="10">
+        <v>235.5</v>
+      </c>
+      <c r="J804" s="11">
+        <v>12.5</v>
+      </c>
+      <c r="K804" s="10">
+        <v>131</v>
+      </c>
+      <c r="L804" s="10">
+        <v>108</v>
+      </c>
+      <c r="M804" s="10">
+        <f t="shared" si="33"/>
+        <v>239</v>
+      </c>
+      <c r="N804" s="10">
+        <f t="shared" si="36"/>
+        <v>23</v>
+      </c>
+      <c r="O804" s="10">
+        <v>1</v>
+      </c>
+      <c r="P804" s="10">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q804" s="10">
+        <f t="shared" si="35"/>
+        <v>3.5</v>
+      </c>
+      <c r="R804" s="10">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S804" s="10" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T804" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="805" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A805" s="9">
+        <v>45700</v>
+      </c>
+      <c r="B805" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C805" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D805" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E805" s="10">
+        <v>0</v>
+      </c>
+      <c r="F805" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G805" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H805" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I805" s="10">
+        <v>240</v>
+      </c>
+      <c r="J805" s="11">
+        <v>-8.5</v>
+      </c>
+      <c r="K805" s="10">
+        <v>148</v>
+      </c>
+      <c r="L805" s="10">
+        <v>149</v>
+      </c>
+      <c r="M805" s="10">
+        <f t="shared" si="33"/>
+        <v>297</v>
+      </c>
+      <c r="N805" s="10">
+        <f t="shared" si="36"/>
+        <v>-1</v>
+      </c>
+      <c r="O805" s="10">
+        <v>1</v>
+      </c>
+      <c r="P805" s="10">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q805" s="10">
+        <f t="shared" si="35"/>
+        <v>57</v>
+      </c>
+      <c r="R805" s="10">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S805" s="10" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T805" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="806" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A806" s="9">
+        <v>45700</v>
+      </c>
+      <c r="B806" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C806" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D806" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E806" s="10">
+        <v>0</v>
+      </c>
+      <c r="F806" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G806" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="H806" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="I806" s="10">
+        <v>238.5</v>
+      </c>
+      <c r="J806" s="11">
+        <v>4</v>
+      </c>
+      <c r="K806" s="10">
+        <v>119</v>
+      </c>
+      <c r="L806" s="10">
+        <v>111</v>
+      </c>
+      <c r="M806" s="10">
+        <f t="shared" si="33"/>
+        <v>230</v>
+      </c>
+      <c r="N806" s="10">
+        <f t="shared" si="36"/>
+        <v>8</v>
+      </c>
+      <c r="O806" s="10">
+        <v>1</v>
+      </c>
+      <c r="P806" s="10">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q806" s="10" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R806" s="10">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S806" s="10">
+        <f t="shared" si="39"/>
+        <v>8.5</v>
+      </c>
+      <c r="T806" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="807" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A807" s="9">
+        <v>45700</v>
+      </c>
+      <c r="B807" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C807" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D807" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E807" s="10">
+        <v>0</v>
+      </c>
+      <c r="F807" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G807" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H807" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="I807" s="10">
+        <v>219.5</v>
+      </c>
+      <c r="J807" s="11">
+        <v>-13.5</v>
+      </c>
+      <c r="K807" s="10">
+        <v>101</v>
+      </c>
+      <c r="L807" s="10">
+        <v>115</v>
+      </c>
+      <c r="M807" s="10">
+        <f t="shared" si="33"/>
+        <v>216</v>
+      </c>
+      <c r="N807" s="10">
+        <f t="shared" si="36"/>
+        <v>-14</v>
+      </c>
+      <c r="O807" s="10">
+        <v>1</v>
+      </c>
+      <c r="P807" s="10">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q807" s="10" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R807" s="10">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S807" s="10">
+        <f t="shared" si="39"/>
+        <v>3.5</v>
+      </c>
+      <c r="T807" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="808" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A808" s="9">
+        <v>45700</v>
+      </c>
+      <c r="B808" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C808" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D808" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E808" s="10">
+        <v>0</v>
+      </c>
+      <c r="F808" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G808" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H808" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I808" s="10">
+        <v>226</v>
+      </c>
+      <c r="J808" s="11">
+        <v>-5.5</v>
+      </c>
+      <c r="K808" s="10">
+        <v>103</v>
+      </c>
+      <c r="L808" s="10">
+        <v>101</v>
+      </c>
+      <c r="M808" s="10">
+        <f t="shared" si="33"/>
+        <v>204</v>
+      </c>
+      <c r="N808" s="10">
+        <f t="shared" si="36"/>
+        <v>2</v>
+      </c>
+      <c r="O808" s="10">
+        <v>1</v>
+      </c>
+      <c r="P808" s="10">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q808" s="10" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R808" s="10">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S808" s="10">
+        <f t="shared" si="39"/>
+        <v>22</v>
+      </c>
+      <c r="T808" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="809" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A809" s="9">
+        <v>45700</v>
+      </c>
+      <c r="B809" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C809" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D809" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E809" s="10">
+        <v>0</v>
+      </c>
+      <c r="F809" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G809" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H809" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="I809" s="10">
+        <v>236.5</v>
+      </c>
+      <c r="J809" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="K809" s="10">
+        <v>128</v>
+      </c>
+      <c r="L809" s="10">
+        <v>110</v>
+      </c>
+      <c r="M809" s="10">
+        <f t="shared" si="33"/>
+        <v>238</v>
+      </c>
+      <c r="N809" s="10">
+        <f t="shared" si="36"/>
+        <v>18</v>
+      </c>
+      <c r="O809" s="10">
+        <v>1</v>
+      </c>
+      <c r="P809" s="10">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q809" s="10">
+        <f t="shared" si="35"/>
+        <v>1.5</v>
+      </c>
+      <c r="R809" s="10">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S809" s="10" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T809" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="810" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A810" s="9">
+        <v>45700</v>
+      </c>
+      <c r="B810" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C810" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D810" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E810" s="10">
+        <v>0</v>
+      </c>
+      <c r="F810" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G810" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H810" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="I810" s="10">
+        <v>223.5</v>
+      </c>
+      <c r="J810" s="11">
+        <v>-6</v>
+      </c>
+      <c r="K810" s="10">
+        <v>111</v>
+      </c>
+      <c r="L810" s="10">
+        <v>119</v>
+      </c>
+      <c r="M810" s="10">
+        <f t="shared" si="33"/>
+        <v>230</v>
+      </c>
+      <c r="N810" s="10">
+        <f t="shared" si="36"/>
+        <v>-8</v>
+      </c>
+      <c r="O810" s="10">
+        <v>1</v>
+      </c>
+      <c r="P810" s="10">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q810" s="10">
+        <f t="shared" si="35"/>
+        <v>6.5</v>
+      </c>
+      <c r="R810" s="10">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S810" s="10" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T810" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="811" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A811" s="9">
+        <v>45700</v>
+      </c>
+      <c r="B811" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C811" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D811" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E811" s="10">
+        <v>0</v>
+      </c>
+      <c r="F811" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G811" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H811" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I811" s="10">
+        <v>231.5</v>
+      </c>
+      <c r="J811" s="11">
+        <v>-11.5</v>
+      </c>
+      <c r="K811" s="10">
+        <v>121</v>
+      </c>
+      <c r="L811" s="10">
+        <v>132</v>
+      </c>
+      <c r="M811" s="10">
+        <f t="shared" si="33"/>
+        <v>253</v>
+      </c>
+      <c r="N811" s="10">
+        <f t="shared" si="36"/>
+        <v>-11</v>
+      </c>
+      <c r="O811" s="10">
+        <v>1</v>
+      </c>
+      <c r="P811" s="10">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q811" s="10">
+        <f t="shared" si="35"/>
+        <v>21.5</v>
+      </c>
+      <c r="R811" s="10">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S811" s="10" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T811" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="812" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A812" s="9">
+        <v>45700</v>
+      </c>
+      <c r="B812" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C812" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D812" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E812" s="10">
+        <v>0</v>
+      </c>
+      <c r="F812" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G812" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H812" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I812" s="10">
+        <v>237.5</v>
+      </c>
+      <c r="J812" s="11">
+        <v>7.5</v>
+      </c>
+      <c r="K812" s="10">
+        <v>119</v>
+      </c>
+      <c r="L812" s="10">
+        <v>131</v>
+      </c>
+      <c r="M812" s="10">
+        <f t="shared" si="33"/>
+        <v>250</v>
+      </c>
+      <c r="N812" s="10">
+        <f t="shared" si="36"/>
+        <v>-12</v>
+      </c>
+      <c r="O812" s="10">
+        <v>1</v>
+      </c>
+      <c r="P812" s="10">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q812" s="10">
+        <f t="shared" si="35"/>
+        <v>12.5</v>
+      </c>
+      <c r="R812" s="10">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S812" s="10" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T812" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="813" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A813" s="9">
+        <v>45700</v>
+      </c>
+      <c r="B813" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C813" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D813" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E813" s="10">
+        <v>0</v>
+      </c>
+      <c r="F813" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G813" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H813" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I813" s="10">
+        <v>232.5</v>
+      </c>
+      <c r="J813" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="K813" s="10">
+        <v>107</v>
+      </c>
+      <c r="L813" s="10">
+        <v>111</v>
+      </c>
+      <c r="M813" s="10">
+        <f t="shared" si="33"/>
+        <v>218</v>
+      </c>
+      <c r="N813" s="10">
+        <f t="shared" si="36"/>
+        <v>-4</v>
+      </c>
+      <c r="O813" s="10">
+        <v>1</v>
+      </c>
+      <c r="P813" s="10">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q813" s="10" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R813" s="10">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S813" s="10">
+        <f t="shared" si="39"/>
+        <v>14.5</v>
+      </c>
+      <c r="T813" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="814" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A814" s="9">
+        <v>45700</v>
+      </c>
+      <c r="B814" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C814" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D814" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E814" s="10">
+        <v>0</v>
+      </c>
+      <c r="F814" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G814" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H814" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I814" s="10">
+        <v>235.5</v>
+      </c>
+      <c r="J814" s="11">
+        <v>-3.5</v>
+      </c>
+      <c r="K814" s="10">
+        <v>114</v>
+      </c>
+      <c r="L814" s="10">
+        <v>128</v>
+      </c>
+      <c r="M814" s="10">
+        <f t="shared" si="33"/>
+        <v>242</v>
+      </c>
+      <c r="N814" s="10">
+        <f t="shared" si="36"/>
+        <v>-14</v>
+      </c>
+      <c r="O814" s="10">
+        <v>1</v>
+      </c>
+      <c r="P814" s="10">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q814" s="10">
+        <f t="shared" si="35"/>
+        <v>6.5</v>
+      </c>
+      <c r="R814" s="10">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S814" s="10" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T814" s="10">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added game data for feb 13, 2025
</commit_message>
<xml_diff>
--- a/data/nba_points_2024_2025.xlsx
+++ b/data/nba_points_2024_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Documents/nba-points/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45C25B0-C79A-074E-B98C-495143C01F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1403999A-BA3D-DC49-8B94-9986B3140AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22940" yWindow="500" windowWidth="45860" windowHeight="28300" xr2:uid="{4B944735-6DC1-314A-AF10-68EBB82A81F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4900" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4930" uniqueCount="148">
   <si>
     <t>Date</t>
   </si>
@@ -1028,11 +1028,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78582E2E-5746-944D-860C-ACA920BD70CB}">
-  <dimension ref="A1:Y814"/>
+  <dimension ref="A1:Y819"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V803" sqref="V803"/>
+      <pane ySplit="1" topLeftCell="A775" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T822" sqref="T822"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1207,15 +1207,15 @@
       </c>
       <c r="V2" s="7">
         <f>SUM(O:O)</f>
-        <v>806</v>
+        <v>811</v>
       </c>
       <c r="W2" s="12">
         <f>SUM(P:P)</f>
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="X2" s="15">
         <f>SUM(R:R)</f>
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="Y2" s="20">
         <f>SUM(T:T)</f>
@@ -1370,15 +1370,15 @@
       </c>
       <c r="W4" s="14">
         <f>W2/V2</f>
-        <v>0.53101736972704716</v>
+        <v>0.53144266337854495</v>
       </c>
       <c r="X4" s="16">
         <f>X2/V2</f>
-        <v>0.46898263027295284</v>
+        <v>0.46855733662145499</v>
       </c>
       <c r="Y4" s="21">
         <f>Y2/V2</f>
-        <v>3.7220843672456576E-3</v>
+        <v>3.6991368680641184E-3</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1526,11 +1526,11 @@
       </c>
       <c r="W6" s="22">
         <f>AVERAGE(Q:Q)</f>
-        <v>14.809579439252337</v>
+        <v>14.827146171693736</v>
       </c>
       <c r="X6" s="23">
         <f>AVERAGE(S:S)</f>
-        <v>15.002645502645503</v>
+        <v>14.978947368421053</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -41521,7 +41521,7 @@
         <v>113</v>
       </c>
       <c r="M587" s="7">
-        <f t="shared" ref="M587:M814" si="33">K587+L587</f>
+        <f t="shared" ref="M587:M819" si="33">K587+L587</f>
         <v>232</v>
       </c>
       <c r="N587" s="7">
@@ -46005,7 +46005,7 @@
         <v>1</v>
       </c>
       <c r="Q652" s="10">
-        <f t="shared" ref="Q652:Q814" si="35">IF(P652=1,(M652-I652), "")</f>
+        <f t="shared" ref="Q652:Q819" si="35">IF(P652=1,(M652-I652), "")</f>
         <v>4</v>
       </c>
       <c r="R652" s="10">
@@ -46063,14 +46063,14 @@
         <v>236</v>
       </c>
       <c r="N653" s="10">
-        <f t="shared" ref="N653:N814" si="36">(L653-K653)*-1</f>
+        <f t="shared" ref="N653:N819" si="36">(L653-K653)*-1</f>
         <v>6</v>
       </c>
       <c r="O653" s="10">
         <v>1</v>
       </c>
       <c r="P653" s="10">
-        <f t="shared" ref="P653:P814" si="37">IF(M653&gt;I653,1,0)</f>
+        <f t="shared" ref="P653:P819" si="37">IF(M653&gt;I653,1,0)</f>
         <v>1</v>
       </c>
       <c r="Q653" s="10">
@@ -46078,15 +46078,15 @@
         <v>17.5</v>
       </c>
       <c r="R653" s="10">
-        <f t="shared" ref="R653:R814" si="38">IF(M653&lt;I653, 1, 0)</f>
+        <f t="shared" ref="R653:R819" si="38">IF(M653&lt;I653, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="S653" s="10" t="str">
-        <f t="shared" ref="S653:S814" si="39">IF(R653=1,(I653-M653),"")</f>
+        <f t="shared" ref="S653:S819" si="39">IF(R653=1,(I653-M653),"")</f>
         <v/>
       </c>
       <c r="T653" s="10">
-        <f t="shared" ref="T653:T814" si="40">IF(M653=I653,1,0)</f>
+        <f t="shared" ref="T653:T819" si="40">IF(M653=I653,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -57187,6 +57187,351 @@
         <v/>
       </c>
       <c r="T814" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="815" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A815" s="29">
+        <v>45701</v>
+      </c>
+      <c r="B815" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C815" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D815" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E815" s="30">
+        <v>0</v>
+      </c>
+      <c r="F815" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="G815" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="H815" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="I815" s="30">
+        <v>240</v>
+      </c>
+      <c r="J815" s="31">
+        <v>5</v>
+      </c>
+      <c r="K815" s="30">
+        <v>133</v>
+      </c>
+      <c r="L815" s="30">
+        <v>140</v>
+      </c>
+      <c r="M815" s="30">
+        <f t="shared" si="33"/>
+        <v>273</v>
+      </c>
+      <c r="N815" s="30">
+        <f t="shared" si="36"/>
+        <v>-7</v>
+      </c>
+      <c r="O815" s="30">
+        <v>1</v>
+      </c>
+      <c r="P815" s="30">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q815" s="30">
+        <f t="shared" si="35"/>
+        <v>33</v>
+      </c>
+      <c r="R815" s="30">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S815" s="30" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T815" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="816" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A816" s="29">
+        <v>45701</v>
+      </c>
+      <c r="B816" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C816" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D816" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E816" s="30">
+        <v>0</v>
+      </c>
+      <c r="F816" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="G816" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="H816" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="I816" s="30">
+        <v>220.5</v>
+      </c>
+      <c r="J816" s="31">
+        <v>-1.5</v>
+      </c>
+      <c r="K816" s="30">
+        <v>105</v>
+      </c>
+      <c r="L816" s="30">
+        <v>98</v>
+      </c>
+      <c r="M816" s="30">
+        <f t="shared" si="33"/>
+        <v>203</v>
+      </c>
+      <c r="N816" s="30">
+        <f t="shared" si="36"/>
+        <v>7</v>
+      </c>
+      <c r="O816" s="30">
+        <v>1</v>
+      </c>
+      <c r="P816" s="30">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q816" s="30" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R816" s="30">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S816" s="30">
+        <f t="shared" si="39"/>
+        <v>17.5</v>
+      </c>
+      <c r="T816" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="817" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A817" s="29">
+        <v>45701</v>
+      </c>
+      <c r="B817" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C817" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D817" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E817" s="30">
+        <v>0</v>
+      </c>
+      <c r="F817" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="G817" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="H817" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="I817" s="30">
+        <v>220.5</v>
+      </c>
+      <c r="J817" s="31">
+        <v>5</v>
+      </c>
+      <c r="K817" s="30">
+        <v>101</v>
+      </c>
+      <c r="L817" s="30">
+        <v>116</v>
+      </c>
+      <c r="M817" s="30">
+        <f t="shared" si="33"/>
+        <v>217</v>
+      </c>
+      <c r="N817" s="30">
+        <f t="shared" si="36"/>
+        <v>-15</v>
+      </c>
+      <c r="O817" s="30">
+        <v>1</v>
+      </c>
+      <c r="P817" s="30">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q817" s="30" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R817" s="30">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S817" s="30">
+        <f t="shared" si="39"/>
+        <v>3.5</v>
+      </c>
+      <c r="T817" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="818" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A818" s="29">
+        <v>45701</v>
+      </c>
+      <c r="B818" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C818" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D818" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="E818" s="30">
+        <v>0</v>
+      </c>
+      <c r="F818" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G818" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="H818" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="I818" s="30">
+        <v>223.5</v>
+      </c>
+      <c r="J818" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="K818" s="30">
+        <v>113</v>
+      </c>
+      <c r="L818" s="30">
+        <v>118</v>
+      </c>
+      <c r="M818" s="30">
+        <f t="shared" si="33"/>
+        <v>231</v>
+      </c>
+      <c r="N818" s="30">
+        <f t="shared" si="36"/>
+        <v>-5</v>
+      </c>
+      <c r="O818" s="30">
+        <v>1</v>
+      </c>
+      <c r="P818" s="30">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q818" s="30">
+        <f t="shared" si="35"/>
+        <v>7.5</v>
+      </c>
+      <c r="R818" s="30">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S818" s="30" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T818" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="819" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A819" s="29">
+        <v>45701</v>
+      </c>
+      <c r="B819" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C819" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D819" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E819" s="30">
+        <v>0</v>
+      </c>
+      <c r="F819" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="G819" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="H819" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="I819" s="30">
+        <v>224.5</v>
+      </c>
+      <c r="J819" s="31">
+        <v>8.5</v>
+      </c>
+      <c r="K819" s="30">
+        <v>120</v>
+      </c>
+      <c r="L819" s="30">
+        <v>116</v>
+      </c>
+      <c r="M819" s="30">
+        <f t="shared" si="33"/>
+        <v>236</v>
+      </c>
+      <c r="N819" s="30">
+        <f t="shared" si="36"/>
+        <v>4</v>
+      </c>
+      <c r="O819" s="30">
+        <v>1</v>
+      </c>
+      <c r="P819" s="30">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q819" s="30">
+        <f t="shared" si="35"/>
+        <v>11.5</v>
+      </c>
+      <c r="R819" s="30">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S819" s="30" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T819" s="30">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added a few days of game data
</commit_message>
<xml_diff>
--- a/data/nba_points_2024_2025.xlsx
+++ b/data/nba_points_2024_2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Documents/nba-points/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1403999A-BA3D-DC49-8B94-9986B3140AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6ABD26-A469-B641-8D1A-E832EE06AC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22940" yWindow="500" windowWidth="45860" windowHeight="28300" xr2:uid="{4B944735-6DC1-314A-AF10-68EBB82A81F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4930" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5074" uniqueCount="148">
   <si>
     <t>Date</t>
   </si>
@@ -1028,11 +1028,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78582E2E-5746-944D-860C-ACA920BD70CB}">
-  <dimension ref="A1:Y819"/>
+  <dimension ref="A1:Y843"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A775" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T822" sqref="T822"/>
+      <pane ySplit="1" topLeftCell="A796" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V815" sqref="V815"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1207,15 +1207,15 @@
       </c>
       <c r="V2" s="7">
         <f>SUM(O:O)</f>
-        <v>811</v>
+        <v>835</v>
       </c>
       <c r="W2" s="12">
         <f>SUM(P:P)</f>
-        <v>431</v>
+        <v>443</v>
       </c>
       <c r="X2" s="15">
         <f>SUM(R:R)</f>
-        <v>380</v>
+        <v>392</v>
       </c>
       <c r="Y2" s="20">
         <f>SUM(T:T)</f>
@@ -1370,15 +1370,15 @@
       </c>
       <c r="W4" s="14">
         <f>W2/V2</f>
-        <v>0.53144266337854495</v>
+        <v>0.53053892215568865</v>
       </c>
       <c r="X4" s="16">
         <f>X2/V2</f>
-        <v>0.46855733662145499</v>
+        <v>0.4694610778443114</v>
       </c>
       <c r="Y4" s="21">
         <f>Y2/V2</f>
-        <v>3.6991368680641184E-3</v>
+        <v>3.592814371257485E-3</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1526,11 +1526,11 @@
       </c>
       <c r="W6" s="22">
         <f>AVERAGE(Q:Q)</f>
-        <v>14.827146171693736</v>
+        <v>14.62528216704289</v>
       </c>
       <c r="X6" s="23">
         <f>AVERAGE(S:S)</f>
-        <v>14.978947368421053</v>
+        <v>14.961734693877551</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -41521,7 +41521,7 @@
         <v>113</v>
       </c>
       <c r="M587" s="7">
-        <f t="shared" ref="M587:M819" si="33">K587+L587</f>
+        <f t="shared" ref="M587:M841" si="33">K587+L587</f>
         <v>232</v>
       </c>
       <c r="N587" s="7">
@@ -46005,7 +46005,7 @@
         <v>1</v>
       </c>
       <c r="Q652" s="10">
-        <f t="shared" ref="Q652:Q819" si="35">IF(P652=1,(M652-I652), "")</f>
+        <f t="shared" ref="Q652:Q843" si="35">IF(P652=1,(M652-I652), "")</f>
         <v>4</v>
       </c>
       <c r="R652" s="10">
@@ -46063,14 +46063,14 @@
         <v>236</v>
       </c>
       <c r="N653" s="10">
-        <f t="shared" ref="N653:N819" si="36">(L653-K653)*-1</f>
+        <f t="shared" ref="N653:N843" si="36">(L653-K653)*-1</f>
         <v>6</v>
       </c>
       <c r="O653" s="10">
         <v>1</v>
       </c>
       <c r="P653" s="10">
-        <f t="shared" ref="P653:P819" si="37">IF(M653&gt;I653,1,0)</f>
+        <f t="shared" ref="P653:P843" si="37">IF(M653&gt;I653,1,0)</f>
         <v>1</v>
       </c>
       <c r="Q653" s="10">
@@ -46078,15 +46078,15 @@
         <v>17.5</v>
       </c>
       <c r="R653" s="10">
-        <f t="shared" ref="R653:R819" si="38">IF(M653&lt;I653, 1, 0)</f>
+        <f t="shared" ref="R653:R843" si="38">IF(M653&lt;I653, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="S653" s="10" t="str">
-        <f t="shared" ref="S653:S819" si="39">IF(R653=1,(I653-M653),"")</f>
+        <f t="shared" ref="S653:S843" si="39">IF(R653=1,(I653-M653),"")</f>
         <v/>
       </c>
       <c r="T653" s="10">
-        <f t="shared" ref="T653:T819" si="40">IF(M653=I653,1,0)</f>
+        <f t="shared" ref="T653:T843" si="40">IF(M653=I653,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -57532,6 +57532,1662 @@
         <v/>
       </c>
       <c r="T819" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="820" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A820" s="9">
+        <v>45707</v>
+      </c>
+      <c r="B820" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C820" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D820" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E820" s="10">
+        <v>0</v>
+      </c>
+      <c r="F820" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G820" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H820" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I820" s="10">
+        <v>230.5</v>
+      </c>
+      <c r="J820" s="11">
+        <v>-13.5</v>
+      </c>
+      <c r="K820" s="10">
+        <v>100</v>
+      </c>
+      <c r="L820" s="10">
+        <v>97</v>
+      </c>
+      <c r="M820" s="10">
+        <f t="shared" si="33"/>
+        <v>197</v>
+      </c>
+      <c r="N820" s="10">
+        <f t="shared" si="36"/>
+        <v>3</v>
+      </c>
+      <c r="O820" s="10">
+        <v>1</v>
+      </c>
+      <c r="P820" s="10">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q820" s="10" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R820" s="10">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S820" s="10">
+        <f t="shared" si="39"/>
+        <v>33.5</v>
+      </c>
+      <c r="T820" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="821" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A821" s="29">
+        <v>45708</v>
+      </c>
+      <c r="B821" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C821" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D821" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E821" s="30">
+        <v>0</v>
+      </c>
+      <c r="F821" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="G821" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H821" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="I821" s="30">
+        <v>224</v>
+      </c>
+      <c r="J821" s="31">
+        <v>8</v>
+      </c>
+      <c r="K821" s="30">
+        <v>124</v>
+      </c>
+      <c r="L821" s="30">
+        <v>104</v>
+      </c>
+      <c r="M821" s="30">
+        <f t="shared" si="33"/>
+        <v>228</v>
+      </c>
+      <c r="N821" s="30">
+        <f t="shared" si="36"/>
+        <v>20</v>
+      </c>
+      <c r="O821" s="30">
+        <v>1</v>
+      </c>
+      <c r="P821" s="30">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q821" s="30">
+        <f t="shared" si="35"/>
+        <v>4</v>
+      </c>
+      <c r="R821" s="30">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S821" s="30" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T821" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="822" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A822" s="29">
+        <v>45708</v>
+      </c>
+      <c r="B822" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C822" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D822" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E822" s="30">
+        <v>0</v>
+      </c>
+      <c r="F822" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G822" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="H822" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="I822" s="30">
+        <v>250.5</v>
+      </c>
+      <c r="J822" s="31">
+        <v>1</v>
+      </c>
+      <c r="K822" s="30">
+        <v>113</v>
+      </c>
+      <c r="L822" s="30">
+        <v>127</v>
+      </c>
+      <c r="M822" s="30">
+        <f t="shared" si="33"/>
+        <v>240</v>
+      </c>
+      <c r="N822" s="30">
+        <f t="shared" si="36"/>
+        <v>-14</v>
+      </c>
+      <c r="O822" s="30">
+        <v>1</v>
+      </c>
+      <c r="P822" s="30">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q822" s="30" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R822" s="30">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S822" s="30">
+        <f t="shared" si="39"/>
+        <v>10.5</v>
+      </c>
+      <c r="T822" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="823" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A823" s="29">
+        <v>45708</v>
+      </c>
+      <c r="B823" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C823" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D823" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E823" s="30">
+        <v>0</v>
+      </c>
+      <c r="F823" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="G823" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="H823" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="I823" s="30">
+        <v>221.5</v>
+      </c>
+      <c r="J823" s="31">
+        <v>13.5</v>
+      </c>
+      <c r="K823" s="30">
+        <v>110</v>
+      </c>
+      <c r="L823" s="30">
+        <v>97</v>
+      </c>
+      <c r="M823" s="30">
+        <f t="shared" si="33"/>
+        <v>207</v>
+      </c>
+      <c r="N823" s="30">
+        <f t="shared" si="36"/>
+        <v>13</v>
+      </c>
+      <c r="O823" s="30">
+        <v>1</v>
+      </c>
+      <c r="P823" s="30">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q823" s="30" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R823" s="30">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S823" s="30">
+        <f t="shared" si="39"/>
+        <v>14.5</v>
+      </c>
+      <c r="T823" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="824" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A824" s="29">
+        <v>45708</v>
+      </c>
+      <c r="B824" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C824" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D824" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E824" s="30">
+        <v>0</v>
+      </c>
+      <c r="F824" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="G824" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="H824" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="I824" s="30">
+        <v>221.5</v>
+      </c>
+      <c r="J824" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="K824" s="30">
+        <v>114</v>
+      </c>
+      <c r="L824" s="30">
+        <v>108</v>
+      </c>
+      <c r="M824" s="30">
+        <f t="shared" si="33"/>
+        <v>222</v>
+      </c>
+      <c r="N824" s="30">
+        <f t="shared" si="36"/>
+        <v>6</v>
+      </c>
+      <c r="O824" s="30">
+        <v>1</v>
+      </c>
+      <c r="P824" s="30">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q824" s="30">
+        <f t="shared" si="35"/>
+        <v>0.5</v>
+      </c>
+      <c r="R824" s="30">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S824" s="30" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T824" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="825" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A825" s="29">
+        <v>45708</v>
+      </c>
+      <c r="B825" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C825" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D825" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E825" s="30">
+        <v>0</v>
+      </c>
+      <c r="F825" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="G825" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H825" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="I825" s="30">
+        <v>243</v>
+      </c>
+      <c r="J825" s="31">
+        <v>-13</v>
+      </c>
+      <c r="K825" s="30">
+        <v>111</v>
+      </c>
+      <c r="L825" s="30">
+        <v>113</v>
+      </c>
+      <c r="M825" s="30">
+        <f t="shared" si="33"/>
+        <v>224</v>
+      </c>
+      <c r="N825" s="30">
+        <f t="shared" si="36"/>
+        <v>-2</v>
+      </c>
+      <c r="O825" s="30">
+        <v>1</v>
+      </c>
+      <c r="P825" s="30">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q825" s="30" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R825" s="30">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S825" s="30">
+        <f t="shared" si="39"/>
+        <v>19</v>
+      </c>
+      <c r="T825" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="826" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A826" s="29">
+        <v>45708</v>
+      </c>
+      <c r="B826" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C826" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D826" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E826" s="30">
+        <v>0</v>
+      </c>
+      <c r="F826" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="G826" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="H826" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="I826" s="30">
+        <v>225</v>
+      </c>
+      <c r="J826" s="31">
+        <v>-1.5</v>
+      </c>
+      <c r="K826" s="30">
+        <v>110</v>
+      </c>
+      <c r="L826" s="30">
+        <v>116</v>
+      </c>
+      <c r="M826" s="30">
+        <f t="shared" si="33"/>
+        <v>226</v>
+      </c>
+      <c r="N826" s="30">
+        <f t="shared" si="36"/>
+        <v>-6</v>
+      </c>
+      <c r="O826" s="30">
+        <v>1</v>
+      </c>
+      <c r="P826" s="30">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q826" s="30">
+        <f t="shared" si="35"/>
+        <v>1</v>
+      </c>
+      <c r="R826" s="30">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S826" s="30" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T826" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="827" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A827" s="29">
+        <v>45708</v>
+      </c>
+      <c r="B827" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C827" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D827" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E827" s="30">
+        <v>0</v>
+      </c>
+      <c r="F827" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G827" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="H827" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="I827" s="30">
+        <v>228</v>
+      </c>
+      <c r="J827" s="31">
+        <v>-15</v>
+      </c>
+      <c r="K827" s="30">
+        <v>115</v>
+      </c>
+      <c r="L827" s="30">
+        <v>129</v>
+      </c>
+      <c r="M827" s="30">
+        <f t="shared" si="33"/>
+        <v>244</v>
+      </c>
+      <c r="N827" s="30">
+        <f t="shared" si="36"/>
+        <v>-14</v>
+      </c>
+      <c r="O827" s="30">
+        <v>1</v>
+      </c>
+      <c r="P827" s="30">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q827" s="30">
+        <f t="shared" si="35"/>
+        <v>16</v>
+      </c>
+      <c r="R827" s="30">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S827" s="30" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T827" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="828" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A828" s="29">
+        <v>45708</v>
+      </c>
+      <c r="B828" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C828" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D828" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="E828" s="30">
+        <v>0</v>
+      </c>
+      <c r="F828" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="G828" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="H828" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="I828" s="30">
+        <v>230.5</v>
+      </c>
+      <c r="J828" s="31">
+        <v>-2</v>
+      </c>
+      <c r="K828" s="30">
+        <v>109</v>
+      </c>
+      <c r="L828" s="30">
+        <v>120</v>
+      </c>
+      <c r="M828" s="30">
+        <f t="shared" si="33"/>
+        <v>229</v>
+      </c>
+      <c r="N828" s="30">
+        <f t="shared" si="36"/>
+        <v>-11</v>
+      </c>
+      <c r="O828" s="30">
+        <v>1</v>
+      </c>
+      <c r="P828" s="30">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q828" s="30" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R828" s="30">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S828" s="30">
+        <f t="shared" si="39"/>
+        <v>1.5</v>
+      </c>
+      <c r="T828" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="829" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A829" s="29">
+        <v>45708</v>
+      </c>
+      <c r="B829" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C829" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D829" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E829" s="30">
+        <v>0</v>
+      </c>
+      <c r="F829" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G829" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="H829" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="I829" s="30">
+        <v>226</v>
+      </c>
+      <c r="J829" s="31">
+        <v>5.5</v>
+      </c>
+      <c r="K829" s="30">
+        <v>110</v>
+      </c>
+      <c r="L829" s="30">
+        <v>102</v>
+      </c>
+      <c r="M829" s="30">
+        <f t="shared" si="33"/>
+        <v>212</v>
+      </c>
+      <c r="N829" s="30">
+        <f t="shared" si="36"/>
+        <v>8</v>
+      </c>
+      <c r="O829" s="30">
+        <v>1</v>
+      </c>
+      <c r="P829" s="30">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q829" s="30" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R829" s="30">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S829" s="30">
+        <f t="shared" si="39"/>
+        <v>14</v>
+      </c>
+      <c r="T829" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="830" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A830" s="9">
+        <v>45709</v>
+      </c>
+      <c r="B830" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C830" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D830" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E830" s="10">
+        <v>0</v>
+      </c>
+      <c r="F830" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G830" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H830" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="I830" s="10">
+        <v>241.5</v>
+      </c>
+      <c r="J830" s="11">
+        <v>-7.5</v>
+      </c>
+      <c r="K830" s="10">
+        <v>105</v>
+      </c>
+      <c r="L830" s="10">
+        <v>142</v>
+      </c>
+      <c r="M830" s="10">
+        <f t="shared" si="33"/>
+        <v>247</v>
+      </c>
+      <c r="N830" s="10">
+        <f t="shared" si="36"/>
+        <v>-37</v>
+      </c>
+      <c r="O830" s="10">
+        <v>1</v>
+      </c>
+      <c r="P830" s="10">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q830" s="10">
+        <f t="shared" si="35"/>
+        <v>5.5</v>
+      </c>
+      <c r="R830" s="10">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S830" s="10" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T830" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="831" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A831" s="9">
+        <v>45709</v>
+      </c>
+      <c r="B831" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C831" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D831" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E831" s="10">
+        <v>0</v>
+      </c>
+      <c r="F831" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G831" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H831" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="I831" s="10">
+        <v>222.5</v>
+      </c>
+      <c r="J831" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="K831" s="10">
+        <v>105</v>
+      </c>
+      <c r="L831" s="10">
+        <v>104</v>
+      </c>
+      <c r="M831" s="10">
+        <f t="shared" si="33"/>
+        <v>209</v>
+      </c>
+      <c r="N831" s="10">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="O831" s="10">
+        <v>1</v>
+      </c>
+      <c r="P831" s="10">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q831" s="10" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R831" s="10">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S831" s="10">
+        <f t="shared" si="39"/>
+        <v>13.5</v>
+      </c>
+      <c r="T831" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="832" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A832" s="9">
+        <v>45709</v>
+      </c>
+      <c r="B832" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C832" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D832" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E832" s="10">
+        <v>0</v>
+      </c>
+      <c r="F832" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G832" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H832" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I832" s="10">
+        <v>228.5</v>
+      </c>
+      <c r="J832" s="11">
+        <v>6.5</v>
+      </c>
+      <c r="K832" s="10">
+        <v>104</v>
+      </c>
+      <c r="L832" s="10">
+        <v>101</v>
+      </c>
+      <c r="M832" s="10">
+        <f t="shared" si="33"/>
+        <v>205</v>
+      </c>
+      <c r="N832" s="10">
+        <f t="shared" si="36"/>
+        <v>3</v>
+      </c>
+      <c r="O832" s="10">
+        <v>1</v>
+      </c>
+      <c r="P832" s="10">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q832" s="10" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R832" s="10">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S832" s="10">
+        <f t="shared" si="39"/>
+        <v>23.5</v>
+      </c>
+      <c r="T832" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="833" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A833" s="9">
+        <v>45709</v>
+      </c>
+      <c r="B833" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C833" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D833" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E833" s="10">
+        <v>0</v>
+      </c>
+      <c r="F833" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G833" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H833" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="I833" s="10">
+        <v>219.5</v>
+      </c>
+      <c r="J833" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="K833" s="10">
+        <v>120</v>
+      </c>
+      <c r="L833" s="10">
+        <v>111</v>
+      </c>
+      <c r="M833" s="10">
+        <f t="shared" si="33"/>
+        <v>231</v>
+      </c>
+      <c r="N833" s="10">
+        <f t="shared" si="36"/>
+        <v>9</v>
+      </c>
+      <c r="O833" s="10">
+        <v>1</v>
+      </c>
+      <c r="P833" s="10">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q833" s="10">
+        <f t="shared" si="35"/>
+        <v>11.5</v>
+      </c>
+      <c r="R833" s="10">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S833" s="10" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T833" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="834" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A834" s="9">
+        <v>45709</v>
+      </c>
+      <c r="B834" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C834" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D834" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E834" s="10">
+        <v>0</v>
+      </c>
+      <c r="F834" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G834" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H834" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I834" s="10">
+        <v>232.5</v>
+      </c>
+      <c r="J834" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="K834" s="10">
+        <v>125</v>
+      </c>
+      <c r="L834" s="10">
+        <v>110</v>
+      </c>
+      <c r="M834" s="10">
+        <f t="shared" si="33"/>
+        <v>235</v>
+      </c>
+      <c r="N834" s="10">
+        <f t="shared" si="36"/>
+        <v>15</v>
+      </c>
+      <c r="O834" s="10">
+        <v>1</v>
+      </c>
+      <c r="P834" s="10">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q834" s="10">
+        <f t="shared" si="35"/>
+        <v>2.5</v>
+      </c>
+      <c r="R834" s="10">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S834" s="10" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T834" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="835" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A835" s="9">
+        <v>45709</v>
+      </c>
+      <c r="B835" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C835" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D835" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E835" s="10">
+        <v>0</v>
+      </c>
+      <c r="F835" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G835" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H835" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I835" s="10">
+        <v>234.5</v>
+      </c>
+      <c r="J835" s="11">
+        <v>-4.5</v>
+      </c>
+      <c r="K835" s="10">
+        <v>103</v>
+      </c>
+      <c r="L835" s="10">
+        <v>111</v>
+      </c>
+      <c r="M835" s="10">
+        <f t="shared" si="33"/>
+        <v>214</v>
+      </c>
+      <c r="N835" s="10">
+        <f t="shared" si="36"/>
+        <v>-8</v>
+      </c>
+      <c r="O835" s="10">
+        <v>1</v>
+      </c>
+      <c r="P835" s="10">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q835" s="10" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R835" s="10">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S835" s="10">
+        <f t="shared" si="39"/>
+        <v>20.5</v>
+      </c>
+      <c r="T835" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="836" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A836" s="9">
+        <v>45709</v>
+      </c>
+      <c r="B836" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C836" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D836" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E836" s="10">
+        <v>0</v>
+      </c>
+      <c r="F836" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G836" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H836" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I836" s="10">
+        <v>216.5</v>
+      </c>
+      <c r="J836" s="11">
+        <v>-5</v>
+      </c>
+      <c r="K836" s="10">
+        <v>115</v>
+      </c>
+      <c r="L836" s="10">
+        <v>121</v>
+      </c>
+      <c r="M836" s="10">
+        <f t="shared" si="33"/>
+        <v>236</v>
+      </c>
+      <c r="N836" s="10">
+        <f t="shared" si="36"/>
+        <v>-6</v>
+      </c>
+      <c r="O836" s="10">
+        <v>1</v>
+      </c>
+      <c r="P836" s="10">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q836" s="10">
+        <f t="shared" si="35"/>
+        <v>19.5</v>
+      </c>
+      <c r="R836" s="10">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S836" s="10" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T836" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="837" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A837" s="9">
+        <v>45709</v>
+      </c>
+      <c r="B837" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C837" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D837" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E837" s="10">
+        <v>0</v>
+      </c>
+      <c r="F837" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G837" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H837" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I837" s="10">
+        <v>235.5</v>
+      </c>
+      <c r="J837" s="11">
+        <v>16.5</v>
+      </c>
+      <c r="K837" s="10">
+        <v>130</v>
+      </c>
+      <c r="L837" s="10">
+        <v>107</v>
+      </c>
+      <c r="M837" s="10">
+        <f t="shared" si="33"/>
+        <v>237</v>
+      </c>
+      <c r="N837" s="10">
+        <f t="shared" si="36"/>
+        <v>23</v>
+      </c>
+      <c r="O837" s="10">
+        <v>1</v>
+      </c>
+      <c r="P837" s="10">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q837" s="10">
+        <f t="shared" si="35"/>
+        <v>1.5</v>
+      </c>
+      <c r="R837" s="10">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S837" s="10" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T837" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="838" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A838" s="9">
+        <v>45709</v>
+      </c>
+      <c r="B838" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C838" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D838" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E838" s="10">
+        <v>0</v>
+      </c>
+      <c r="F838" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G838" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H838" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I838" s="10">
+        <v>234.5</v>
+      </c>
+      <c r="J838" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="K838" s="10">
+        <v>132</v>
+      </c>
+      <c r="L838" s="10">
+        <v>108</v>
+      </c>
+      <c r="M838" s="10">
+        <f t="shared" si="33"/>
+        <v>240</v>
+      </c>
+      <c r="N838" s="10">
+        <f t="shared" si="36"/>
+        <v>24</v>
+      </c>
+      <c r="O838" s="10">
+        <v>1</v>
+      </c>
+      <c r="P838" s="10">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q838" s="10">
+        <f t="shared" si="35"/>
+        <v>5.5</v>
+      </c>
+      <c r="R838" s="10">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S838" s="10" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T838" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="839" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A839" s="29">
+        <v>45710</v>
+      </c>
+      <c r="B839" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C839" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D839" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E839" s="30">
+        <v>0</v>
+      </c>
+      <c r="F839" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="G839" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="H839" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="I839" s="30">
+        <v>239</v>
+      </c>
+      <c r="J839" s="31">
+        <v>5.5</v>
+      </c>
+      <c r="K839" s="30">
+        <v>121</v>
+      </c>
+      <c r="L839" s="30">
+        <v>117</v>
+      </c>
+      <c r="M839" s="30">
+        <f t="shared" si="33"/>
+        <v>238</v>
+      </c>
+      <c r="N839" s="30">
+        <f t="shared" si="36"/>
+        <v>4</v>
+      </c>
+      <c r="O839" s="30">
+        <v>1</v>
+      </c>
+      <c r="P839" s="30">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q839" s="30" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R839" s="30">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S839" s="30">
+        <f t="shared" si="39"/>
+        <v>1</v>
+      </c>
+      <c r="T839" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="840" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A840" s="29">
+        <v>45710</v>
+      </c>
+      <c r="B840" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C840" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D840" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E840" s="30">
+        <v>0</v>
+      </c>
+      <c r="F840" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G840" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="H840" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="I840" s="30">
+        <v>212</v>
+      </c>
+      <c r="J840" s="31">
+        <v>-9.5</v>
+      </c>
+      <c r="K840" s="30">
+        <v>105</v>
+      </c>
+      <c r="L840" s="30">
+        <v>103</v>
+      </c>
+      <c r="M840" s="30">
+        <f t="shared" si="33"/>
+        <v>208</v>
+      </c>
+      <c r="N840" s="30">
+        <f t="shared" si="36"/>
+        <v>2</v>
+      </c>
+      <c r="O840" s="30">
+        <v>1</v>
+      </c>
+      <c r="P840" s="30">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q840" s="30" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R840" s="30">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S840" s="30">
+        <f t="shared" si="39"/>
+        <v>4</v>
+      </c>
+      <c r="T840" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="841" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A841" s="29">
+        <v>45710</v>
+      </c>
+      <c r="B841" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C841" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D841" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E841" s="30">
+        <v>0</v>
+      </c>
+      <c r="F841" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="G841" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="H841" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="I841" s="30">
+        <v>240.5</v>
+      </c>
+      <c r="J841" s="31">
+        <v>-6.5</v>
+      </c>
+      <c r="K841" s="30">
+        <v>123</v>
+      </c>
+      <c r="L841" s="30">
+        <v>100</v>
+      </c>
+      <c r="M841" s="30">
+        <f t="shared" si="33"/>
+        <v>223</v>
+      </c>
+      <c r="N841" s="30">
+        <f t="shared" si="36"/>
+        <v>23</v>
+      </c>
+      <c r="O841" s="30">
+        <v>1</v>
+      </c>
+      <c r="P841" s="30">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q841" s="30" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R841" s="30">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S841" s="30">
+        <f t="shared" si="39"/>
+        <v>17.5</v>
+      </c>
+      <c r="T841" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="842" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A842" s="29">
+        <v>45710</v>
+      </c>
+      <c r="B842" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C842" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D842" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E842" s="30">
+        <v>0</v>
+      </c>
+      <c r="F842" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G842" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="H842" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="I842" s="30">
+        <v>229.5</v>
+      </c>
+      <c r="J842" s="31">
+        <v>8.5</v>
+      </c>
+      <c r="K842" s="30">
+        <v>115</v>
+      </c>
+      <c r="L842" s="30">
+        <v>124</v>
+      </c>
+      <c r="M842" s="30">
+        <f t="shared" ref="M842:M843" si="41">K842+L842</f>
+        <v>239</v>
+      </c>
+      <c r="N842" s="30">
+        <f t="shared" si="36"/>
+        <v>-9</v>
+      </c>
+      <c r="O842" s="30">
+        <v>1</v>
+      </c>
+      <c r="P842" s="30">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q842" s="30">
+        <f t="shared" si="35"/>
+        <v>9.5</v>
+      </c>
+      <c r="R842" s="30">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S842" s="30" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T842" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="843" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A843" s="29">
+        <v>45710</v>
+      </c>
+      <c r="B843" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C843" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D843" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E843" s="30">
+        <v>0</v>
+      </c>
+      <c r="F843" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G843" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H843" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I843" s="30">
+        <v>217.5</v>
+      </c>
+      <c r="J843" s="31">
+        <v>-5.5</v>
+      </c>
+      <c r="K843" s="30">
+        <v>88</v>
+      </c>
+      <c r="L843" s="30">
+        <v>141</v>
+      </c>
+      <c r="M843" s="30">
+        <f t="shared" si="41"/>
+        <v>229</v>
+      </c>
+      <c r="N843" s="30">
+        <f t="shared" si="36"/>
+        <v>-53</v>
+      </c>
+      <c r="O843" s="30">
+        <v>1</v>
+      </c>
+      <c r="P843" s="30">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q843" s="30">
+        <f t="shared" si="35"/>
+        <v>11.5</v>
+      </c>
+      <c r="R843" s="30">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S843" s="30" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T843" s="30">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added game data for feb 27, 2025
</commit_message>
<xml_diff>
--- a/data/nba_points_2024_2025.xlsx
+++ b/data/nba_points_2024_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Documents/nba-points/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1299DDCA-737F-F348-8E3D-1C082171CAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67B763F-6C6B-7F46-8EAD-CA54D7BD6322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22940" yWindow="500" windowWidth="45860" windowHeight="28300" xr2:uid="{4B944735-6DC1-314A-AF10-68EBB82A81F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5224" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5278" uniqueCount="148">
   <si>
     <t>Date</t>
   </si>
@@ -1028,11 +1028,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78582E2E-5746-944D-860C-ACA920BD70CB}">
-  <dimension ref="A1:Y868"/>
+  <dimension ref="A1:Y877"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A822" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A869" sqref="A869"/>
+      <pane ySplit="1" topLeftCell="A837" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E852" sqref="E852"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1207,15 +1207,15 @@
       </c>
       <c r="V2" s="7">
         <f>SUM(O:O)</f>
-        <v>860</v>
+        <v>869</v>
       </c>
       <c r="W2" s="12">
         <f>SUM(P:P)</f>
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="X2" s="15">
         <f>SUM(R:R)</f>
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="Y2" s="20">
         <f>SUM(T:T)</f>
@@ -1370,15 +1370,15 @@
       </c>
       <c r="W4" s="14">
         <f>W2/V2</f>
-        <v>0.52558139534883719</v>
+        <v>0.52474108170310707</v>
       </c>
       <c r="X4" s="16">
         <f>X2/V2</f>
-        <v>0.47441860465116281</v>
+        <v>0.47525891829689298</v>
       </c>
       <c r="Y4" s="21">
         <f>Y2/V2</f>
-        <v>3.4883720930232558E-3</v>
+        <v>3.4522439585730723E-3</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1526,11 +1526,11 @@
       </c>
       <c r="W6" s="22">
         <f>AVERAGE(Q:Q)</f>
-        <v>14.793141592920353</v>
+        <v>14.834429824561404</v>
       </c>
       <c r="X6" s="23">
         <f>AVERAGE(S:S)</f>
-        <v>15.042892156862745</v>
+        <v>15.062953995157384</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -46005,7 +46005,7 @@
         <v>1</v>
       </c>
       <c r="Q652" s="10">
-        <f t="shared" ref="Q652:Q868" si="35">IF(P652=1,(M652-I652), "")</f>
+        <f t="shared" ref="Q652:Q877" si="35">IF(P652=1,(M652-I652), "")</f>
         <v>4</v>
       </c>
       <c r="R652" s="10">
@@ -46063,14 +46063,14 @@
         <v>236</v>
       </c>
       <c r="N653" s="10">
-        <f t="shared" ref="N653:N868" si="36">(L653-K653)*-1</f>
+        <f t="shared" ref="N653:N877" si="36">(L653-K653)*-1</f>
         <v>6</v>
       </c>
       <c r="O653" s="10">
         <v>1</v>
       </c>
       <c r="P653" s="10">
-        <f t="shared" ref="P653:P868" si="37">IF(M653&gt;I653,1,0)</f>
+        <f t="shared" ref="P653:P877" si="37">IF(M653&gt;I653,1,0)</f>
         <v>1</v>
       </c>
       <c r="Q653" s="10">
@@ -46078,15 +46078,15 @@
         <v>17.5</v>
       </c>
       <c r="R653" s="10">
-        <f t="shared" ref="R653:R868" si="38">IF(M653&lt;I653, 1, 0)</f>
+        <f t="shared" ref="R653:R877" si="38">IF(M653&lt;I653, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="S653" s="10" t="str">
-        <f t="shared" ref="S653:S868" si="39">IF(R653=1,(I653-M653),"")</f>
+        <f t="shared" ref="S653:S877" si="39">IF(R653=1,(I653-M653),"")</f>
         <v/>
       </c>
       <c r="T653" s="10">
-        <f t="shared" ref="T653:T868" si="40">IF(M653=I653,1,0)</f>
+        <f t="shared" ref="T653:T877" si="40">IF(M653=I653,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -59092,7 +59092,7 @@
         <v>124</v>
       </c>
       <c r="M842" s="30">
-        <f t="shared" ref="M842:M868" si="41">K842+L842</f>
+        <f t="shared" ref="M842:M877" si="41">K842+L842</f>
         <v>239</v>
       </c>
       <c r="N842" s="30">
@@ -60913,6 +60913,627 @@
         <v>21</v>
       </c>
       <c r="T868" s="10">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="869" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A869" s="29">
+        <v>45714</v>
+      </c>
+      <c r="B869" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C869" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D869" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E869" s="30">
+        <v>0</v>
+      </c>
+      <c r="F869" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="G869" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H869" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="I869" s="30">
+        <v>239</v>
+      </c>
+      <c r="J869" s="31">
+        <v>-9.5</v>
+      </c>
+      <c r="K869" s="30">
+        <v>91</v>
+      </c>
+      <c r="L869" s="30">
+        <v>111</v>
+      </c>
+      <c r="M869" s="30">
+        <f t="shared" si="41"/>
+        <v>202</v>
+      </c>
+      <c r="N869" s="30">
+        <f t="shared" si="36"/>
+        <v>-20</v>
+      </c>
+      <c r="O869" s="30">
+        <v>1</v>
+      </c>
+      <c r="P869" s="30">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q869" s="30" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R869" s="30">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S869" s="30">
+        <f t="shared" si="39"/>
+        <v>37</v>
+      </c>
+      <c r="T869" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="870" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A870" s="29">
+        <v>45714</v>
+      </c>
+      <c r="B870" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C870" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D870" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E870" s="30">
+        <v>0</v>
+      </c>
+      <c r="F870" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="G870" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="H870" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="I870" s="30">
+        <v>228</v>
+      </c>
+      <c r="J870" s="31">
+        <v>5.5</v>
+      </c>
+      <c r="K870" s="30">
+        <v>129</v>
+      </c>
+      <c r="L870" s="30">
+        <v>121</v>
+      </c>
+      <c r="M870" s="30">
+        <f t="shared" si="41"/>
+        <v>250</v>
+      </c>
+      <c r="N870" s="30">
+        <f t="shared" si="36"/>
+        <v>8</v>
+      </c>
+      <c r="O870" s="30">
+        <v>1</v>
+      </c>
+      <c r="P870" s="30">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q870" s="30">
+        <f t="shared" si="35"/>
+        <v>22</v>
+      </c>
+      <c r="R870" s="30">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S870" s="30" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T870" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="871" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A871" s="29">
+        <v>45714</v>
+      </c>
+      <c r="B871" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C871" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D871" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E871" s="30">
+        <v>0</v>
+      </c>
+      <c r="F871" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="G871" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="H871" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="I871" s="30">
+        <v>232.5</v>
+      </c>
+      <c r="J871" s="31">
+        <v>-9.5</v>
+      </c>
+      <c r="K871" s="30">
+        <v>105</v>
+      </c>
+      <c r="L871" s="30">
+        <v>110</v>
+      </c>
+      <c r="M871" s="30">
+        <f t="shared" si="41"/>
+        <v>215</v>
+      </c>
+      <c r="N871" s="30">
+        <f t="shared" si="36"/>
+        <v>-5</v>
+      </c>
+      <c r="O871" s="30">
+        <v>1</v>
+      </c>
+      <c r="P871" s="30">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q871" s="30" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R871" s="30">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S871" s="30">
+        <f t="shared" si="39"/>
+        <v>17.5</v>
+      </c>
+      <c r="T871" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="872" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A872" s="29">
+        <v>45714</v>
+      </c>
+      <c r="B872" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C872" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D872" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E872" s="30">
+        <v>0</v>
+      </c>
+      <c r="F872" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="G872" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="H872" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="I872" s="30">
+        <v>225.5</v>
+      </c>
+      <c r="J872" s="31">
+        <v>4.5</v>
+      </c>
+      <c r="K872" s="30">
+        <v>97</v>
+      </c>
+      <c r="L872" s="30">
+        <v>117</v>
+      </c>
+      <c r="M872" s="30">
+        <f t="shared" si="41"/>
+        <v>214</v>
+      </c>
+      <c r="N872" s="30">
+        <f t="shared" si="36"/>
+        <v>-20</v>
+      </c>
+      <c r="O872" s="30">
+        <v>1</v>
+      </c>
+      <c r="P872" s="30">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q872" s="30" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R872" s="30">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S872" s="30">
+        <f t="shared" si="39"/>
+        <v>11.5</v>
+      </c>
+      <c r="T872" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="873" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A873" s="29">
+        <v>45714</v>
+      </c>
+      <c r="B873" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C873" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D873" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E873" s="30">
+        <v>0</v>
+      </c>
+      <c r="F873" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G873" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H873" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="I873" s="30">
+        <v>214.5</v>
+      </c>
+      <c r="J873" s="31">
+        <v>15.5</v>
+      </c>
+      <c r="K873" s="30">
+        <v>129</v>
+      </c>
+      <c r="L873" s="30">
+        <v>121</v>
+      </c>
+      <c r="M873" s="30">
+        <f t="shared" si="41"/>
+        <v>250</v>
+      </c>
+      <c r="N873" s="30">
+        <f t="shared" si="36"/>
+        <v>8</v>
+      </c>
+      <c r="O873" s="30">
+        <v>1</v>
+      </c>
+      <c r="P873" s="30">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q873" s="30">
+        <f t="shared" si="35"/>
+        <v>35.5</v>
+      </c>
+      <c r="R873" s="30">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S873" s="30" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T873" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="874" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A874" s="29">
+        <v>45714</v>
+      </c>
+      <c r="B874" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C874" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D874" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E874" s="30">
+        <v>0</v>
+      </c>
+      <c r="F874" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="G874" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="H874" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="I874" s="30">
+        <v>229.5</v>
+      </c>
+      <c r="J874" s="31">
+        <v>-1.5</v>
+      </c>
+      <c r="K874" s="30">
+        <v>109</v>
+      </c>
+      <c r="L874" s="30">
+        <v>131</v>
+      </c>
+      <c r="M874" s="30">
+        <f t="shared" si="41"/>
+        <v>240</v>
+      </c>
+      <c r="N874" s="30">
+        <f t="shared" si="36"/>
+        <v>-22</v>
+      </c>
+      <c r="O874" s="30">
+        <v>1</v>
+      </c>
+      <c r="P874" s="30">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q874" s="30">
+        <f t="shared" si="35"/>
+        <v>10.5</v>
+      </c>
+      <c r="R874" s="30">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S874" s="30" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T874" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="875" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A875" s="29">
+        <v>45714</v>
+      </c>
+      <c r="B875" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C875" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D875" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E875" s="30">
+        <v>0</v>
+      </c>
+      <c r="F875" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="G875" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="H875" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="I875" s="30">
+        <v>229</v>
+      </c>
+      <c r="J875" s="31">
+        <v>6.5</v>
+      </c>
+      <c r="K875" s="30">
+        <v>122</v>
+      </c>
+      <c r="L875" s="30">
+        <v>117</v>
+      </c>
+      <c r="M875" s="30">
+        <f t="shared" si="41"/>
+        <v>239</v>
+      </c>
+      <c r="N875" s="30">
+        <f t="shared" si="36"/>
+        <v>5</v>
+      </c>
+      <c r="O875" s="30">
+        <v>1</v>
+      </c>
+      <c r="P875" s="30">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="Q875" s="30">
+        <f t="shared" si="35"/>
+        <v>10</v>
+      </c>
+      <c r="R875" s="30">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="S875" s="30" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="T875" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="876" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A876" s="29">
+        <v>45714</v>
+      </c>
+      <c r="B876" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C876" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D876" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E876" s="30">
+        <v>0</v>
+      </c>
+      <c r="F876" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G876" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="H876" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="I876" s="30">
+        <v>236</v>
+      </c>
+      <c r="J876" s="31">
+        <v>8</v>
+      </c>
+      <c r="K876" s="30">
+        <v>118</v>
+      </c>
+      <c r="L876" s="30">
+        <v>101</v>
+      </c>
+      <c r="M876" s="30">
+        <f t="shared" si="41"/>
+        <v>219</v>
+      </c>
+      <c r="N876" s="30">
+        <f t="shared" si="36"/>
+        <v>17</v>
+      </c>
+      <c r="O876" s="30">
+        <v>1</v>
+      </c>
+      <c r="P876" s="30">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q876" s="30" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R876" s="30">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S876" s="30">
+        <f t="shared" si="39"/>
+        <v>17</v>
+      </c>
+      <c r="T876" s="30">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="877" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A877" s="29">
+        <v>45714</v>
+      </c>
+      <c r="B877" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C877" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D877" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E877" s="30">
+        <v>0</v>
+      </c>
+      <c r="F877" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="G877" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="H877" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="I877" s="30">
+        <v>224.5</v>
+      </c>
+      <c r="J877" s="31">
+        <v>-8.5</v>
+      </c>
+      <c r="K877" s="30">
+        <v>106</v>
+      </c>
+      <c r="L877" s="30">
+        <v>118</v>
+      </c>
+      <c r="M877" s="30">
+        <f t="shared" si="41"/>
+        <v>224</v>
+      </c>
+      <c r="N877" s="30">
+        <f t="shared" si="36"/>
+        <v>-12</v>
+      </c>
+      <c r="O877" s="30">
+        <v>1</v>
+      </c>
+      <c r="P877" s="30">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Q877" s="30" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R877" s="30">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="S877" s="30">
+        <f t="shared" si="39"/>
+        <v>0.5</v>
+      </c>
+      <c r="T877" s="30">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
updated eda notebook, added game data
</commit_message>
<xml_diff>
--- a/data/nba_points_2024_2025.xlsx
+++ b/data/nba_points_2024_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Documents/nba-points/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444702D7-AEB5-554F-B674-36F2700E4ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B585E9-6B17-214C-9FF5-A6B903F170CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22940" yWindow="500" windowWidth="45860" windowHeight="28300" xr2:uid="{4B944735-6DC1-314A-AF10-68EBB82A81F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5554" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5602" uniqueCount="148">
   <si>
     <t>Date</t>
   </si>
@@ -1028,11 +1028,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78582E2E-5746-944D-860C-ACA920BD70CB}">
-  <dimension ref="A1:Y923"/>
+  <dimension ref="A1:Y931"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A883" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A924" sqref="A924"/>
+      <pane ySplit="1" topLeftCell="A893" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A932" sqref="A932"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1207,15 +1207,15 @@
       </c>
       <c r="V2" s="7">
         <f>SUM(O:O)</f>
-        <v>915</v>
+        <v>923</v>
       </c>
       <c r="W2" s="12">
         <f>SUM(P:P)</f>
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="X2" s="15">
         <f>SUM(R:R)</f>
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="Y2" s="20">
         <f>SUM(T:T)</f>
@@ -1370,15 +1370,15 @@
       </c>
       <c r="W4" s="14">
         <f>W2/V2</f>
-        <v>0.52677595628415297</v>
+        <v>0.52762730227518961</v>
       </c>
       <c r="X4" s="16">
         <f>X2/V2</f>
-        <v>0.47322404371584698</v>
+        <v>0.47237269772481039</v>
       </c>
       <c r="Y4" s="21">
         <f>Y2/V2</f>
-        <v>3.2786885245901639E-3</v>
+        <v>3.2502708559046588E-3</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1526,11 +1526,11 @@
       </c>
       <c r="W6" s="22">
         <f>AVERAGE(Q:Q)</f>
-        <v>14.883817427385893</v>
+        <v>14.906570841889117</v>
       </c>
       <c r="X6" s="23">
         <f>AVERAGE(S:S)</f>
-        <v>14.935334872979215</v>
+        <v>14.927752293577981</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -62542,34 +62542,34 @@
         <v>106</v>
       </c>
       <c r="M892" s="30">
-        <f t="shared" ref="M892:M923" si="42">K892+L892</f>
+        <f t="shared" ref="M892:M931" si="42">K892+L892</f>
         <v>208</v>
       </c>
       <c r="N892" s="30">
-        <f t="shared" ref="N892:N923" si="43">(L892-K892)*-1</f>
+        <f t="shared" ref="N892:N931" si="43">(L892-K892)*-1</f>
         <v>-4</v>
       </c>
       <c r="O892" s="30">
         <v>1</v>
       </c>
       <c r="P892" s="30">
-        <f t="shared" ref="P892:P923" si="44">IF(M892&gt;I892,1,0)</f>
+        <f t="shared" ref="P892:P931" si="44">IF(M892&gt;I892,1,0)</f>
         <v>0</v>
       </c>
       <c r="Q892" s="30" t="str">
-        <f t="shared" ref="Q892:Q923" si="45">IF(P892=1,(M892-I892), "")</f>
+        <f t="shared" ref="Q892:Q931" si="45">IF(P892=1,(M892-I892), "")</f>
         <v/>
       </c>
       <c r="R892" s="30">
-        <f t="shared" ref="R892:R923" si="46">IF(M892&lt;I892, 1, 0)</f>
+        <f t="shared" ref="R892:R931" si="46">IF(M892&lt;I892, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="S892" s="30">
-        <f t="shared" ref="S892:S923" si="47">IF(R892=1,(I892-M892),"")</f>
+        <f t="shared" ref="S892:S931" si="47">IF(R892=1,(I892-M892),"")</f>
         <v>13.5</v>
       </c>
       <c r="T892" s="30">
-        <f t="shared" ref="T892:T923" si="48">IF(M892=I892,1,0)</f>
+        <f t="shared" ref="T892:T931" si="48">IF(M892=I892,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -64708,6 +64708,558 @@
         <v/>
       </c>
       <c r="T923" s="30">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="924" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A924" s="9">
+        <v>45721</v>
+      </c>
+      <c r="B924" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C924" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D924" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E924" s="10">
+        <v>0</v>
+      </c>
+      <c r="F924" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G924" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H924" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I924" s="10">
+        <v>233.5</v>
+      </c>
+      <c r="J924" s="11">
+        <v>-4.5</v>
+      </c>
+      <c r="K924" s="10">
+        <v>122</v>
+      </c>
+      <c r="L924" s="10">
+        <v>125</v>
+      </c>
+      <c r="M924" s="10">
+        <f t="shared" si="42"/>
+        <v>247</v>
+      </c>
+      <c r="N924" s="10">
+        <f t="shared" si="43"/>
+        <v>-3</v>
+      </c>
+      <c r="O924" s="10">
+        <v>1</v>
+      </c>
+      <c r="P924" s="10">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="Q924" s="10">
+        <f t="shared" si="45"/>
+        <v>13.5</v>
+      </c>
+      <c r="R924" s="10">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="S924" s="10" t="str">
+        <f t="shared" si="47"/>
+        <v/>
+      </c>
+      <c r="T924" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="925" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A925" s="9">
+        <v>45721</v>
+      </c>
+      <c r="B925" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C925" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D925" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E925" s="10">
+        <v>0</v>
+      </c>
+      <c r="F925" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G925" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H925" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I925" s="10">
+        <v>221.5</v>
+      </c>
+      <c r="J925" s="11">
+        <v>8.5</v>
+      </c>
+      <c r="K925" s="10">
+        <v>125</v>
+      </c>
+      <c r="L925" s="10">
+        <v>110</v>
+      </c>
+      <c r="M925" s="10">
+        <f t="shared" si="42"/>
+        <v>235</v>
+      </c>
+      <c r="N925" s="10">
+        <f t="shared" si="43"/>
+        <v>15</v>
+      </c>
+      <c r="O925" s="10">
+        <v>1</v>
+      </c>
+      <c r="P925" s="10">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="Q925" s="10">
+        <f t="shared" si="45"/>
+        <v>13.5</v>
+      </c>
+      <c r="R925" s="10">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="S925" s="10" t="str">
+        <f t="shared" si="47"/>
+        <v/>
+      </c>
+      <c r="T925" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="926" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A926" s="9">
+        <v>45721</v>
+      </c>
+      <c r="B926" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C926" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D926" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E926" s="10">
+        <v>0</v>
+      </c>
+      <c r="F926" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G926" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H926" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I926" s="10">
+        <v>225</v>
+      </c>
+      <c r="J926" s="11">
+        <v>-10.5</v>
+      </c>
+      <c r="K926" s="10">
+        <v>118</v>
+      </c>
+      <c r="L926" s="10">
+        <v>128</v>
+      </c>
+      <c r="M926" s="10">
+        <f t="shared" si="42"/>
+        <v>246</v>
+      </c>
+      <c r="N926" s="10">
+        <f t="shared" si="43"/>
+        <v>-10</v>
+      </c>
+      <c r="O926" s="10">
+        <v>1</v>
+      </c>
+      <c r="P926" s="10">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="Q926" s="10">
+        <f t="shared" si="45"/>
+        <v>21</v>
+      </c>
+      <c r="R926" s="10">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="S926" s="10" t="str">
+        <f t="shared" si="47"/>
+        <v/>
+      </c>
+      <c r="T926" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="927" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A927" s="9">
+        <v>45721</v>
+      </c>
+      <c r="B927" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C927" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D927" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E927" s="10">
+        <v>0</v>
+      </c>
+      <c r="F927" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G927" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H927" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I927" s="10">
+        <v>226.5</v>
+      </c>
+      <c r="J927" s="11">
+        <v>-11.5</v>
+      </c>
+      <c r="K927" s="10">
+        <v>107</v>
+      </c>
+      <c r="L927" s="10">
+        <v>112</v>
+      </c>
+      <c r="M927" s="10">
+        <f t="shared" si="42"/>
+        <v>219</v>
+      </c>
+      <c r="N927" s="10">
+        <f t="shared" si="43"/>
+        <v>-5</v>
+      </c>
+      <c r="O927" s="10">
+        <v>1</v>
+      </c>
+      <c r="P927" s="10">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="Q927" s="10" t="str">
+        <f t="shared" si="45"/>
+        <v/>
+      </c>
+      <c r="R927" s="10">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="S927" s="10">
+        <f t="shared" si="47"/>
+        <v>7.5</v>
+      </c>
+      <c r="T927" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="928" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A928" s="9">
+        <v>45721</v>
+      </c>
+      <c r="B928" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C928" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D928" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E928" s="10">
+        <v>0</v>
+      </c>
+      <c r="F928" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G928" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H928" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I928" s="10">
+        <v>225.5</v>
+      </c>
+      <c r="J928" s="11">
+        <v>-9.5</v>
+      </c>
+      <c r="K928" s="10">
+        <v>107</v>
+      </c>
+      <c r="L928" s="10">
+        <v>137</v>
+      </c>
+      <c r="M928" s="10">
+        <f t="shared" si="42"/>
+        <v>244</v>
+      </c>
+      <c r="N928" s="10">
+        <f t="shared" si="43"/>
+        <v>-30</v>
+      </c>
+      <c r="O928" s="10">
+        <v>1</v>
+      </c>
+      <c r="P928" s="10">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="Q928" s="10">
+        <f t="shared" si="45"/>
+        <v>18.5</v>
+      </c>
+      <c r="R928" s="10">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="S928" s="10" t="str">
+        <f t="shared" si="47"/>
+        <v/>
+      </c>
+      <c r="T928" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="929" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A929" s="9">
+        <v>45721</v>
+      </c>
+      <c r="B929" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C929" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D929" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E929" s="10">
+        <v>0</v>
+      </c>
+      <c r="F929" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G929" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H929" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="I929" s="10">
+        <v>236.5</v>
+      </c>
+      <c r="J929" s="11">
+        <v>-6.5</v>
+      </c>
+      <c r="K929" s="10">
+        <v>110</v>
+      </c>
+      <c r="L929" s="10">
+        <v>116</v>
+      </c>
+      <c r="M929" s="10">
+        <f t="shared" si="42"/>
+        <v>226</v>
+      </c>
+      <c r="N929" s="10">
+        <f t="shared" si="43"/>
+        <v>-6</v>
+      </c>
+      <c r="O929" s="10">
+        <v>1</v>
+      </c>
+      <c r="P929" s="10">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="Q929" s="10" t="str">
+        <f t="shared" si="45"/>
+        <v/>
+      </c>
+      <c r="R929" s="10">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="S929" s="10">
+        <f t="shared" si="47"/>
+        <v>10.5</v>
+      </c>
+      <c r="T929" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="930" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A930" s="9">
+        <v>45721</v>
+      </c>
+      <c r="B930" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C930" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D930" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E930" s="10">
+        <v>0</v>
+      </c>
+      <c r="F930" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G930" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H930" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I930" s="10">
+        <v>246.5</v>
+      </c>
+      <c r="J930" s="11">
+        <v>7.5</v>
+      </c>
+      <c r="K930" s="10">
+        <v>120</v>
+      </c>
+      <c r="L930" s="10">
+        <v>103</v>
+      </c>
+      <c r="M930" s="10">
+        <f t="shared" si="42"/>
+        <v>223</v>
+      </c>
+      <c r="N930" s="10">
+        <f t="shared" si="43"/>
+        <v>17</v>
+      </c>
+      <c r="O930" s="10">
+        <v>1</v>
+      </c>
+      <c r="P930" s="10">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="Q930" s="10" t="str">
+        <f t="shared" si="45"/>
+        <v/>
+      </c>
+      <c r="R930" s="10">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="S930" s="10">
+        <f t="shared" si="47"/>
+        <v>23.5</v>
+      </c>
+      <c r="T930" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="931" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A931" s="9">
+        <v>45721</v>
+      </c>
+      <c r="B931" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C931" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D931" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E931" s="10">
+        <v>0</v>
+      </c>
+      <c r="F931" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G931" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H931" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="I931" s="10">
+        <v>219</v>
+      </c>
+      <c r="J931" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="K931" s="10">
+        <v>115</v>
+      </c>
+      <c r="L931" s="10">
+        <v>123</v>
+      </c>
+      <c r="M931" s="10">
+        <f t="shared" si="42"/>
+        <v>238</v>
+      </c>
+      <c r="N931" s="10">
+        <f t="shared" si="43"/>
+        <v>-8</v>
+      </c>
+      <c r="O931" s="10">
+        <v>1</v>
+      </c>
+      <c r="P931" s="10">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="Q931" s="10">
+        <f t="shared" si="45"/>
+        <v>19</v>
+      </c>
+      <c r="R931" s="10">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="S931" s="10" t="str">
+        <f t="shared" si="47"/>
+        <v/>
+      </c>
+      <c r="T931" s="10">
         <f t="shared" si="48"/>
         <v>0</v>
       </c>

</xml_diff>